<commit_message>
Updating projet_list_all with project test set (3 projects per instrument)
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="65">
   <si>
     <t>Project_ID</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>object_area</t>
+  </si>
+  <si>
+    <t>object_annotation_category</t>
   </si>
   <si>
     <t>Variables</t>
@@ -678,6 +681,9 @@
       <c r="U2" t="s">
         <v>33</v>
       </c>
+      <c r="Y2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3">
@@ -710,6 +716,9 @@
       <c r="U3" t="s">
         <v>33</v>
       </c>
+      <c r="Y3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4">
@@ -742,6 +751,9 @@
       <c r="U4" t="s">
         <v>33</v>
       </c>
+      <c r="Y4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5">
@@ -774,6 +786,9 @@
       <c r="U5" t="s">
         <v>33</v>
       </c>
+      <c r="Y5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6">
@@ -806,6 +821,9 @@
       <c r="U6" t="s">
         <v>33</v>
       </c>
+      <c r="Y6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7">
@@ -838,6 +856,9 @@
       <c r="U7" t="s">
         <v>33</v>
       </c>
+      <c r="Y7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8">
@@ -870,6 +891,9 @@
       <c r="U8" t="s">
         <v>33</v>
       </c>
+      <c r="Y8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9">
@@ -902,6 +926,9 @@
       <c r="U9" t="s">
         <v>33</v>
       </c>
+      <c r="Y9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10">
@@ -934,6 +961,9 @@
       <c r="U10" t="s">
         <v>33</v>
       </c>
+      <c r="Y10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11">
@@ -966,6 +996,9 @@
       <c r="U11" t="s">
         <v>33</v>
       </c>
+      <c r="Y11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12">
@@ -998,6 +1031,9 @@
       <c r="U12" t="s">
         <v>33</v>
       </c>
+      <c r="Y12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13">
@@ -1030,6 +1066,9 @@
       <c r="U13" t="s">
         <v>33</v>
       </c>
+      <c r="Y13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14">
@@ -1062,6 +1101,9 @@
       <c r="U14" t="s">
         <v>33</v>
       </c>
+      <c r="Y14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15">
@@ -1094,6 +1136,9 @@
       <c r="U15" t="s">
         <v>33</v>
       </c>
+      <c r="Y15" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16">
@@ -1126,8 +1171,11 @@
       <c r="U16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="Y16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -1158,8 +1206,11 @@
       <c r="U17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="Y17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -1190,8 +1241,11 @@
       <c r="U18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="Y18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -1222,8 +1276,11 @@
       <c r="U19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="Y19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -1254,8 +1311,11 @@
       <c r="U20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="Y20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -1286,8 +1346,11 @@
       <c r="U21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="Y21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -1318,8 +1381,11 @@
       <c r="U22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="Y22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -1350,8 +1416,11 @@
       <c r="U23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="Y23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -1382,8 +1451,11 @@
       <c r="U24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="Y24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -1414,8 +1486,11 @@
       <c r="U25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="Y25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -1446,8 +1521,11 @@
       <c r="U26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="Y26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -1478,8 +1556,11 @@
       <c r="U27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="Y27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -1510,8 +1591,11 @@
       <c r="U28" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="Y28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -1542,8 +1626,11 @@
       <c r="U29" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="Y29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -1574,8 +1661,11 @@
       <c r="U30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:21">
+      <c r="Y30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -1606,8 +1696,11 @@
       <c r="U31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="Y31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -1638,8 +1731,11 @@
       <c r="U32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="Y32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -1670,8 +1766,11 @@
       <c r="U33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="Y33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -1702,8 +1801,11 @@
       <c r="U34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="Y34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -1734,8 +1836,11 @@
       <c r="U35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="Y35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -1766,8 +1871,11 @@
       <c r="U36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="Y36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -1798,8 +1906,11 @@
       <c r="U37" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:21">
+      <c r="Y37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -1830,8 +1941,11 @@
       <c r="U38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:21">
+      <c r="Y38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -1862,8 +1976,11 @@
       <c r="U39" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="Y39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -1894,8 +2011,11 @@
       <c r="U40" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="Y40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -1926,8 +2046,11 @@
       <c r="U41" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="1:21">
+      <c r="Y41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -1958,8 +2081,11 @@
       <c r="U42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="Y42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -1990,8 +2116,11 @@
       <c r="U43" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:21">
+      <c r="Y43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -2022,8 +2151,11 @@
       <c r="U44" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:21">
+      <c r="Y44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -2054,8 +2186,11 @@
       <c r="U45" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="46" spans="1:21">
+      <c r="Y45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -2086,8 +2221,11 @@
       <c r="U46" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="1:21">
+      <c r="Y46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -2117,6 +2255,9 @@
       </c>
       <c r="U47" t="s">
         <v>33</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2134,13 +2275,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2148,10 +2289,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2159,10 +2300,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2170,10 +2311,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2181,10 +2322,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2192,10 +2333,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2203,10 +2344,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2214,10 +2355,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2225,10 +2366,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2236,10 +2377,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2247,10 +2388,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2258,10 +2399,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2269,10 +2410,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2280,10 +2421,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2291,10 +2432,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2302,10 +2443,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2313,10 +2454,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2324,10 +2465,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2335,10 +2476,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2346,10 +2487,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2357,10 +2498,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2368,10 +2509,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2379,10 +2520,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2390,10 +2531,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2401,10 +2542,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2412,10 +2553,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some column names, but others are unclear
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D947903F-B784-BE43-A5F8-A10BFC2897C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="68">
   <si>
     <t>Project_ID</t>
   </si>
@@ -210,13 +216,22 @@
   </si>
   <si>
     <t>Name of the category ID column in project export file</t>
+  </si>
+  <si>
+    <t>object_equivdiameter</t>
+  </si>
+  <si>
+    <t>meters</t>
+  </si>
+  <si>
+    <t>process_pixel_to_micron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +294,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -325,7 +348,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,9 +380,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,6 +432,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -566,14 +625,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -672,20 +748,29 @@
       <c r="J2" t="s">
         <v>30</v>
       </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
       <c r="L2" t="s">
         <v>31</v>
       </c>
+      <c r="M2" t="s">
+        <v>66</v>
+      </c>
       <c r="S2" t="s">
         <v>32</v>
       </c>
       <c r="U2" t="s">
         <v>33</v>
       </c>
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
       <c r="Y2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -720,7 +805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -755,7 +840,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -790,7 +875,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -825,7 +910,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -860,7 +945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -895,7 +980,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -930,7 +1015,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -965,7 +1050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -1000,7 +1085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -1035,7 +1120,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -1070,7 +1155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -1105,7 +1190,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -1140,7 +1225,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -1175,7 +1260,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -1210,7 +1295,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -1245,7 +1330,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -1280,7 +1365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -1305,6 +1390,9 @@
       <c r="L20" t="s">
         <v>31</v>
       </c>
+      <c r="Q20" t="s">
+        <v>65</v>
+      </c>
       <c r="S20" t="s">
         <v>32</v>
       </c>
@@ -1315,7 +1403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -1350,7 +1438,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -1385,7 +1473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -1420,7 +1508,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -1455,7 +1543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -1490,7 +1578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -1525,7 +1613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -1560,7 +1648,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -1595,7 +1683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -1630,7 +1718,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -1665,7 +1753,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -1700,7 +1788,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -1735,7 +1823,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -1770,7 +1858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -1805,7 +1893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -1840,7 +1928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -1875,7 +1963,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -1910,7 +1998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -1945,7 +2033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -1980,7 +2068,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -2015,7 +2103,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -2050,7 +2138,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -2085,7 +2173,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -2120,7 +2208,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -2155,7 +2243,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -2190,7 +2278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -2225,7 +2313,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -2266,14 +2354,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2284,7 +2372,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2383,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2306,7 +2394,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2317,7 +2405,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2328,7 +2416,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2339,7 +2427,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2350,7 +2438,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2361,7 +2449,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2372,7 +2460,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2471,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2394,7 +2482,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2405,7 +2493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2416,7 +2504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2427,7 +2515,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2438,7 +2526,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2449,7 +2537,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2460,7 +2548,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2471,7 +2559,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2482,7 +2570,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2493,7 +2581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2504,7 +2592,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2515,7 +2603,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2526,7 +2614,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2537,7 +2625,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2548,7 +2636,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
completed and added info on station number, leg number and empty coordinate fields
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93730C3B-1EFE-6540-9013-58C108CA9F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDEC98C-ABBF-FF4C-99D9-4A658835212D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39260" yWindow="1960" windowWidth="30240" windowHeight="17320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="86">
   <si>
     <t>Project_ID</t>
   </si>
@@ -254,7 +254,31 @@
     <t>station.ID.fromName</t>
   </si>
   <si>
-    <t>number of the station ID inferred from the project export file</t>
+    <t>empty.coord</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>projects with empty fields in lat &amp; lon</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>leg.from.name</t>
+  </si>
+  <si>
+    <t>leg_from_name</t>
+  </si>
+  <si>
+    <t>leg number of the expedition</t>
+  </si>
+  <si>
+    <t>number of the station ID inferred from the project export file. If NaN, mutiple stations in a project</t>
   </si>
 </sst>
 </file>
@@ -343,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -353,6 +377,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,31 +722,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="X26" sqref="I16:X26"/>
+    <sheetView topLeftCell="B1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,74 +760,80 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -809,73 +847,79 @@
         <v>27</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>159</v>
       </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
       <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
         <v>31</v>
       </c>
-      <c r="N2" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" t="s">
-        <v>68</v>
-      </c>
       <c r="P2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
         <v>68</v>
       </c>
       <c r="R2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2" t="s">
         <v>65</v>
       </c>
-      <c r="S2" t="s">
-        <v>70</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" t="s">
         <v>32</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>71</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>33</v>
       </c>
-      <c r="W2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z2" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -889,73 +933,79 @@
         <v>27</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>160</v>
       </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
       <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" t="s">
-        <v>68</v>
-      </c>
       <c r="P3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
         <v>68</v>
       </c>
       <c r="R3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" t="s">
         <v>65</v>
       </c>
-      <c r="S3" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>71</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>33</v>
       </c>
-      <c r="W3" t="s">
-        <v>70</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z3" t="s">
         <v>67</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -968,32 +1018,80 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>167</v>
+      </c>
       <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" t="s">
         <v>30</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" t="s">
         <v>31</v>
       </c>
+      <c r="P4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>68</v>
+      </c>
       <c r="R4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" t="s">
         <v>65</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" t="s">
         <v>32</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
+        <v>71</v>
+      </c>
+      <c r="X4" t="s">
         <v>33</v>
       </c>
+      <c r="Y4" t="s">
+        <v>70</v>
+      </c>
       <c r="Z4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1006,34 +1104,79 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>155</v>
+      </c>
       <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
         <v>30</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" t="s">
         <v>31</v>
       </c>
+      <c r="P5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>68</v>
+      </c>
       <c r="R5" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" t="s">
         <v>65</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" t="s">
         <v>32</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>33</v>
       </c>
+      <c r="Y5" t="s">
+        <v>70</v>
+      </c>
       <c r="Z5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3294</v>
+        <v>3292</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -1044,34 +1187,79 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>156</v>
+      </c>
       <c r="G6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" t="s">
         <v>29</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" t="s">
         <v>30</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" t="s">
         <v>31</v>
       </c>
+      <c r="P6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>68</v>
+      </c>
       <c r="R6" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" t="s">
+        <v>68</v>
+      </c>
+      <c r="T6" t="s">
         <v>65</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
+        <v>70</v>
+      </c>
+      <c r="V6" t="s">
         <v>32</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>33</v>
       </c>
+      <c r="Y6" t="s">
+        <v>70</v>
+      </c>
       <c r="Z6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3295</v>
+        <v>3293</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -1082,34 +1270,79 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>157</v>
+      </c>
       <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="s">
         <v>29</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" t="s">
         <v>30</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" t="s">
         <v>31</v>
       </c>
+      <c r="P7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>68</v>
+      </c>
       <c r="R7" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T7" t="s">
         <v>65</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7" t="s">
         <v>32</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>33</v>
       </c>
+      <c r="Y7" t="s">
+        <v>70</v>
+      </c>
       <c r="Z7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3296</v>
+        <v>3294</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1120,34 +1353,79 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>158</v>
+      </c>
       <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
         <v>29</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" t="s">
         <v>30</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O8" t="s">
         <v>31</v>
       </c>
+      <c r="P8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>68</v>
+      </c>
       <c r="R8" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" t="s">
+        <v>68</v>
+      </c>
+      <c r="T8" t="s">
         <v>65</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
+        <v>70</v>
+      </c>
+      <c r="V8" t="s">
         <v>32</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>33</v>
       </c>
+      <c r="Y8" t="s">
+        <v>70</v>
+      </c>
       <c r="Z8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3297</v>
+        <v>3295</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1158,34 +1436,79 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>161</v>
+      </c>
       <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
         <v>29</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" t="s">
         <v>30</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" t="s">
         <v>31</v>
       </c>
+      <c r="P9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>68</v>
+      </c>
       <c r="R9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" t="s">
+        <v>68</v>
+      </c>
+      <c r="T9" t="s">
         <v>65</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
+        <v>70</v>
+      </c>
+      <c r="V9" t="s">
         <v>32</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>33</v>
       </c>
+      <c r="Y9" t="s">
+        <v>70</v>
+      </c>
       <c r="Z9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3298</v>
+        <v>3296</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -1196,34 +1519,79 @@
       <c r="D10" t="s">
         <v>27</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>162</v>
+      </c>
       <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" t="s">
         <v>28</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
         <v>29</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
         <v>30</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" t="s">
         <v>31</v>
       </c>
+      <c r="P10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>68</v>
+      </c>
       <c r="R10" t="s">
+        <v>68</v>
+      </c>
+      <c r="S10" t="s">
+        <v>68</v>
+      </c>
+      <c r="T10" t="s">
         <v>65</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
+        <v>70</v>
+      </c>
+      <c r="V10" t="s">
         <v>32</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>33</v>
       </c>
+      <c r="Y10" t="s">
+        <v>70</v>
+      </c>
       <c r="Z10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3299</v>
+        <v>3297</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -1234,34 +1602,79 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>163</v>
+      </c>
       <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" t="s">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
         <v>29</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
         <v>30</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" t="s">
         <v>31</v>
       </c>
+      <c r="P11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>68</v>
+      </c>
       <c r="R11" t="s">
+        <v>68</v>
+      </c>
+      <c r="S11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T11" t="s">
         <v>65</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
+        <v>70</v>
+      </c>
+      <c r="V11" t="s">
         <v>32</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>33</v>
       </c>
+      <c r="Y11" t="s">
+        <v>70</v>
+      </c>
       <c r="Z11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3300</v>
+        <v>3298</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1272,34 +1685,79 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
       <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" t="s">
         <v>28</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
         <v>29</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
+        <v>69</v>
+      </c>
+      <c r="M12" t="s">
         <v>30</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12" t="s">
         <v>31</v>
       </c>
+      <c r="P12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>68</v>
+      </c>
       <c r="R12" t="s">
+        <v>68</v>
+      </c>
+      <c r="S12" t="s">
+        <v>68</v>
+      </c>
+      <c r="T12" t="s">
         <v>65</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
+        <v>70</v>
+      </c>
+      <c r="V12" t="s">
         <v>32</v>
       </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
         <v>33</v>
       </c>
+      <c r="Y12" t="s">
+        <v>70</v>
+      </c>
       <c r="Z12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>3301</v>
+        <v>3299</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1310,34 +1768,79 @@
       <c r="D13" t="s">
         <v>27</v>
       </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
       <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" t="s">
         <v>28</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" t="s">
         <v>29</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" t="s">
         <v>30</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" t="s">
         <v>31</v>
       </c>
+      <c r="P13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>68</v>
+      </c>
       <c r="R13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S13" t="s">
+        <v>68</v>
+      </c>
+      <c r="T13" t="s">
         <v>65</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
+        <v>70</v>
+      </c>
+      <c r="V13" t="s">
         <v>32</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
         <v>33</v>
       </c>
+      <c r="Y13" t="s">
+        <v>70</v>
+      </c>
       <c r="Z13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>3302</v>
+        <v>3300</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -1348,34 +1851,79 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>165</v>
+      </c>
       <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" t="s">
         <v>28</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" t="s">
         <v>29</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" t="s">
         <v>30</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
+        <v>66</v>
+      </c>
+      <c r="O14" t="s">
         <v>31</v>
       </c>
+      <c r="P14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>68</v>
+      </c>
       <c r="R14" t="s">
+        <v>68</v>
+      </c>
+      <c r="S14" t="s">
+        <v>68</v>
+      </c>
+      <c r="T14" t="s">
         <v>65</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
+        <v>70</v>
+      </c>
+      <c r="V14" t="s">
         <v>32</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>33</v>
       </c>
+      <c r="Y14" t="s">
+        <v>70</v>
+      </c>
       <c r="Z14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3303</v>
+        <v>3301</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -1386,34 +1934,79 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>166</v>
+      </c>
       <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" t="s">
         <v>28</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
         <v>29</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" t="s">
         <v>30</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
+        <v>66</v>
+      </c>
+      <c r="O15" t="s">
         <v>31</v>
       </c>
+      <c r="P15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>68</v>
+      </c>
       <c r="R15" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" t="s">
+        <v>68</v>
+      </c>
+      <c r="T15" t="s">
         <v>65</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
+        <v>70</v>
+      </c>
+      <c r="V15" t="s">
         <v>32</v>
       </c>
-      <c r="V15" t="s">
+      <c r="X15" t="s">
         <v>33</v>
       </c>
+      <c r="Y15" t="s">
+        <v>70</v>
+      </c>
       <c r="Z15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>3304</v>
+        <v>3302</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1424,34 +2017,79 @@
       <c r="D16" t="s">
         <v>27</v>
       </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>168</v>
+      </c>
       <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" t="s">
         <v>28</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" t="s">
         <v>29</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
+        <v>69</v>
+      </c>
+      <c r="M16" t="s">
         <v>30</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" t="s">
         <v>31</v>
       </c>
+      <c r="P16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>68</v>
+      </c>
       <c r="R16" t="s">
+        <v>68</v>
+      </c>
+      <c r="S16" t="s">
+        <v>68</v>
+      </c>
+      <c r="T16" t="s">
         <v>65</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
+        <v>70</v>
+      </c>
+      <c r="V16" t="s">
         <v>32</v>
       </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
         <v>33</v>
       </c>
+      <c r="Y16" t="s">
+        <v>70</v>
+      </c>
       <c r="Z16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>3305</v>
+        <v>3303</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -1462,34 +2100,79 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>169</v>
+      </c>
       <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" t="s">
         <v>28</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" t="s">
         <v>29</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" t="s">
         <v>30</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17" t="s">
         <v>31</v>
       </c>
+      <c r="P17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>68</v>
+      </c>
       <c r="R17" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" t="s">
+        <v>68</v>
+      </c>
+      <c r="T17" t="s">
         <v>65</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
+        <v>70</v>
+      </c>
+      <c r="V17" t="s">
         <v>32</v>
       </c>
-      <c r="V17" t="s">
+      <c r="X17" t="s">
         <v>33</v>
       </c>
+      <c r="Y17" t="s">
+        <v>70</v>
+      </c>
       <c r="Z17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>3306</v>
+        <v>3304</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -1500,34 +2183,79 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>170</v>
+      </c>
       <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" t="s">
         <v>28</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" t="s">
         <v>29</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" t="s">
         <v>30</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
+        <v>66</v>
+      </c>
+      <c r="O18" t="s">
         <v>31</v>
       </c>
+      <c r="P18" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>68</v>
+      </c>
       <c r="R18" t="s">
+        <v>68</v>
+      </c>
+      <c r="S18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T18" t="s">
         <v>65</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
+        <v>70</v>
+      </c>
+      <c r="V18" t="s">
         <v>32</v>
       </c>
-      <c r="V18" t="s">
+      <c r="X18" t="s">
         <v>33</v>
       </c>
+      <c r="Y18" t="s">
+        <v>70</v>
+      </c>
       <c r="Z18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>3307</v>
+        <v>3305</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -1538,34 +2266,79 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>171</v>
+      </c>
       <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" t="s">
         <v>28</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" t="s">
         <v>29</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
+        <v>69</v>
+      </c>
+      <c r="M19" t="s">
         <v>30</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
+        <v>66</v>
+      </c>
+      <c r="O19" t="s">
         <v>31</v>
       </c>
+      <c r="P19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>68</v>
+      </c>
       <c r="R19" t="s">
+        <v>68</v>
+      </c>
+      <c r="S19" t="s">
+        <v>68</v>
+      </c>
+      <c r="T19" t="s">
         <v>65</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
+        <v>70</v>
+      </c>
+      <c r="V19" t="s">
         <v>32</v>
       </c>
-      <c r="V19" t="s">
+      <c r="X19" t="s">
         <v>33</v>
       </c>
+      <c r="Y19" t="s">
+        <v>70</v>
+      </c>
       <c r="Z19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>3308</v>
+        <v>3306</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -1576,34 +2349,79 @@
       <c r="D20" t="s">
         <v>27</v>
       </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>172</v>
+      </c>
       <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" t="s">
         <v>28</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" t="s">
         <v>29</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
+        <v>69</v>
+      </c>
+      <c r="M20" t="s">
         <v>30</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
+        <v>66</v>
+      </c>
+      <c r="O20" t="s">
         <v>31</v>
       </c>
+      <c r="P20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>68</v>
+      </c>
       <c r="R20" t="s">
+        <v>68</v>
+      </c>
+      <c r="S20" t="s">
+        <v>68</v>
+      </c>
+      <c r="T20" t="s">
         <v>65</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
+        <v>70</v>
+      </c>
+      <c r="V20" t="s">
         <v>32</v>
       </c>
-      <c r="V20" t="s">
+      <c r="X20" t="s">
         <v>33</v>
       </c>
+      <c r="Y20" t="s">
+        <v>70</v>
+      </c>
       <c r="Z20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>3309</v>
+        <v>3307</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -1614,34 +2432,79 @@
       <c r="D21" t="s">
         <v>27</v>
       </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>173</v>
+      </c>
       <c r="G21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" t="s">
         <v>28</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" t="s">
         <v>29</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M21" t="s">
         <v>30</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
+        <v>66</v>
+      </c>
+      <c r="O21" t="s">
         <v>31</v>
       </c>
+      <c r="P21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>68</v>
+      </c>
       <c r="R21" t="s">
+        <v>68</v>
+      </c>
+      <c r="S21" t="s">
+        <v>68</v>
+      </c>
+      <c r="T21" t="s">
         <v>65</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
+        <v>70</v>
+      </c>
+      <c r="V21" t="s">
         <v>32</v>
       </c>
-      <c r="V21" t="s">
+      <c r="X21" t="s">
         <v>33</v>
       </c>
+      <c r="Y21" t="s">
+        <v>70</v>
+      </c>
       <c r="Z21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>3310</v>
+        <v>3308</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -1652,34 +2515,79 @@
       <c r="D22" t="s">
         <v>27</v>
       </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>174</v>
+      </c>
       <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" t="s">
         <v>28</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" t="s">
         <v>29</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
+        <v>69</v>
+      </c>
+      <c r="M22" t="s">
         <v>30</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O22" t="s">
         <v>31</v>
       </c>
+      <c r="P22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>68</v>
+      </c>
       <c r="R22" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" t="s">
+        <v>68</v>
+      </c>
+      <c r="T22" t="s">
         <v>65</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
+        <v>70</v>
+      </c>
+      <c r="V22" t="s">
         <v>32</v>
       </c>
-      <c r="V22" t="s">
+      <c r="X22" t="s">
         <v>33</v>
       </c>
+      <c r="Y22" t="s">
+        <v>70</v>
+      </c>
       <c r="Z22" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>3311</v>
+        <v>3309</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -1690,34 +2598,79 @@
       <c r="D23" t="s">
         <v>27</v>
       </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>175</v>
+      </c>
       <c r="G23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" t="s">
         <v>28</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" t="s">
         <v>29</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M23" t="s">
         <v>30</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
+        <v>66</v>
+      </c>
+      <c r="O23" t="s">
         <v>31</v>
       </c>
+      <c r="P23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>68</v>
+      </c>
       <c r="R23" t="s">
+        <v>68</v>
+      </c>
+      <c r="S23" t="s">
+        <v>68</v>
+      </c>
+      <c r="T23" t="s">
         <v>65</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
+        <v>70</v>
+      </c>
+      <c r="V23" t="s">
         <v>32</v>
       </c>
-      <c r="V23" t="s">
+      <c r="X23" t="s">
         <v>33</v>
       </c>
+      <c r="Y23" t="s">
+        <v>70</v>
+      </c>
       <c r="Z23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>3312</v>
+        <v>3310</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1728,34 +2681,79 @@
       <c r="D24" t="s">
         <v>27</v>
       </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>176</v>
+      </c>
       <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" t="s">
         <v>28</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" t="s">
         <v>29</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
+        <v>69</v>
+      </c>
+      <c r="M24" t="s">
         <v>30</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
+        <v>66</v>
+      </c>
+      <c r="O24" t="s">
         <v>31</v>
       </c>
+      <c r="P24" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>68</v>
+      </c>
       <c r="R24" t="s">
+        <v>68</v>
+      </c>
+      <c r="S24" t="s">
+        <v>68</v>
+      </c>
+      <c r="T24" t="s">
         <v>65</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
+        <v>70</v>
+      </c>
+      <c r="V24" t="s">
         <v>32</v>
       </c>
-      <c r="V24" t="s">
+      <c r="X24" t="s">
         <v>33</v>
       </c>
+      <c r="Y24" t="s">
+        <v>70</v>
+      </c>
       <c r="Z24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>3313</v>
+        <v>3311</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -1766,34 +2764,79 @@
       <c r="D25" t="s">
         <v>27</v>
       </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>177</v>
+      </c>
       <c r="G25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" t="s">
         <v>28</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" t="s">
         <v>29</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" t="s">
         <v>30</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
+        <v>66</v>
+      </c>
+      <c r="O25" t="s">
         <v>31</v>
       </c>
+      <c r="P25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>68</v>
+      </c>
       <c r="R25" t="s">
+        <v>68</v>
+      </c>
+      <c r="S25" t="s">
+        <v>68</v>
+      </c>
+      <c r="T25" t="s">
         <v>65</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
+        <v>70</v>
+      </c>
+      <c r="V25" t="s">
         <v>32</v>
       </c>
-      <c r="V25" t="s">
+      <c r="X25" t="s">
         <v>33</v>
       </c>
+      <c r="Y25" t="s">
+        <v>70</v>
+      </c>
       <c r="Z25" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>3314</v>
+        <v>3312</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -1804,34 +2847,79 @@
       <c r="D26" t="s">
         <v>27</v>
       </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>178</v>
+      </c>
       <c r="G26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" t="s">
         <v>28</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" t="s">
         <v>29</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" t="s">
         <v>30</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
+        <v>66</v>
+      </c>
+      <c r="O26" t="s">
         <v>31</v>
       </c>
+      <c r="P26" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>68</v>
+      </c>
       <c r="R26" t="s">
+        <v>68</v>
+      </c>
+      <c r="S26" t="s">
+        <v>68</v>
+      </c>
+      <c r="T26" t="s">
         <v>65</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
+        <v>70</v>
+      </c>
+      <c r="V26" t="s">
         <v>32</v>
       </c>
-      <c r="V26" t="s">
+      <c r="X26" t="s">
         <v>33</v>
       </c>
+      <c r="Y26" t="s">
+        <v>70</v>
+      </c>
       <c r="Z26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>3315</v>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3313</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -1842,70 +2930,79 @@
       <c r="D27" t="s">
         <v>27</v>
       </c>
-      <c r="E27" t="s">
-        <v>68</v>
+      <c r="E27">
+        <v>7</v>
       </c>
       <c r="F27" t="s">
         <v>68</v>
       </c>
       <c r="G27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" t="s">
         <v>28</v>
       </c>
-      <c r="H27" t="s">
-        <v>69</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" t="s">
         <v>29</v>
       </c>
-      <c r="J27" t="s">
-        <v>69</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
+        <v>69</v>
+      </c>
+      <c r="M27" t="s">
         <v>30</v>
       </c>
-      <c r="L27" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
+        <v>66</v>
+      </c>
+      <c r="O27" t="s">
         <v>31</v>
       </c>
-      <c r="N27" t="s">
-        <v>66</v>
-      </c>
-      <c r="O27" t="s">
-        <v>68</v>
-      </c>
       <c r="P27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q27" t="s">
         <v>68</v>
       </c>
       <c r="R27" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" t="s">
+        <v>68</v>
+      </c>
+      <c r="T27" t="s">
         <v>65</v>
       </c>
-      <c r="S27" t="s">
-        <v>70</v>
-      </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
+        <v>70</v>
+      </c>
+      <c r="V27" t="s">
         <v>32</v>
       </c>
-      <c r="V27" t="s">
+      <c r="X27" t="s">
         <v>33</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z27" t="s">
         <v>67</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="AA27" t="s">
         <v>74</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AB27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>3318</v>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3314</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
@@ -1916,70 +3013,79 @@
       <c r="D28" t="s">
         <v>27</v>
       </c>
-      <c r="E28" t="s">
-        <v>68</v>
+      <c r="E28">
+        <v>2</v>
       </c>
       <c r="F28" t="s">
         <v>68</v>
       </c>
       <c r="G28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" t="s">
         <v>28</v>
       </c>
-      <c r="H28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" t="s">
         <v>29</v>
       </c>
-      <c r="J28" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
+        <v>69</v>
+      </c>
+      <c r="M28" t="s">
         <v>30</v>
       </c>
-      <c r="L28" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
+        <v>66</v>
+      </c>
+      <c r="O28" t="s">
         <v>31</v>
       </c>
-      <c r="N28" t="s">
-        <v>66</v>
-      </c>
-      <c r="O28" t="s">
-        <v>68</v>
-      </c>
       <c r="P28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q28" t="s">
         <v>68</v>
       </c>
       <c r="R28" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" t="s">
+        <v>68</v>
+      </c>
+      <c r="T28" t="s">
         <v>65</v>
       </c>
-      <c r="S28" t="s">
-        <v>70</v>
-      </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
+        <v>70</v>
+      </c>
+      <c r="V28" t="s">
         <v>32</v>
       </c>
-      <c r="V28" t="s">
+      <c r="X28" t="s">
         <v>33</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Y28" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z28" t="s">
         <v>67</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="AA28" t="s">
         <v>74</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="AB28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>3320</v>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>3315</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -1990,34 +3096,79 @@
       <c r="D29" t="s">
         <v>27</v>
       </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>68</v>
+      </c>
       <c r="G29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" t="s">
         <v>28</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
+        <v>69</v>
+      </c>
+      <c r="K29" t="s">
         <v>29</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
+        <v>69</v>
+      </c>
+      <c r="M29" t="s">
         <v>30</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
+        <v>66</v>
+      </c>
+      <c r="O29" t="s">
         <v>31</v>
       </c>
+      <c r="P29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>68</v>
+      </c>
       <c r="R29" t="s">
+        <v>68</v>
+      </c>
+      <c r="S29" t="s">
+        <v>68</v>
+      </c>
+      <c r="T29" t="s">
         <v>65</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
+        <v>70</v>
+      </c>
+      <c r="V29" t="s">
         <v>32</v>
       </c>
-      <c r="V29" t="s">
+      <c r="X29" t="s">
         <v>33</v>
       </c>
+      <c r="Y29" t="s">
+        <v>70</v>
+      </c>
       <c r="Z29" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>3321</v>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>3318</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
@@ -2028,34 +3179,79 @@
       <c r="D30" t="s">
         <v>27</v>
       </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
       <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" t="s">
         <v>28</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" t="s">
         <v>29</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
+        <v>69</v>
+      </c>
+      <c r="M30" t="s">
         <v>30</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
+        <v>66</v>
+      </c>
+      <c r="O30" t="s">
         <v>31</v>
       </c>
+      <c r="P30" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>68</v>
+      </c>
       <c r="R30" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" t="s">
+        <v>68</v>
+      </c>
+      <c r="T30" t="s">
         <v>65</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
+        <v>70</v>
+      </c>
+      <c r="V30" t="s">
         <v>32</v>
       </c>
-      <c r="V30" t="s">
+      <c r="X30" t="s">
         <v>33</v>
       </c>
+      <c r="Y30" t="s">
+        <v>70</v>
+      </c>
       <c r="Z30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>3322</v>
+        <v>3320</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -2066,34 +3262,79 @@
       <c r="D31" t="s">
         <v>27</v>
       </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>205</v>
+      </c>
       <c r="G31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" t="s">
         <v>28</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" t="s">
         <v>29</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
+        <v>69</v>
+      </c>
+      <c r="M31" t="s">
         <v>30</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
+        <v>66</v>
+      </c>
+      <c r="O31" t="s">
         <v>31</v>
       </c>
+      <c r="P31" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>68</v>
+      </c>
       <c r="R31" t="s">
+        <v>68</v>
+      </c>
+      <c r="S31" t="s">
+        <v>68</v>
+      </c>
+      <c r="T31" t="s">
         <v>65</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
+        <v>70</v>
+      </c>
+      <c r="V31" t="s">
         <v>32</v>
       </c>
-      <c r="V31" t="s">
+      <c r="X31" t="s">
         <v>33</v>
       </c>
+      <c r="Y31" t="s">
+        <v>70</v>
+      </c>
       <c r="Z31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>3323</v>
+        <v>3321</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
@@ -2104,34 +3345,79 @@
       <c r="D32" t="s">
         <v>27</v>
       </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>206</v>
+      </c>
       <c r="G32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" t="s">
         <v>28</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" t="s">
         <v>29</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
+        <v>69</v>
+      </c>
+      <c r="M32" t="s">
         <v>30</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
+        <v>66</v>
+      </c>
+      <c r="O32" t="s">
         <v>31</v>
       </c>
+      <c r="P32" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>68</v>
+      </c>
       <c r="R32" t="s">
+        <v>68</v>
+      </c>
+      <c r="S32" t="s">
+        <v>68</v>
+      </c>
+      <c r="T32" t="s">
         <v>65</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
+        <v>70</v>
+      </c>
+      <c r="V32" t="s">
         <v>32</v>
       </c>
-      <c r="V32" t="s">
+      <c r="X32" t="s">
         <v>33</v>
       </c>
+      <c r="Y32" t="s">
+        <v>70</v>
+      </c>
       <c r="Z32" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>3324</v>
+        <v>3322</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
@@ -2142,34 +3428,79 @@
       <c r="D33" t="s">
         <v>27</v>
       </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>207</v>
+      </c>
       <c r="G33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" t="s">
         <v>28</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K33" t="s">
         <v>29</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
+        <v>69</v>
+      </c>
+      <c r="M33" t="s">
         <v>30</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
+        <v>66</v>
+      </c>
+      <c r="O33" t="s">
         <v>31</v>
       </c>
+      <c r="P33" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>68</v>
+      </c>
       <c r="R33" t="s">
+        <v>68</v>
+      </c>
+      <c r="S33" t="s">
+        <v>68</v>
+      </c>
+      <c r="T33" t="s">
         <v>65</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
+        <v>70</v>
+      </c>
+      <c r="V33" t="s">
         <v>32</v>
       </c>
-      <c r="V33" t="s">
+      <c r="X33" t="s">
         <v>33</v>
       </c>
+      <c r="Y33" t="s">
+        <v>70</v>
+      </c>
       <c r="Z33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>3325</v>
+        <v>3323</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
@@ -2180,34 +3511,79 @@
       <c r="D34" t="s">
         <v>27</v>
       </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>208</v>
+      </c>
       <c r="G34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" t="s">
         <v>28</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K34" t="s">
         <v>29</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
+        <v>69</v>
+      </c>
+      <c r="M34" t="s">
         <v>30</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
+        <v>66</v>
+      </c>
+      <c r="O34" t="s">
         <v>31</v>
       </c>
+      <c r="P34" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>68</v>
+      </c>
       <c r="R34" t="s">
+        <v>68</v>
+      </c>
+      <c r="S34" t="s">
+        <v>68</v>
+      </c>
+      <c r="T34" t="s">
         <v>65</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
+        <v>70</v>
+      </c>
+      <c r="V34" t="s">
         <v>32</v>
       </c>
-      <c r="V34" t="s">
+      <c r="X34" t="s">
         <v>33</v>
       </c>
+      <c r="Y34" t="s">
+        <v>70</v>
+      </c>
       <c r="Z34" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
-        <v>3326</v>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3324</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -2218,70 +3594,79 @@
       <c r="D35" t="s">
         <v>27</v>
       </c>
-      <c r="E35" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" t="s">
-        <v>68</v>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>209</v>
       </c>
       <c r="G35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" t="s">
         <v>28</v>
       </c>
-      <c r="H35" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
         <v>29</v>
       </c>
-      <c r="J35" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
+        <v>69</v>
+      </c>
+      <c r="M35" t="s">
         <v>30</v>
       </c>
-      <c r="L35" t="s">
-        <v>66</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
+        <v>66</v>
+      </c>
+      <c r="O35" t="s">
         <v>31</v>
       </c>
-      <c r="N35" t="s">
-        <v>66</v>
-      </c>
-      <c r="O35" t="s">
-        <v>68</v>
-      </c>
       <c r="P35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q35" t="s">
         <v>68</v>
       </c>
       <c r="R35" t="s">
+        <v>68</v>
+      </c>
+      <c r="S35" t="s">
+        <v>68</v>
+      </c>
+      <c r="T35" t="s">
         <v>65</v>
       </c>
-      <c r="S35" t="s">
-        <v>70</v>
-      </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
+        <v>70</v>
+      </c>
+      <c r="V35" t="s">
         <v>32</v>
       </c>
-      <c r="V35" t="s">
+      <c r="X35" t="s">
         <v>33</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z35" t="s">
         <v>67</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="AA35" t="s">
         <v>74</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="AB35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>3331</v>
+        <v>3325</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
@@ -2292,34 +3677,79 @@
       <c r="D36" t="s">
         <v>27</v>
       </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>210</v>
+      </c>
       <c r="G36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I36" t="s">
         <v>28</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36" t="s">
         <v>29</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
+        <v>69</v>
+      </c>
+      <c r="M36" t="s">
         <v>30</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
+        <v>66</v>
+      </c>
+      <c r="O36" t="s">
         <v>31</v>
       </c>
+      <c r="P36" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>68</v>
+      </c>
       <c r="R36" t="s">
+        <v>68</v>
+      </c>
+      <c r="S36" t="s">
+        <v>68</v>
+      </c>
+      <c r="T36" t="s">
         <v>65</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
+        <v>70</v>
+      </c>
+      <c r="V36" t="s">
         <v>32</v>
       </c>
-      <c r="V36" t="s">
+      <c r="X36" t="s">
         <v>33</v>
       </c>
+      <c r="Y36" t="s">
+        <v>70</v>
+      </c>
       <c r="Z36" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>3332</v>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>3326</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -2330,34 +3760,79 @@
       <c r="D37" t="s">
         <v>27</v>
       </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
       <c r="G37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I37" t="s">
         <v>28</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
+        <v>69</v>
+      </c>
+      <c r="K37" t="s">
         <v>29</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
+        <v>69</v>
+      </c>
+      <c r="M37" t="s">
         <v>30</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
+        <v>66</v>
+      </c>
+      <c r="O37" t="s">
         <v>31</v>
       </c>
+      <c r="P37" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>68</v>
+      </c>
       <c r="R37" t="s">
+        <v>68</v>
+      </c>
+      <c r="S37" t="s">
+        <v>68</v>
+      </c>
+      <c r="T37" t="s">
         <v>65</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
+        <v>70</v>
+      </c>
+      <c r="V37" t="s">
         <v>32</v>
       </c>
-      <c r="V37" t="s">
+      <c r="X37" t="s">
         <v>33</v>
       </c>
+      <c r="Y37" t="s">
+        <v>70</v>
+      </c>
       <c r="Z37" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>3333</v>
+        <v>3331</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
@@ -2368,34 +3843,79 @@
       <c r="D38" t="s">
         <v>27</v>
       </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>182</v>
+      </c>
       <c r="G38" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38" t="s">
         <v>28</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" t="s">
         <v>29</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
+        <v>69</v>
+      </c>
+      <c r="M38" t="s">
         <v>30</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
+        <v>66</v>
+      </c>
+      <c r="O38" t="s">
         <v>31</v>
       </c>
+      <c r="P38" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>68</v>
+      </c>
       <c r="R38" t="s">
+        <v>68</v>
+      </c>
+      <c r="S38" t="s">
+        <v>68</v>
+      </c>
+      <c r="T38" t="s">
         <v>65</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
+        <v>70</v>
+      </c>
+      <c r="V38" t="s">
         <v>32</v>
       </c>
-      <c r="V38" t="s">
+      <c r="X38" t="s">
         <v>33</v>
       </c>
+      <c r="Y38" t="s">
+        <v>70</v>
+      </c>
       <c r="Z38" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>3334</v>
+        <v>3332</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
@@ -2406,34 +3926,79 @@
       <c r="D39" t="s">
         <v>27</v>
       </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>186</v>
+      </c>
       <c r="G39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" t="s">
         <v>28</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39" t="s">
         <v>29</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39" t="s">
         <v>30</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
+        <v>66</v>
+      </c>
+      <c r="O39" t="s">
         <v>31</v>
       </c>
+      <c r="P39" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>68</v>
+      </c>
       <c r="R39" t="s">
+        <v>68</v>
+      </c>
+      <c r="S39" t="s">
+        <v>68</v>
+      </c>
+      <c r="T39" t="s">
         <v>65</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
+        <v>70</v>
+      </c>
+      <c r="V39" t="s">
         <v>32</v>
       </c>
-      <c r="V39" t="s">
+      <c r="X39" t="s">
         <v>33</v>
       </c>
+      <c r="Y39" t="s">
+        <v>70</v>
+      </c>
       <c r="Z39" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>3335</v>
+        <v>3333</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
@@ -2444,34 +4009,79 @@
       <c r="D40" t="s">
         <v>27</v>
       </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>187</v>
+      </c>
       <c r="G40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" t="s">
         <v>28</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" t="s">
         <v>29</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40" t="s">
         <v>30</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
+        <v>66</v>
+      </c>
+      <c r="O40" t="s">
         <v>31</v>
       </c>
+      <c r="P40" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>68</v>
+      </c>
       <c r="R40" t="s">
+        <v>68</v>
+      </c>
+      <c r="S40" t="s">
+        <v>68</v>
+      </c>
+      <c r="T40" t="s">
         <v>65</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
+        <v>70</v>
+      </c>
+      <c r="V40" t="s">
         <v>32</v>
       </c>
-      <c r="V40" t="s">
+      <c r="X40" t="s">
         <v>33</v>
       </c>
+      <c r="Y40" t="s">
+        <v>70</v>
+      </c>
       <c r="Z40" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>3337</v>
+        <v>3334</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
@@ -2482,34 +4092,79 @@
       <c r="D41" t="s">
         <v>27</v>
       </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>188</v>
+      </c>
       <c r="G41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" t="s">
         <v>28</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" t="s">
         <v>29</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
+        <v>69</v>
+      </c>
+      <c r="M41" t="s">
         <v>30</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
+        <v>66</v>
+      </c>
+      <c r="O41" t="s">
         <v>31</v>
       </c>
+      <c r="P41" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>68</v>
+      </c>
       <c r="R41" t="s">
+        <v>68</v>
+      </c>
+      <c r="S41" t="s">
+        <v>68</v>
+      </c>
+      <c r="T41" t="s">
         <v>65</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
+        <v>70</v>
+      </c>
+      <c r="V41" t="s">
         <v>32</v>
       </c>
-      <c r="V41" t="s">
+      <c r="X41" t="s">
         <v>33</v>
       </c>
+      <c r="Y41" t="s">
+        <v>70</v>
+      </c>
       <c r="Z41" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>3338</v>
+        <v>3335</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
@@ -2520,34 +4175,79 @@
       <c r="D42" t="s">
         <v>27</v>
       </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>189</v>
+      </c>
       <c r="G42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I42" t="s">
         <v>28</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
+        <v>69</v>
+      </c>
+      <c r="K42" t="s">
         <v>29</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>69</v>
+      </c>
+      <c r="M42" t="s">
         <v>30</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
+        <v>66</v>
+      </c>
+      <c r="O42" t="s">
         <v>31</v>
       </c>
+      <c r="P42" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>68</v>
+      </c>
       <c r="R42" t="s">
+        <v>68</v>
+      </c>
+      <c r="S42" t="s">
+        <v>68</v>
+      </c>
+      <c r="T42" t="s">
         <v>65</v>
       </c>
-      <c r="T42" t="s">
+      <c r="U42" t="s">
+        <v>70</v>
+      </c>
+      <c r="V42" t="s">
         <v>32</v>
       </c>
-      <c r="V42" t="s">
+      <c r="X42" t="s">
         <v>33</v>
       </c>
+      <c r="Y42" t="s">
+        <v>70</v>
+      </c>
       <c r="Z42" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB42" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>3339</v>
+        <v>3337</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
@@ -2558,34 +4258,79 @@
       <c r="D43" t="s">
         <v>27</v>
       </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>194</v>
+      </c>
       <c r="G43" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" t="s">
         <v>28</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
+        <v>69</v>
+      </c>
+      <c r="K43" t="s">
         <v>29</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
+        <v>69</v>
+      </c>
+      <c r="M43" t="s">
         <v>30</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
+        <v>66</v>
+      </c>
+      <c r="O43" t="s">
         <v>31</v>
       </c>
+      <c r="P43" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>68</v>
+      </c>
       <c r="R43" t="s">
+        <v>68</v>
+      </c>
+      <c r="S43" t="s">
+        <v>68</v>
+      </c>
+      <c r="T43" t="s">
         <v>65</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
+        <v>70</v>
+      </c>
+      <c r="V43" t="s">
         <v>32</v>
       </c>
-      <c r="V43" t="s">
+      <c r="X43" t="s">
         <v>33</v>
       </c>
+      <c r="Y43" t="s">
+        <v>70</v>
+      </c>
       <c r="Z43" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>3340</v>
+        <v>3338</v>
       </c>
       <c r="B44" t="s">
         <v>25</v>
@@ -2596,34 +4341,79 @@
       <c r="D44" t="s">
         <v>27</v>
       </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>195</v>
+      </c>
       <c r="G44" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I44" t="s">
         <v>28</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" t="s">
         <v>29</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
+        <v>69</v>
+      </c>
+      <c r="M44" t="s">
         <v>30</v>
       </c>
-      <c r="M44" t="s">
+      <c r="N44" t="s">
+        <v>66</v>
+      </c>
+      <c r="O44" t="s">
         <v>31</v>
       </c>
+      <c r="P44" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>68</v>
+      </c>
       <c r="R44" t="s">
+        <v>68</v>
+      </c>
+      <c r="S44" t="s">
+        <v>68</v>
+      </c>
+      <c r="T44" t="s">
         <v>65</v>
       </c>
-      <c r="T44" t="s">
+      <c r="U44" t="s">
+        <v>70</v>
+      </c>
+      <c r="V44" t="s">
         <v>32</v>
       </c>
-      <c r="V44" t="s">
+      <c r="X44" t="s">
         <v>33</v>
       </c>
+      <c r="Y44" t="s">
+        <v>70</v>
+      </c>
       <c r="Z44" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>3341</v>
+        <v>3339</v>
       </c>
       <c r="B45" t="s">
         <v>25</v>
@@ -2634,34 +4424,79 @@
       <c r="D45" t="s">
         <v>27</v>
       </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>196</v>
+      </c>
       <c r="G45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I45" t="s">
         <v>28</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
+        <v>69</v>
+      </c>
+      <c r="K45" t="s">
         <v>29</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
+        <v>69</v>
+      </c>
+      <c r="M45" t="s">
         <v>30</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
+        <v>66</v>
+      </c>
+      <c r="O45" t="s">
         <v>31</v>
       </c>
+      <c r="P45" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>68</v>
+      </c>
       <c r="R45" t="s">
+        <v>68</v>
+      </c>
+      <c r="S45" t="s">
+        <v>68</v>
+      </c>
+      <c r="T45" t="s">
         <v>65</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
+        <v>70</v>
+      </c>
+      <c r="V45" t="s">
         <v>32</v>
       </c>
-      <c r="V45" t="s">
+      <c r="X45" t="s">
         <v>33</v>
       </c>
+      <c r="Y45" t="s">
+        <v>70</v>
+      </c>
       <c r="Z45" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>3342</v>
+        <v>3340</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -2672,34 +4507,79 @@
       <c r="D46" t="s">
         <v>27</v>
       </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>197</v>
+      </c>
       <c r="G46" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" t="s">
         <v>28</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
+        <v>69</v>
+      </c>
+      <c r="K46" t="s">
         <v>29</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
+        <v>69</v>
+      </c>
+      <c r="M46" t="s">
         <v>30</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
+        <v>66</v>
+      </c>
+      <c r="O46" t="s">
         <v>31</v>
       </c>
+      <c r="P46" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>68</v>
+      </c>
       <c r="R46" t="s">
+        <v>68</v>
+      </c>
+      <c r="S46" t="s">
+        <v>68</v>
+      </c>
+      <c r="T46" t="s">
         <v>65</v>
       </c>
-      <c r="T46" t="s">
+      <c r="U46" t="s">
+        <v>70</v>
+      </c>
+      <c r="V46" t="s">
         <v>32</v>
       </c>
-      <c r="V46" t="s">
+      <c r="X46" t="s">
         <v>33</v>
       </c>
+      <c r="Y46" t="s">
+        <v>70</v>
+      </c>
       <c r="Z46" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>3343</v>
+        <v>3341</v>
       </c>
       <c r="B47" t="s">
         <v>25</v>
@@ -2710,28 +4590,239 @@
       <c r="D47" t="s">
         <v>27</v>
       </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>198</v>
+      </c>
       <c r="G47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I47" t="s">
         <v>28</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
+        <v>69</v>
+      </c>
+      <c r="K47" t="s">
         <v>29</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
+        <v>69</v>
+      </c>
+      <c r="M47" t="s">
         <v>30</v>
       </c>
-      <c r="M47" t="s">
+      <c r="N47" t="s">
+        <v>66</v>
+      </c>
+      <c r="O47" t="s">
         <v>31</v>
       </c>
+      <c r="P47" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>68</v>
+      </c>
       <c r="R47" t="s">
+        <v>68</v>
+      </c>
+      <c r="S47" t="s">
+        <v>68</v>
+      </c>
+      <c r="T47" t="s">
         <v>65</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
+        <v>70</v>
+      </c>
+      <c r="V47" t="s">
         <v>32</v>
       </c>
-      <c r="V47" t="s">
+      <c r="X47" t="s">
         <v>33</v>
       </c>
+      <c r="Y47" t="s">
+        <v>70</v>
+      </c>
       <c r="Z47" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3342</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>199</v>
+      </c>
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I48" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" t="s">
+        <v>69</v>
+      </c>
+      <c r="K48" t="s">
+        <v>29</v>
+      </c>
+      <c r="L48" t="s">
+        <v>69</v>
+      </c>
+      <c r="M48" t="s">
+        <v>30</v>
+      </c>
+      <c r="N48" t="s">
+        <v>66</v>
+      </c>
+      <c r="O48" t="s">
+        <v>31</v>
+      </c>
+      <c r="P48" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>68</v>
+      </c>
+      <c r="R48" t="s">
+        <v>68</v>
+      </c>
+      <c r="S48" t="s">
+        <v>68</v>
+      </c>
+      <c r="T48" t="s">
+        <v>65</v>
+      </c>
+      <c r="U48" t="s">
+        <v>70</v>
+      </c>
+      <c r="V48" t="s">
+        <v>32</v>
+      </c>
+      <c r="X48" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3343</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>202</v>
+      </c>
+      <c r="G49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I49" t="s">
+        <v>28</v>
+      </c>
+      <c r="J49" t="s">
+        <v>69</v>
+      </c>
+      <c r="K49" t="s">
+        <v>29</v>
+      </c>
+      <c r="L49" t="s">
+        <v>69</v>
+      </c>
+      <c r="M49" t="s">
+        <v>30</v>
+      </c>
+      <c r="N49" t="s">
+        <v>66</v>
+      </c>
+      <c r="O49" t="s">
+        <v>31</v>
+      </c>
+      <c r="P49" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>68</v>
+      </c>
+      <c r="R49" t="s">
+        <v>68</v>
+      </c>
+      <c r="S49" t="s">
+        <v>68</v>
+      </c>
+      <c r="T49" t="s">
+        <v>65</v>
+      </c>
+      <c r="U49" t="s">
+        <v>70</v>
+      </c>
+      <c r="V49" t="s">
+        <v>32</v>
+      </c>
+      <c r="X49" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB49" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2742,10 +4833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2817,246 +4908,268 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
       </c>
       <c r="C27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating IFCB standardizer spreadsheet
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A9AD8C-CD8D-6947-A884-9A3CB6C8EFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45880E8-F631-BC4E-943C-0E8C9D0B2F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="1560" windowWidth="30240" windowHeight="17360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AA$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AC$49</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="100">
   <si>
     <t>Project_ID</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>degree</t>
-  </si>
-  <si>
-    <t>object_biovolume, object_summed_biovolume</t>
   </si>
   <si>
     <t>missing_index</t>
@@ -309,13 +306,37 @@
   </si>
   <si>
     <t>object_minoraxislength</t>
+  </si>
+  <si>
+    <t>Missing_index</t>
+  </si>
+  <si>
+    <t>object_biovolume,object_summedbiovolume</t>
+  </si>
+  <si>
+    <t>Sampling_date_field</t>
+  </si>
+  <si>
+    <t>Sampling_time_field</t>
+  </si>
+  <si>
+    <t>object_date</t>
+  </si>
+  <si>
+    <t>object_time</t>
+  </si>
+  <si>
+    <t>Name of the sampling date (yyyymmdd in UTC) column in project export file</t>
+  </si>
+  <si>
+    <t>Name of the sampling time (hhmmss in UTC) column in project export file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +358,21 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -352,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -386,11 +422,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -410,6 +459,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:T49"/>
+    <sheetView topLeftCell="F1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -766,19 +822,20 @@
     <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,79 +849,85 @@
         <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -898,41 +961,47 @@
       <c r="N2" t="s">
         <v>45</v>
       </c>
-      <c r="R2" t="s">
+      <c r="O2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" t="s">
-        <v>48</v>
-      </c>
       <c r="U2" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W2" t="s">
         <v>81</v>
       </c>
       <c r="X2" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y2" t="s">
         <v>80</v>
       </c>
       <c r="Z2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -966,41 +1035,47 @@
       <c r="N3" t="s">
         <v>45</v>
       </c>
-      <c r="R3" t="s">
+      <c r="O3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" t="s">
         <v>39</v>
       </c>
-      <c r="S3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" t="s">
-        <v>48</v>
-      </c>
       <c r="U3" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W3" t="s">
         <v>81</v>
       </c>
       <c r="X3" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y3" t="s">
         <v>80</v>
       </c>
       <c r="Z3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB3" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1034,41 +1109,47 @@
       <c r="N4" t="s">
         <v>45</v>
       </c>
-      <c r="R4" t="s">
+      <c r="O4" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T4" t="s">
         <v>39</v>
       </c>
-      <c r="S4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" t="s">
-        <v>48</v>
-      </c>
       <c r="U4" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V4" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W4" t="s">
         <v>81</v>
       </c>
       <c r="X4" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y4" t="s">
         <v>80</v>
       </c>
       <c r="Z4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB4" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1079,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1105,41 +1186,47 @@
       <c r="N5" t="s">
         <v>45</v>
       </c>
-      <c r="R5" t="s">
+      <c r="O5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T5" t="s">
         <v>39</v>
       </c>
-      <c r="S5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" t="s">
-        <v>48</v>
-      </c>
       <c r="U5" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W5" t="s">
         <v>81</v>
       </c>
       <c r="X5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y5" t="s">
         <v>80</v>
       </c>
       <c r="Z5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB5" t="s">
         <v>8</v>
       </c>
-      <c r="AA5" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3292</v>
       </c>
@@ -1173,41 +1260,47 @@
       <c r="N6" t="s">
         <v>45</v>
       </c>
-      <c r="R6" t="s">
+      <c r="O6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T6" t="s">
         <v>39</v>
       </c>
-      <c r="S6" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" t="s">
-        <v>48</v>
-      </c>
       <c r="U6" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V6" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W6" t="s">
         <v>81</v>
       </c>
       <c r="X6" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y6" t="s">
         <v>80</v>
       </c>
       <c r="Z6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB6" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3293</v>
       </c>
@@ -1241,41 +1334,47 @@
       <c r="N7" t="s">
         <v>45</v>
       </c>
-      <c r="R7" t="s">
+      <c r="O7" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T7" t="s">
         <v>39</v>
       </c>
-      <c r="S7" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" t="s">
-        <v>48</v>
-      </c>
       <c r="U7" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V7" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W7" t="s">
         <v>81</v>
       </c>
       <c r="X7" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y7" t="s">
         <v>80</v>
       </c>
       <c r="Z7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB7" t="s">
         <v>8</v>
       </c>
-      <c r="AA7" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3294</v>
       </c>
@@ -1309,41 +1408,47 @@
       <c r="N8" t="s">
         <v>45</v>
       </c>
-      <c r="R8" t="s">
+      <c r="O8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T8" t="s">
         <v>39</v>
       </c>
-      <c r="S8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T8" t="s">
-        <v>48</v>
-      </c>
       <c r="U8" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V8" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W8" t="s">
         <v>81</v>
       </c>
       <c r="X8" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y8" t="s">
         <v>80</v>
       </c>
       <c r="Z8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB8" t="s">
         <v>8</v>
       </c>
-      <c r="AA8" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3295</v>
       </c>
@@ -1377,41 +1482,47 @@
       <c r="N9" t="s">
         <v>45</v>
       </c>
-      <c r="R9" t="s">
+      <c r="O9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T9" t="s">
         <v>39</v>
       </c>
-      <c r="S9" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" t="s">
-        <v>48</v>
-      </c>
       <c r="U9" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V9" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W9" t="s">
         <v>81</v>
       </c>
       <c r="X9" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y9" t="s">
         <v>80</v>
       </c>
       <c r="Z9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB9" t="s">
         <v>8</v>
       </c>
-      <c r="AA9" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3296</v>
       </c>
@@ -1445,41 +1556,47 @@
       <c r="N10" t="s">
         <v>45</v>
       </c>
-      <c r="R10" t="s">
+      <c r="O10" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T10" t="s">
         <v>39</v>
       </c>
-      <c r="S10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T10" t="s">
-        <v>48</v>
-      </c>
       <c r="U10" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V10" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W10" t="s">
         <v>81</v>
       </c>
       <c r="X10" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y10" t="s">
         <v>80</v>
       </c>
       <c r="Z10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB10" t="s">
         <v>8</v>
       </c>
-      <c r="AA10" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3297</v>
       </c>
@@ -1490,7 +1607,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -1516,41 +1633,47 @@
       <c r="N11" t="s">
         <v>45</v>
       </c>
-      <c r="R11" t="s">
+      <c r="O11" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T11" t="s">
         <v>39</v>
       </c>
-      <c r="S11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T11" t="s">
-        <v>48</v>
-      </c>
       <c r="U11" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V11" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W11" t="s">
         <v>81</v>
       </c>
       <c r="X11" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y11" t="s">
         <v>80</v>
       </c>
       <c r="Z11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB11" t="s">
         <v>8</v>
       </c>
-      <c r="AA11" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3298</v>
       </c>
@@ -1561,7 +1684,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1587,41 +1710,47 @@
       <c r="N12" t="s">
         <v>45</v>
       </c>
-      <c r="R12" t="s">
+      <c r="O12" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T12" t="s">
         <v>39</v>
       </c>
-      <c r="S12" t="s">
-        <v>46</v>
-      </c>
-      <c r="T12" t="s">
-        <v>48</v>
-      </c>
       <c r="U12" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V12" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W12" t="s">
         <v>81</v>
       </c>
       <c r="X12" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y12" t="s">
         <v>80</v>
       </c>
       <c r="Z12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB12" t="s">
         <v>8</v>
       </c>
-      <c r="AA12" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3299</v>
       </c>
@@ -1632,7 +1761,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -1658,41 +1787,47 @@
       <c r="N13" t="s">
         <v>45</v>
       </c>
-      <c r="R13" t="s">
+      <c r="O13" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T13" t="s">
         <v>39</v>
       </c>
-      <c r="S13" t="s">
-        <v>46</v>
-      </c>
-      <c r="T13" t="s">
-        <v>48</v>
-      </c>
       <c r="U13" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V13" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W13" t="s">
         <v>81</v>
       </c>
       <c r="X13" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y13" t="s">
         <v>80</v>
       </c>
       <c r="Z13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB13" t="s">
         <v>8</v>
       </c>
-      <c r="AA13" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3300</v>
       </c>
@@ -1726,41 +1861,47 @@
       <c r="N14" t="s">
         <v>45</v>
       </c>
-      <c r="R14" t="s">
+      <c r="O14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T14" t="s">
         <v>39</v>
       </c>
-      <c r="S14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T14" t="s">
-        <v>48</v>
-      </c>
       <c r="U14" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W14" t="s">
         <v>81</v>
       </c>
       <c r="X14" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y14" t="s">
         <v>80</v>
       </c>
       <c r="Z14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB14" t="s">
         <v>8</v>
       </c>
-      <c r="AA14" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC14" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3301</v>
       </c>
@@ -1794,41 +1935,47 @@
       <c r="N15" t="s">
         <v>45</v>
       </c>
-      <c r="R15" t="s">
+      <c r="O15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T15" t="s">
         <v>39</v>
       </c>
-      <c r="S15" t="s">
-        <v>46</v>
-      </c>
-      <c r="T15" t="s">
-        <v>48</v>
-      </c>
       <c r="U15" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W15" t="s">
         <v>81</v>
       </c>
       <c r="X15" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y15" t="s">
         <v>80</v>
       </c>
       <c r="Z15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB15" t="s">
         <v>8</v>
       </c>
-      <c r="AA15" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3302</v>
       </c>
@@ -1862,41 +2009,47 @@
       <c r="N16" t="s">
         <v>45</v>
       </c>
-      <c r="R16" t="s">
+      <c r="O16" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T16" t="s">
         <v>39</v>
       </c>
-      <c r="S16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T16" t="s">
-        <v>48</v>
-      </c>
       <c r="U16" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V16" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W16" t="s">
         <v>81</v>
       </c>
       <c r="X16" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y16" t="s">
         <v>80</v>
       </c>
       <c r="Z16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB16" t="s">
         <v>8</v>
       </c>
-      <c r="AA16" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3303</v>
       </c>
@@ -1930,41 +2083,47 @@
       <c r="N17" t="s">
         <v>45</v>
       </c>
-      <c r="R17" t="s">
+      <c r="O17" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T17" t="s">
         <v>39</v>
       </c>
-      <c r="S17" t="s">
-        <v>46</v>
-      </c>
-      <c r="T17" t="s">
-        <v>48</v>
-      </c>
       <c r="U17" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V17" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W17" t="s">
         <v>81</v>
       </c>
       <c r="X17" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y17" t="s">
         <v>80</v>
       </c>
       <c r="Z17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB17" t="s">
         <v>8</v>
       </c>
-      <c r="AA17" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3304</v>
       </c>
@@ -1998,41 +2157,47 @@
       <c r="N18" t="s">
         <v>45</v>
       </c>
-      <c r="R18" t="s">
+      <c r="O18" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T18" t="s">
         <v>39</v>
       </c>
-      <c r="S18" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" t="s">
-        <v>48</v>
-      </c>
       <c r="U18" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V18" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W18" t="s">
         <v>81</v>
       </c>
       <c r="X18" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y18" t="s">
         <v>80</v>
       </c>
       <c r="Z18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB18" t="s">
         <v>8</v>
       </c>
-      <c r="AA18" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3305</v>
       </c>
@@ -2066,41 +2231,47 @@
       <c r="N19" t="s">
         <v>45</v>
       </c>
-      <c r="R19" t="s">
+      <c r="O19" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P19" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T19" t="s">
         <v>39</v>
       </c>
-      <c r="S19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T19" t="s">
-        <v>48</v>
-      </c>
       <c r="U19" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V19" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W19" t="s">
         <v>81</v>
       </c>
       <c r="X19" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y19" t="s">
         <v>80</v>
       </c>
       <c r="Z19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB19" t="s">
         <v>8</v>
       </c>
-      <c r="AA19" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3306</v>
       </c>
@@ -2134,41 +2305,47 @@
       <c r="N20" t="s">
         <v>45</v>
       </c>
-      <c r="R20" t="s">
+      <c r="O20" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T20" t="s">
         <v>39</v>
       </c>
-      <c r="S20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" t="s">
-        <v>48</v>
-      </c>
       <c r="U20" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V20" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W20" t="s">
         <v>81</v>
       </c>
       <c r="X20" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y20" t="s">
         <v>80</v>
       </c>
       <c r="Z20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB20" t="s">
         <v>8</v>
       </c>
-      <c r="AA20" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC20" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3307</v>
       </c>
@@ -2202,41 +2379,47 @@
       <c r="N21" t="s">
         <v>45</v>
       </c>
-      <c r="R21" t="s">
+      <c r="O21" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T21" t="s">
         <v>39</v>
       </c>
-      <c r="S21" t="s">
-        <v>46</v>
-      </c>
-      <c r="T21" t="s">
-        <v>48</v>
-      </c>
       <c r="U21" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V21" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W21" t="s">
         <v>81</v>
       </c>
       <c r="X21" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y21" t="s">
         <v>80</v>
       </c>
       <c r="Z21" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB21" t="s">
         <v>8</v>
       </c>
-      <c r="AA21" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3308</v>
       </c>
@@ -2270,41 +2453,47 @@
       <c r="N22" t="s">
         <v>45</v>
       </c>
-      <c r="R22" t="s">
+      <c r="O22" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T22" t="s">
         <v>39</v>
       </c>
-      <c r="S22" t="s">
-        <v>46</v>
-      </c>
-      <c r="T22" t="s">
-        <v>48</v>
-      </c>
       <c r="U22" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V22" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W22" t="s">
         <v>81</v>
       </c>
       <c r="X22" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y22" t="s">
         <v>80</v>
       </c>
       <c r="Z22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB22" t="s">
         <v>8</v>
       </c>
-      <c r="AA22" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3309</v>
       </c>
@@ -2338,41 +2527,47 @@
       <c r="N23" t="s">
         <v>45</v>
       </c>
-      <c r="R23" t="s">
+      <c r="O23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T23" t="s">
         <v>39</v>
       </c>
-      <c r="S23" t="s">
-        <v>46</v>
-      </c>
-      <c r="T23" t="s">
-        <v>48</v>
-      </c>
       <c r="U23" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V23" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W23" t="s">
         <v>81</v>
       </c>
       <c r="X23" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y23" t="s">
         <v>80</v>
       </c>
       <c r="Z23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB23" t="s">
         <v>8</v>
       </c>
-      <c r="AA23" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3310</v>
       </c>
@@ -2406,41 +2601,47 @@
       <c r="N24" t="s">
         <v>45</v>
       </c>
-      <c r="R24" t="s">
+      <c r="O24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T24" t="s">
         <v>39</v>
       </c>
-      <c r="S24" t="s">
-        <v>46</v>
-      </c>
-      <c r="T24" t="s">
-        <v>48</v>
-      </c>
       <c r="U24" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V24" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W24" t="s">
         <v>81</v>
       </c>
       <c r="X24" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y24" t="s">
         <v>80</v>
       </c>
       <c r="Z24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB24" t="s">
         <v>8</v>
       </c>
-      <c r="AA24" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3311</v>
       </c>
@@ -2474,41 +2675,47 @@
       <c r="N25" t="s">
         <v>45</v>
       </c>
-      <c r="R25" t="s">
+      <c r="O25" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T25" t="s">
         <v>39</v>
       </c>
-      <c r="S25" t="s">
-        <v>46</v>
-      </c>
-      <c r="T25" t="s">
-        <v>48</v>
-      </c>
       <c r="U25" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V25" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W25" t="s">
         <v>81</v>
       </c>
       <c r="X25" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y25" t="s">
         <v>80</v>
       </c>
       <c r="Z25" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB25" t="s">
         <v>8</v>
       </c>
-      <c r="AA25" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3312</v>
       </c>
@@ -2542,41 +2749,47 @@
       <c r="N26" t="s">
         <v>45</v>
       </c>
-      <c r="R26" t="s">
+      <c r="O26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T26" t="s">
         <v>39</v>
       </c>
-      <c r="S26" t="s">
-        <v>46</v>
-      </c>
-      <c r="T26" t="s">
-        <v>48</v>
-      </c>
       <c r="U26" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V26" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W26" t="s">
         <v>81</v>
       </c>
       <c r="X26" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y26" t="s">
         <v>80</v>
       </c>
       <c r="Z26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB26" t="s">
         <v>8</v>
       </c>
-      <c r="AA26" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3313</v>
       </c>
@@ -2587,7 +2800,7 @@
         <v>3</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -2613,41 +2826,47 @@
       <c r="N27" t="s">
         <v>45</v>
       </c>
-      <c r="R27" t="s">
+      <c r="O27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T27" t="s">
         <v>39</v>
       </c>
-      <c r="S27" t="s">
-        <v>46</v>
-      </c>
-      <c r="T27" t="s">
-        <v>48</v>
-      </c>
       <c r="U27" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V27" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W27" t="s">
         <v>81</v>
       </c>
       <c r="X27" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y27" t="s">
         <v>80</v>
       </c>
       <c r="Z27" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB27" t="s">
         <v>8</v>
       </c>
-      <c r="AA27" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3314</v>
       </c>
@@ -2681,41 +2900,47 @@
       <c r="N28" t="s">
         <v>45</v>
       </c>
-      <c r="R28" t="s">
+      <c r="O28" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T28" t="s">
         <v>39</v>
       </c>
-      <c r="S28" t="s">
-        <v>46</v>
-      </c>
-      <c r="T28" t="s">
-        <v>48</v>
-      </c>
       <c r="U28" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V28" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W28" t="s">
         <v>81</v>
       </c>
       <c r="X28" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y28" t="s">
         <v>80</v>
       </c>
       <c r="Z28" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB28" t="s">
         <v>8</v>
       </c>
-      <c r="AA28" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>3315</v>
       </c>
@@ -2749,41 +2974,47 @@
       <c r="N29" t="s">
         <v>45</v>
       </c>
-      <c r="R29" t="s">
+      <c r="O29" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T29" t="s">
         <v>39</v>
       </c>
-      <c r="S29" t="s">
-        <v>46</v>
-      </c>
-      <c r="T29" t="s">
-        <v>48</v>
-      </c>
       <c r="U29" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V29" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W29" t="s">
         <v>81</v>
       </c>
       <c r="X29" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y29" t="s">
         <v>80</v>
       </c>
       <c r="Z29" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB29" t="s">
         <v>8</v>
       </c>
-      <c r="AA29" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC29" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>3318</v>
       </c>
@@ -2817,41 +3048,47 @@
       <c r="N30" t="s">
         <v>45</v>
       </c>
-      <c r="R30" t="s">
+      <c r="O30" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T30" t="s">
         <v>39</v>
       </c>
-      <c r="S30" t="s">
-        <v>46</v>
-      </c>
-      <c r="T30" t="s">
-        <v>48</v>
-      </c>
       <c r="U30" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V30" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W30" t="s">
         <v>81</v>
       </c>
       <c r="X30" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y30" t="s">
         <v>80</v>
       </c>
       <c r="Z30" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB30" t="s">
         <v>8</v>
       </c>
-      <c r="AA30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC30" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3320</v>
       </c>
@@ -2885,41 +3122,47 @@
       <c r="N31" t="s">
         <v>45</v>
       </c>
-      <c r="R31" t="s">
+      <c r="O31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P31" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T31" t="s">
         <v>39</v>
       </c>
-      <c r="S31" t="s">
-        <v>46</v>
-      </c>
-      <c r="T31" t="s">
-        <v>48</v>
-      </c>
       <c r="U31" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V31" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W31" t="s">
         <v>81</v>
       </c>
       <c r="X31" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y31" t="s">
         <v>80</v>
       </c>
       <c r="Z31" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB31" t="s">
         <v>8</v>
       </c>
-      <c r="AA31" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC31" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3321</v>
       </c>
@@ -2953,41 +3196,47 @@
       <c r="N32" t="s">
         <v>45</v>
       </c>
-      <c r="R32" t="s">
+      <c r="O32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T32" t="s">
         <v>39</v>
       </c>
-      <c r="S32" t="s">
-        <v>46</v>
-      </c>
-      <c r="T32" t="s">
-        <v>48</v>
-      </c>
       <c r="U32" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V32" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W32" t="s">
         <v>81</v>
       </c>
       <c r="X32" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y32" t="s">
         <v>80</v>
       </c>
       <c r="Z32" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB32" t="s">
         <v>8</v>
       </c>
-      <c r="AA32" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC32" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3322</v>
       </c>
@@ -3021,41 +3270,47 @@
       <c r="N33" t="s">
         <v>45</v>
       </c>
-      <c r="R33" t="s">
+      <c r="O33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P33" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T33" t="s">
         <v>39</v>
       </c>
-      <c r="S33" t="s">
-        <v>46</v>
-      </c>
-      <c r="T33" t="s">
-        <v>48</v>
-      </c>
       <c r="U33" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V33" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W33" t="s">
         <v>81</v>
       </c>
       <c r="X33" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y33" t="s">
         <v>80</v>
       </c>
       <c r="Z33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB33" t="s">
         <v>8</v>
       </c>
-      <c r="AA33" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3323</v>
       </c>
@@ -3089,41 +3344,47 @@
       <c r="N34" t="s">
         <v>45</v>
       </c>
-      <c r="R34" t="s">
+      <c r="O34" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T34" t="s">
         <v>39</v>
       </c>
-      <c r="S34" t="s">
-        <v>46</v>
-      </c>
-      <c r="T34" t="s">
-        <v>48</v>
-      </c>
       <c r="U34" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V34" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W34" t="s">
         <v>81</v>
       </c>
       <c r="X34" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y34" t="s">
         <v>80</v>
       </c>
       <c r="Z34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB34" t="s">
         <v>8</v>
       </c>
-      <c r="AA34" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC34" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3324</v>
       </c>
@@ -3157,41 +3418,47 @@
       <c r="N35" t="s">
         <v>45</v>
       </c>
-      <c r="R35" t="s">
+      <c r="O35" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T35" t="s">
         <v>39</v>
       </c>
-      <c r="S35" t="s">
-        <v>46</v>
-      </c>
-      <c r="T35" t="s">
-        <v>48</v>
-      </c>
       <c r="U35" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V35" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W35" t="s">
         <v>81</v>
       </c>
       <c r="X35" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y35" t="s">
         <v>80</v>
       </c>
       <c r="Z35" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB35" t="s">
         <v>8</v>
       </c>
-      <c r="AA35" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3325</v>
       </c>
@@ -3225,41 +3492,47 @@
       <c r="N36" t="s">
         <v>45</v>
       </c>
-      <c r="R36" t="s">
+      <c r="O36" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T36" t="s">
         <v>39</v>
       </c>
-      <c r="S36" t="s">
-        <v>46</v>
-      </c>
-      <c r="T36" t="s">
-        <v>48</v>
-      </c>
       <c r="U36" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V36" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W36" t="s">
         <v>81</v>
       </c>
       <c r="X36" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y36" t="s">
         <v>80</v>
       </c>
       <c r="Z36" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB36" t="s">
         <v>8</v>
       </c>
-      <c r="AA36" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC36" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>3326</v>
       </c>
@@ -3293,41 +3566,47 @@
       <c r="N37" t="s">
         <v>45</v>
       </c>
-      <c r="R37" t="s">
+      <c r="O37" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T37" t="s">
         <v>39</v>
       </c>
-      <c r="S37" t="s">
-        <v>46</v>
-      </c>
-      <c r="T37" t="s">
-        <v>48</v>
-      </c>
       <c r="U37" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V37" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W37" t="s">
         <v>81</v>
       </c>
       <c r="X37" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y37" t="s">
         <v>80</v>
       </c>
       <c r="Z37" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB37" t="s">
         <v>8</v>
       </c>
-      <c r="AA37" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3331</v>
       </c>
@@ -3361,41 +3640,47 @@
       <c r="N38" t="s">
         <v>45</v>
       </c>
-      <c r="R38" t="s">
+      <c r="O38" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P38" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T38" t="s">
         <v>39</v>
       </c>
-      <c r="S38" t="s">
-        <v>46</v>
-      </c>
-      <c r="T38" t="s">
-        <v>48</v>
-      </c>
       <c r="U38" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V38" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W38" t="s">
         <v>81</v>
       </c>
       <c r="X38" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y38" t="s">
         <v>80</v>
       </c>
       <c r="Z38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB38" t="s">
         <v>8</v>
       </c>
-      <c r="AA38" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC38" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3332</v>
       </c>
@@ -3429,41 +3714,47 @@
       <c r="N39" t="s">
         <v>45</v>
       </c>
-      <c r="R39" t="s">
+      <c r="O39" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T39" t="s">
         <v>39</v>
       </c>
-      <c r="S39" t="s">
-        <v>46</v>
-      </c>
-      <c r="T39" t="s">
-        <v>48</v>
-      </c>
       <c r="U39" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V39" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W39" t="s">
         <v>81</v>
       </c>
       <c r="X39" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y39" t="s">
         <v>80</v>
       </c>
       <c r="Z39" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB39" t="s">
         <v>8</v>
       </c>
-      <c r="AA39" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC39" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3333</v>
       </c>
@@ -3497,41 +3788,47 @@
       <c r="N40" t="s">
         <v>45</v>
       </c>
-      <c r="R40" t="s">
+      <c r="O40" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T40" t="s">
         <v>39</v>
       </c>
-      <c r="S40" t="s">
-        <v>46</v>
-      </c>
-      <c r="T40" t="s">
-        <v>48</v>
-      </c>
       <c r="U40" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V40" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W40" t="s">
         <v>81</v>
       </c>
       <c r="X40" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y40" t="s">
         <v>80</v>
       </c>
       <c r="Z40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB40" t="s">
         <v>8</v>
       </c>
-      <c r="AA40" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC40" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3334</v>
       </c>
@@ -3565,41 +3862,47 @@
       <c r="N41" t="s">
         <v>45</v>
       </c>
-      <c r="R41" t="s">
+      <c r="O41" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P41" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T41" t="s">
         <v>39</v>
       </c>
-      <c r="S41" t="s">
-        <v>46</v>
-      </c>
-      <c r="T41" t="s">
-        <v>48</v>
-      </c>
       <c r="U41" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V41" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W41" t="s">
         <v>81</v>
       </c>
       <c r="X41" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y41" t="s">
         <v>80</v>
       </c>
       <c r="Z41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB41" t="s">
         <v>8</v>
       </c>
-      <c r="AA41" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3335</v>
       </c>
@@ -3610,7 +3913,7 @@
         <v>3</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -3636,41 +3939,47 @@
       <c r="N42" t="s">
         <v>45</v>
       </c>
-      <c r="R42" t="s">
+      <c r="O42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P42" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T42" t="s">
         <v>39</v>
       </c>
-      <c r="S42" t="s">
-        <v>46</v>
-      </c>
-      <c r="T42" t="s">
-        <v>48</v>
-      </c>
       <c r="U42" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V42" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W42" t="s">
         <v>81</v>
       </c>
       <c r="X42" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y42" t="s">
         <v>80</v>
       </c>
       <c r="Z42" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB42" t="s">
         <v>8</v>
       </c>
-      <c r="AA42" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC42" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3337</v>
       </c>
@@ -3681,7 +3990,7 @@
         <v>3</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -3707,41 +4016,47 @@
       <c r="N43" t="s">
         <v>45</v>
       </c>
-      <c r="R43" t="s">
+      <c r="O43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T43" t="s">
         <v>39</v>
       </c>
-      <c r="S43" t="s">
-        <v>46</v>
-      </c>
-      <c r="T43" t="s">
-        <v>48</v>
-      </c>
       <c r="U43" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V43" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W43" t="s">
         <v>81</v>
       </c>
       <c r="X43" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y43" t="s">
         <v>80</v>
       </c>
       <c r="Z43" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB43" t="s">
         <v>8</v>
       </c>
-      <c r="AA43" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC43" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3338</v>
       </c>
@@ -3775,41 +4090,47 @@
       <c r="N44" t="s">
         <v>45</v>
       </c>
-      <c r="R44" t="s">
+      <c r="O44" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P44" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T44" t="s">
         <v>39</v>
       </c>
-      <c r="S44" t="s">
-        <v>46</v>
-      </c>
-      <c r="T44" t="s">
-        <v>48</v>
-      </c>
       <c r="U44" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V44" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W44" t="s">
         <v>81</v>
       </c>
       <c r="X44" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y44" t="s">
         <v>80</v>
       </c>
       <c r="Z44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB44" t="s">
         <v>8</v>
       </c>
-      <c r="AA44" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC44" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3339</v>
       </c>
@@ -3843,41 +4164,47 @@
       <c r="N45" t="s">
         <v>45</v>
       </c>
-      <c r="R45" t="s">
+      <c r="O45" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T45" t="s">
         <v>39</v>
       </c>
-      <c r="S45" t="s">
-        <v>46</v>
-      </c>
-      <c r="T45" t="s">
-        <v>48</v>
-      </c>
       <c r="U45" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V45" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W45" t="s">
         <v>81</v>
       </c>
       <c r="X45" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y45" t="s">
         <v>80</v>
       </c>
       <c r="Z45" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB45" t="s">
         <v>8</v>
       </c>
-      <c r="AA45" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC45" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3340</v>
       </c>
@@ -3911,41 +4238,47 @@
       <c r="N46" t="s">
         <v>45</v>
       </c>
-      <c r="R46" t="s">
+      <c r="O46" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T46" t="s">
         <v>39</v>
       </c>
-      <c r="S46" t="s">
-        <v>46</v>
-      </c>
-      <c r="T46" t="s">
-        <v>48</v>
-      </c>
       <c r="U46" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V46" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W46" t="s">
         <v>81</v>
       </c>
       <c r="X46" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y46" t="s">
         <v>80</v>
       </c>
       <c r="Z46" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB46" t="s">
         <v>8</v>
       </c>
-      <c r="AA46" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3341</v>
       </c>
@@ -3979,41 +4312,47 @@
       <c r="N47" t="s">
         <v>45</v>
       </c>
-      <c r="R47" t="s">
+      <c r="O47" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P47" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T47" t="s">
         <v>39</v>
       </c>
-      <c r="S47" t="s">
-        <v>46</v>
-      </c>
-      <c r="T47" t="s">
-        <v>48</v>
-      </c>
       <c r="U47" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V47" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W47" t="s">
         <v>81</v>
       </c>
       <c r="X47" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y47" t="s">
         <v>80</v>
       </c>
       <c r="Z47" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB47" t="s">
         <v>8</v>
       </c>
-      <c r="AA47" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC47" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3342</v>
       </c>
@@ -4047,41 +4386,47 @@
       <c r="N48" t="s">
         <v>45</v>
       </c>
-      <c r="R48" t="s">
+      <c r="O48" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T48" t="s">
         <v>39</v>
       </c>
-      <c r="S48" t="s">
-        <v>46</v>
-      </c>
-      <c r="T48" t="s">
-        <v>48</v>
-      </c>
       <c r="U48" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V48" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W48" t="s">
         <v>81</v>
       </c>
       <c r="X48" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y48" t="s">
         <v>80</v>
       </c>
       <c r="Z48" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB48" t="s">
         <v>8</v>
       </c>
-      <c r="AA48" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC48" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3343</v>
       </c>
@@ -4115,37 +4460,43 @@
       <c r="N49" t="s">
         <v>45</v>
       </c>
-      <c r="R49" t="s">
+      <c r="O49" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P49" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T49" t="s">
         <v>39</v>
       </c>
-      <c r="S49" t="s">
-        <v>46</v>
-      </c>
-      <c r="T49" t="s">
-        <v>48</v>
-      </c>
       <c r="U49" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="V49" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W49" t="s">
         <v>81</v>
       </c>
       <c r="X49" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Y49" t="s">
         <v>80</v>
       </c>
       <c r="Z49" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB49" t="s">
         <v>8</v>
       </c>
-      <c r="AA49" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB49" t="s">
+      <c r="AC49" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD49" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4156,17 +4507,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="89.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4181,7 +4532,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4230,7 +4581,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -4241,7 +4592,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -4252,18 +4603,18 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -4274,7 +4625,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -4285,7 +4636,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -4296,7 +4647,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -4307,7 +4658,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -4318,7 +4669,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -4329,7 +4680,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -4340,7 +4691,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -4351,165 +4702,187 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating path for ecotaca projects to raw/ecotaxa. Updating gitgnore and path in scripts
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDEF707-72B9-514B-9561-A5160E58A3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A5E6A-FFF3-C442-8243-AC273F201EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34820" yWindow="-700" windowWidth="30020" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="24200" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
     <t>Additoinal description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
   </si>
   <si>
-    <t>~/GIT/PSSdb/raw/API/IFCB</t>
+    <t>~/GIT/PSSdb/raw/ecotaxa/IFCB</t>
   </si>
 </sst>
 </file>
@@ -935,56 +935,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C47"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AM23" sqref="AM23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixing flag report bugs
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF900CC-D729-9648-B3DB-873CF0E81163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="166">
   <si>
     <t>Project_ID</t>
   </si>
@@ -363,84 +369,6 @@
   </si>
   <si>
     <t>object_annotation_status</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_2248_20220829_1556_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3147_20220829_1606_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3289_20220829_1608_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3290_20220829_1608_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3294_20220829_1610_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3295_20220829_1615_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3296_20220829_1615_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3297_20220829_1616_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3298_20220829_1705_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3313_20220829_1805_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3314_20220829_1808_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3315_20220609_1352_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3318_20220610_0723_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3320_20220829_1815_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3321_20220829_1816_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3322_20220829_1818_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3323_20220829_1818_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3324_20220829_1819_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3325_20220829_1821_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3337_20220829_1824_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3338_20220829_1824_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3339_20220829_1825_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3340_20220829_1825_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3341_20220829_1825_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3342_20220829_1825_flags.tsv</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/IFCB/ecotaxa_export_3343_20220829_1825_flags.tsv</t>
   </si>
   <si>
     <t>Variables</t>
@@ -596,8 +524,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +601,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -719,7 +655,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,9 +687,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -785,6 +739,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -960,14 +932,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AK47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1078,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -1192,11 +1166,8 @@
       <c r="AJ2" t="s">
         <v>115</v>
       </c>
-      <c r="AK2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45">
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -1284,11 +1255,8 @@
       <c r="AJ3" t="s">
         <v>115</v>
       </c>
-      <c r="AK3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45">
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1376,11 +1344,8 @@
       <c r="AJ4" t="s">
         <v>115</v>
       </c>
-      <c r="AK4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45">
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1468,11 +1433,8 @@
       <c r="AJ5" t="s">
         <v>115</v>
       </c>
-      <c r="AK5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45">
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -1560,11 +1522,8 @@
       <c r="AJ6" t="s">
         <v>115</v>
       </c>
-      <c r="AK6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45">
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -1652,11 +1611,8 @@
       <c r="AJ7" t="s">
         <v>115</v>
       </c>
-      <c r="AK7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45">
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -1744,11 +1700,8 @@
       <c r="AJ8" t="s">
         <v>115</v>
       </c>
-      <c r="AK8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45">
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -1836,11 +1789,8 @@
       <c r="AJ9" t="s">
         <v>115</v>
       </c>
-      <c r="AK9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45">
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -1928,11 +1878,8 @@
       <c r="AJ10" t="s">
         <v>115</v>
       </c>
-      <c r="AK10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45">
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -2021,7 +1968,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -2110,7 +2057,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -2199,7 +2146,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -2288,7 +2235,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -2377,7 +2324,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -2466,7 +2413,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2555,7 +2502,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -2644,7 +2591,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -2733,7 +2680,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -2822,7 +2769,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -2911,7 +2858,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3000,7 +2947,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3089,7 +3036,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3178,7 +3125,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3266,11 +3213,8 @@
       <c r="AJ25" t="s">
         <v>115</v>
       </c>
-      <c r="AK25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37">
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3358,11 +3302,8 @@
       <c r="AJ26" t="s">
         <v>115</v>
       </c>
-      <c r="AK26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:37">
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3450,11 +3391,8 @@
       <c r="AJ27" t="s">
         <v>115</v>
       </c>
-      <c r="AK27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:37">
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3542,11 +3480,8 @@
       <c r="AJ28" t="s">
         <v>115</v>
       </c>
-      <c r="AK28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:37">
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -3634,11 +3569,8 @@
       <c r="AJ29" t="s">
         <v>115</v>
       </c>
-      <c r="AK29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:37">
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -3726,11 +3658,8 @@
       <c r="AJ30" t="s">
         <v>115</v>
       </c>
-      <c r="AK30" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:37">
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -3818,11 +3747,8 @@
       <c r="AJ31" t="s">
         <v>115</v>
       </c>
-      <c r="AK31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:37">
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -3910,11 +3836,8 @@
       <c r="AJ32" t="s">
         <v>115</v>
       </c>
-      <c r="AK32" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" spans="1:37">
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4002,11 +3925,8 @@
       <c r="AJ33" t="s">
         <v>115</v>
       </c>
-      <c r="AK33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:37">
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4094,11 +4014,8 @@
       <c r="AJ34" t="s">
         <v>115</v>
       </c>
-      <c r="AK34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="1:37">
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4187,7 +4104,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4276,7 +4193,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4365,7 +4282,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4454,7 +4371,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4543,7 +4460,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -4632,7 +4549,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -4720,11 +4637,8 @@
       <c r="AJ41" t="s">
         <v>115</v>
       </c>
-      <c r="AK41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:37">
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -4812,11 +4726,8 @@
       <c r="AJ42" t="s">
         <v>115</v>
       </c>
-      <c r="AK42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:37">
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -4904,11 +4815,8 @@
       <c r="AJ43" t="s">
         <v>115</v>
       </c>
-      <c r="AK43" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:37">
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -4996,11 +4904,8 @@
       <c r="AJ44" t="s">
         <v>115</v>
       </c>
-      <c r="AK44" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:37">
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5088,11 +4993,8 @@
       <c r="AJ45" t="s">
         <v>115</v>
       </c>
-      <c r="AK45" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:37">
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5180,11 +5082,8 @@
       <c r="AJ46" t="s">
         <v>115</v>
       </c>
-      <c r="AK46" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:37">
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5272,575 +5171,572 @@
       <c r="AJ47" t="s">
         <v>115</v>
       </c>
-      <c r="AK47" t="s">
-        <v>141</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C23" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" t="s">
         <v>146</v>
       </c>
-      <c r="C27" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C38" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included the information to standardize the IFCB dashboard projects
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35B1412-2113-9548-A077-C7EE18E61E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453BCA87-3B91-434D-A7F9-C6469E7F59D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="25040" windowHeight="13820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="3780" windowWidth="25040" windowHeight="13820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="228">
   <si>
     <t>Project_ID</t>
   </si>
@@ -519,13 +519,199 @@
   </si>
   <si>
     <t>~/GIT/PSSdb/raw/ecotaxa/IFCB</t>
+  </si>
+  <si>
+    <t>SPIROPA</t>
+  </si>
+  <si>
+    <t>WHOI_dock</t>
+  </si>
+  <si>
+    <t>EXPORTS</t>
+  </si>
+  <si>
+    <t>NAAMES</t>
+  </si>
+  <si>
+    <t>NESLTER_transect</t>
+  </si>
+  <si>
+    <t>arctic</t>
+  </si>
+  <si>
+    <t>SIO_Delmar_mooring</t>
+  </si>
+  <si>
+    <t>NESLTER_broadscale</t>
+  </si>
+  <si>
+    <t>IFCB14_dock_WHOI</t>
+  </si>
+  <si>
+    <t>gsodock</t>
+  </si>
+  <si>
+    <t>fiddlers</t>
+  </si>
+  <si>
+    <t>OTZ_Atlantic</t>
+  </si>
+  <si>
+    <t>mvco</t>
+  </si>
+  <si>
+    <t>NBP2202</t>
+  </si>
+  <si>
+    <t>san-francisco-pier-17</t>
+  </si>
+  <si>
+    <t>santa-cruz-municipal-wharf</t>
+  </si>
+  <si>
+    <t>scripps-pier</t>
+  </si>
+  <si>
+    <t>mbari-power-buoy</t>
+  </si>
+  <si>
+    <t>newport-beach-pier</t>
+  </si>
+  <si>
+    <t>stearns-wharf</t>
+  </si>
+  <si>
+    <t>del-mar-mooring</t>
+  </si>
+  <si>
+    <t>bodega-marine-lab</t>
+  </si>
+  <si>
+    <t>cal-poly-humboldt-hioc</t>
+  </si>
+  <si>
+    <t>https://ifcb-data.whoi.edu</t>
+  </si>
+  <si>
+    <t>https://ifcb.caloos.org/</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/SPIROPA</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/WHOI_dock</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/EXPORTS</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/NAAMES</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/NESLTER_transect</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/arctic</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/SIO_Delmar_mooring</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/NESLTER_broadscale</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/IFCB14_dock_WHOI</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/gsodock</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/fiddlers</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/OTZ_Atlantic</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/mvco</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/NBP2202</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/san-francisco-pier-17</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/santa-cruz-municipal-wharf</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/scripps-pier</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/mbari-power-buoy</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/newport-beach-pier</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/stearns-wharf</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/del-mar-mooring</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/bodega-marine-lab</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/IFCB_dashboard_downloads/cal-poly-humboldt-hioc</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>vol_analyzed</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>roi_number</t>
+  </si>
+  <si>
+    <t>EquivDiameter</t>
+  </si>
+  <si>
+    <t>pixels</t>
+  </si>
+  <si>
+    <t>Biovolume</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>MinorAxisLength</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +732,19 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -588,12 +787,18 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -933,17 +1138,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS47"/>
+  <dimension ref="A1:AS70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE32" workbookViewId="0">
-      <selection activeCell="AK47" sqref="AK2:AK47"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -5216,6 +5421,2260 @@
       </c>
       <c r="AJ47" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+      <c r="H48" t="s">
+        <v>93</v>
+      </c>
+      <c r="I48" t="s">
+        <v>214</v>
+      </c>
+      <c r="J48" t="s">
+        <v>95</v>
+      </c>
+      <c r="K48" t="s">
+        <v>215</v>
+      </c>
+      <c r="L48" t="s">
+        <v>95</v>
+      </c>
+      <c r="M48" t="s">
+        <v>216</v>
+      </c>
+      <c r="N48" t="s">
+        <v>98</v>
+      </c>
+      <c r="O48" t="s">
+        <v>216</v>
+      </c>
+      <c r="P48" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>226</v>
+      </c>
+      <c r="R48" t="s">
+        <v>101</v>
+      </c>
+      <c r="S48" t="s">
+        <v>227</v>
+      </c>
+      <c r="T48" t="s">
+        <v>103</v>
+      </c>
+      <c r="U48" t="s">
+        <v>217</v>
+      </c>
+      <c r="V48" t="s">
+        <v>218</v>
+      </c>
+      <c r="X48" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y48" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE48" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH48" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" t="s">
+        <v>192</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" t="s">
+        <v>92</v>
+      </c>
+      <c r="H49" t="s">
+        <v>93</v>
+      </c>
+      <c r="I49" t="s">
+        <v>214</v>
+      </c>
+      <c r="J49" t="s">
+        <v>95</v>
+      </c>
+      <c r="K49" t="s">
+        <v>215</v>
+      </c>
+      <c r="L49" t="s">
+        <v>95</v>
+      </c>
+      <c r="M49" t="s">
+        <v>216</v>
+      </c>
+      <c r="N49" t="s">
+        <v>98</v>
+      </c>
+      <c r="O49" t="s">
+        <v>216</v>
+      </c>
+      <c r="P49" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>226</v>
+      </c>
+      <c r="R49" t="s">
+        <v>101</v>
+      </c>
+      <c r="S49" t="s">
+        <v>227</v>
+      </c>
+      <c r="T49" t="s">
+        <v>103</v>
+      </c>
+      <c r="U49" t="s">
+        <v>217</v>
+      </c>
+      <c r="V49" t="s">
+        <v>218</v>
+      </c>
+      <c r="X49" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y49" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE49" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH49" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" t="s">
+        <v>193</v>
+      </c>
+      <c r="D50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" t="s">
+        <v>93</v>
+      </c>
+      <c r="I50" t="s">
+        <v>214</v>
+      </c>
+      <c r="J50" t="s">
+        <v>95</v>
+      </c>
+      <c r="K50" t="s">
+        <v>215</v>
+      </c>
+      <c r="L50" t="s">
+        <v>95</v>
+      </c>
+      <c r="M50" t="s">
+        <v>216</v>
+      </c>
+      <c r="N50" t="s">
+        <v>98</v>
+      </c>
+      <c r="O50" t="s">
+        <v>216</v>
+      </c>
+      <c r="P50" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>226</v>
+      </c>
+      <c r="R50" t="s">
+        <v>101</v>
+      </c>
+      <c r="S50" t="s">
+        <v>227</v>
+      </c>
+      <c r="T50" t="s">
+        <v>103</v>
+      </c>
+      <c r="U50" t="s">
+        <v>217</v>
+      </c>
+      <c r="V50" t="s">
+        <v>218</v>
+      </c>
+      <c r="X50" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y50" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE50" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH50" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" t="s">
+        <v>194</v>
+      </c>
+      <c r="D51" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+      <c r="H51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I51" t="s">
+        <v>214</v>
+      </c>
+      <c r="J51" t="s">
+        <v>95</v>
+      </c>
+      <c r="K51" t="s">
+        <v>215</v>
+      </c>
+      <c r="L51" t="s">
+        <v>95</v>
+      </c>
+      <c r="M51" t="s">
+        <v>216</v>
+      </c>
+      <c r="N51" t="s">
+        <v>98</v>
+      </c>
+      <c r="O51" t="s">
+        <v>216</v>
+      </c>
+      <c r="P51" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>226</v>
+      </c>
+      <c r="R51" t="s">
+        <v>101</v>
+      </c>
+      <c r="S51" t="s">
+        <v>227</v>
+      </c>
+      <c r="T51" t="s">
+        <v>103</v>
+      </c>
+      <c r="U51" t="s">
+        <v>217</v>
+      </c>
+      <c r="V51" t="s">
+        <v>218</v>
+      </c>
+      <c r="X51" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y51" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE51" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" t="s">
+        <v>195</v>
+      </c>
+      <c r="D52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" t="s">
+        <v>214</v>
+      </c>
+      <c r="J52" t="s">
+        <v>95</v>
+      </c>
+      <c r="K52" t="s">
+        <v>215</v>
+      </c>
+      <c r="L52" t="s">
+        <v>95</v>
+      </c>
+      <c r="M52" t="s">
+        <v>216</v>
+      </c>
+      <c r="N52" t="s">
+        <v>98</v>
+      </c>
+      <c r="O52" t="s">
+        <v>216</v>
+      </c>
+      <c r="P52" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>226</v>
+      </c>
+      <c r="R52" t="s">
+        <v>101</v>
+      </c>
+      <c r="S52" t="s">
+        <v>227</v>
+      </c>
+      <c r="T52" t="s">
+        <v>103</v>
+      </c>
+      <c r="U52" t="s">
+        <v>217</v>
+      </c>
+      <c r="V52" t="s">
+        <v>218</v>
+      </c>
+      <c r="X52" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y52" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE52" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH52" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" t="s">
+        <v>93</v>
+      </c>
+      <c r="I53" t="s">
+        <v>214</v>
+      </c>
+      <c r="J53" t="s">
+        <v>95</v>
+      </c>
+      <c r="K53" t="s">
+        <v>215</v>
+      </c>
+      <c r="L53" t="s">
+        <v>95</v>
+      </c>
+      <c r="M53" t="s">
+        <v>216</v>
+      </c>
+      <c r="N53" t="s">
+        <v>98</v>
+      </c>
+      <c r="O53" t="s">
+        <v>216</v>
+      </c>
+      <c r="P53" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>226</v>
+      </c>
+      <c r="R53" t="s">
+        <v>101</v>
+      </c>
+      <c r="S53" t="s">
+        <v>227</v>
+      </c>
+      <c r="T53" t="s">
+        <v>103</v>
+      </c>
+      <c r="U53" t="s">
+        <v>217</v>
+      </c>
+      <c r="V53" t="s">
+        <v>218</v>
+      </c>
+      <c r="X53" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y53" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE53" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" t="s">
+        <v>197</v>
+      </c>
+      <c r="D54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+      <c r="H54" t="s">
+        <v>93</v>
+      </c>
+      <c r="I54" t="s">
+        <v>214</v>
+      </c>
+      <c r="J54" t="s">
+        <v>95</v>
+      </c>
+      <c r="K54" t="s">
+        <v>215</v>
+      </c>
+      <c r="L54" t="s">
+        <v>95</v>
+      </c>
+      <c r="M54" t="s">
+        <v>216</v>
+      </c>
+      <c r="N54" t="s">
+        <v>98</v>
+      </c>
+      <c r="O54" t="s">
+        <v>216</v>
+      </c>
+      <c r="P54" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>226</v>
+      </c>
+      <c r="R54" t="s">
+        <v>101</v>
+      </c>
+      <c r="S54" t="s">
+        <v>227</v>
+      </c>
+      <c r="T54" t="s">
+        <v>103</v>
+      </c>
+      <c r="U54" t="s">
+        <v>217</v>
+      </c>
+      <c r="V54" t="s">
+        <v>218</v>
+      </c>
+      <c r="X54" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y54" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE54" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH54" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" t="s">
+        <v>198</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55" t="s">
+        <v>93</v>
+      </c>
+      <c r="I55" t="s">
+        <v>214</v>
+      </c>
+      <c r="J55" t="s">
+        <v>95</v>
+      </c>
+      <c r="K55" t="s">
+        <v>215</v>
+      </c>
+      <c r="L55" t="s">
+        <v>95</v>
+      </c>
+      <c r="M55" t="s">
+        <v>216</v>
+      </c>
+      <c r="N55" t="s">
+        <v>98</v>
+      </c>
+      <c r="O55" t="s">
+        <v>216</v>
+      </c>
+      <c r="P55" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>226</v>
+      </c>
+      <c r="R55" t="s">
+        <v>101</v>
+      </c>
+      <c r="S55" t="s">
+        <v>227</v>
+      </c>
+      <c r="T55" t="s">
+        <v>103</v>
+      </c>
+      <c r="U55" t="s">
+        <v>217</v>
+      </c>
+      <c r="V55" t="s">
+        <v>218</v>
+      </c>
+      <c r="X55" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y55" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE55" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH55" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+      <c r="H56" t="s">
+        <v>93</v>
+      </c>
+      <c r="I56" t="s">
+        <v>214</v>
+      </c>
+      <c r="J56" t="s">
+        <v>95</v>
+      </c>
+      <c r="K56" t="s">
+        <v>215</v>
+      </c>
+      <c r="L56" t="s">
+        <v>95</v>
+      </c>
+      <c r="M56" t="s">
+        <v>216</v>
+      </c>
+      <c r="N56" t="s">
+        <v>98</v>
+      </c>
+      <c r="O56" t="s">
+        <v>216</v>
+      </c>
+      <c r="P56" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>226</v>
+      </c>
+      <c r="R56" t="s">
+        <v>101</v>
+      </c>
+      <c r="S56" t="s">
+        <v>227</v>
+      </c>
+      <c r="T56" t="s">
+        <v>103</v>
+      </c>
+      <c r="U56" t="s">
+        <v>217</v>
+      </c>
+      <c r="V56" t="s">
+        <v>218</v>
+      </c>
+      <c r="X56" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y56" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE56" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF56" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH56" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C57" t="s">
+        <v>200</v>
+      </c>
+      <c r="D57" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" t="s">
+        <v>92</v>
+      </c>
+      <c r="H57" t="s">
+        <v>93</v>
+      </c>
+      <c r="I57" t="s">
+        <v>214</v>
+      </c>
+      <c r="J57" t="s">
+        <v>95</v>
+      </c>
+      <c r="K57" t="s">
+        <v>215</v>
+      </c>
+      <c r="L57" t="s">
+        <v>95</v>
+      </c>
+      <c r="M57" t="s">
+        <v>216</v>
+      </c>
+      <c r="N57" t="s">
+        <v>98</v>
+      </c>
+      <c r="O57" t="s">
+        <v>216</v>
+      </c>
+      <c r="P57" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>226</v>
+      </c>
+      <c r="R57" t="s">
+        <v>101</v>
+      </c>
+      <c r="S57" t="s">
+        <v>227</v>
+      </c>
+      <c r="T57" t="s">
+        <v>103</v>
+      </c>
+      <c r="U57" t="s">
+        <v>217</v>
+      </c>
+      <c r="V57" t="s">
+        <v>218</v>
+      </c>
+      <c r="X57" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y57" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE57" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" t="s">
+        <v>201</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+      <c r="H58" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" t="s">
+        <v>214</v>
+      </c>
+      <c r="J58" t="s">
+        <v>95</v>
+      </c>
+      <c r="K58" t="s">
+        <v>215</v>
+      </c>
+      <c r="L58" t="s">
+        <v>95</v>
+      </c>
+      <c r="M58" t="s">
+        <v>216</v>
+      </c>
+      <c r="N58" t="s">
+        <v>98</v>
+      </c>
+      <c r="O58" t="s">
+        <v>216</v>
+      </c>
+      <c r="P58" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>226</v>
+      </c>
+      <c r="R58" t="s">
+        <v>101</v>
+      </c>
+      <c r="S58" t="s">
+        <v>227</v>
+      </c>
+      <c r="T58" t="s">
+        <v>103</v>
+      </c>
+      <c r="U58" t="s">
+        <v>217</v>
+      </c>
+      <c r="V58" t="s">
+        <v>218</v>
+      </c>
+      <c r="X58" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y58" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE58" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG58" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH58" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" t="s">
+        <v>92</v>
+      </c>
+      <c r="H59" t="s">
+        <v>93</v>
+      </c>
+      <c r="I59" t="s">
+        <v>214</v>
+      </c>
+      <c r="J59" t="s">
+        <v>95</v>
+      </c>
+      <c r="K59" t="s">
+        <v>215</v>
+      </c>
+      <c r="L59" t="s">
+        <v>95</v>
+      </c>
+      <c r="M59" t="s">
+        <v>216</v>
+      </c>
+      <c r="N59" t="s">
+        <v>98</v>
+      </c>
+      <c r="O59" t="s">
+        <v>216</v>
+      </c>
+      <c r="P59" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>226</v>
+      </c>
+      <c r="R59" t="s">
+        <v>101</v>
+      </c>
+      <c r="S59" t="s">
+        <v>227</v>
+      </c>
+      <c r="T59" t="s">
+        <v>103</v>
+      </c>
+      <c r="U59" t="s">
+        <v>217</v>
+      </c>
+      <c r="V59" t="s">
+        <v>218</v>
+      </c>
+      <c r="X59" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y59" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE59" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH59" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI59" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" t="s">
+        <v>203</v>
+      </c>
+      <c r="D60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" t="s">
+        <v>93</v>
+      </c>
+      <c r="I60" t="s">
+        <v>214</v>
+      </c>
+      <c r="J60" t="s">
+        <v>95</v>
+      </c>
+      <c r="K60" t="s">
+        <v>215</v>
+      </c>
+      <c r="L60" t="s">
+        <v>95</v>
+      </c>
+      <c r="M60" t="s">
+        <v>216</v>
+      </c>
+      <c r="N60" t="s">
+        <v>98</v>
+      </c>
+      <c r="O60" t="s">
+        <v>216</v>
+      </c>
+      <c r="P60" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>226</v>
+      </c>
+      <c r="R60" t="s">
+        <v>101</v>
+      </c>
+      <c r="S60" t="s">
+        <v>227</v>
+      </c>
+      <c r="T60" t="s">
+        <v>103</v>
+      </c>
+      <c r="U60" t="s">
+        <v>217</v>
+      </c>
+      <c r="V60" t="s">
+        <v>218</v>
+      </c>
+      <c r="X60" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y60" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE60" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG60" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH60" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI60" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" t="s">
+        <v>204</v>
+      </c>
+      <c r="D61" t="s">
+        <v>91</v>
+      </c>
+      <c r="E61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H61" t="s">
+        <v>93</v>
+      </c>
+      <c r="I61" t="s">
+        <v>214</v>
+      </c>
+      <c r="J61" t="s">
+        <v>95</v>
+      </c>
+      <c r="K61" t="s">
+        <v>215</v>
+      </c>
+      <c r="L61" t="s">
+        <v>95</v>
+      </c>
+      <c r="M61" t="s">
+        <v>216</v>
+      </c>
+      <c r="N61" t="s">
+        <v>98</v>
+      </c>
+      <c r="O61" t="s">
+        <v>216</v>
+      </c>
+      <c r="P61" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>226</v>
+      </c>
+      <c r="R61" t="s">
+        <v>101</v>
+      </c>
+      <c r="S61" t="s">
+        <v>227</v>
+      </c>
+      <c r="T61" t="s">
+        <v>103</v>
+      </c>
+      <c r="U61" t="s">
+        <v>217</v>
+      </c>
+      <c r="V61" t="s">
+        <v>218</v>
+      </c>
+      <c r="X61" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y61" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE61" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG61" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH61" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI61" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62" t="s">
+        <v>93</v>
+      </c>
+      <c r="I62" t="s">
+        <v>214</v>
+      </c>
+      <c r="J62" t="s">
+        <v>95</v>
+      </c>
+      <c r="K62" t="s">
+        <v>215</v>
+      </c>
+      <c r="L62" t="s">
+        <v>95</v>
+      </c>
+      <c r="M62" t="s">
+        <v>216</v>
+      </c>
+      <c r="N62" t="s">
+        <v>98</v>
+      </c>
+      <c r="O62" t="s">
+        <v>216</v>
+      </c>
+      <c r="P62" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>226</v>
+      </c>
+      <c r="R62" t="s">
+        <v>101</v>
+      </c>
+      <c r="S62" t="s">
+        <v>227</v>
+      </c>
+      <c r="T62" t="s">
+        <v>103</v>
+      </c>
+      <c r="U62" t="s">
+        <v>217</v>
+      </c>
+      <c r="V62" t="s">
+        <v>218</v>
+      </c>
+      <c r="X62" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y62" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE62" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF62" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG62" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH62" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI62" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
+        <v>206</v>
+      </c>
+      <c r="D63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" t="s">
+        <v>92</v>
+      </c>
+      <c r="H63" t="s">
+        <v>93</v>
+      </c>
+      <c r="I63" t="s">
+        <v>214</v>
+      </c>
+      <c r="J63" t="s">
+        <v>95</v>
+      </c>
+      <c r="K63" t="s">
+        <v>215</v>
+      </c>
+      <c r="L63" t="s">
+        <v>95</v>
+      </c>
+      <c r="M63" t="s">
+        <v>216</v>
+      </c>
+      <c r="N63" t="s">
+        <v>98</v>
+      </c>
+      <c r="O63" t="s">
+        <v>216</v>
+      </c>
+      <c r="P63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>226</v>
+      </c>
+      <c r="R63" t="s">
+        <v>101</v>
+      </c>
+      <c r="S63" t="s">
+        <v>227</v>
+      </c>
+      <c r="T63" t="s">
+        <v>103</v>
+      </c>
+      <c r="U63" t="s">
+        <v>217</v>
+      </c>
+      <c r="V63" t="s">
+        <v>218</v>
+      </c>
+      <c r="X63" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y63" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE63" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H64" t="s">
+        <v>93</v>
+      </c>
+      <c r="I64" t="s">
+        <v>214</v>
+      </c>
+      <c r="J64" t="s">
+        <v>95</v>
+      </c>
+      <c r="K64" t="s">
+        <v>215</v>
+      </c>
+      <c r="L64" t="s">
+        <v>95</v>
+      </c>
+      <c r="M64" t="s">
+        <v>216</v>
+      </c>
+      <c r="N64" t="s">
+        <v>98</v>
+      </c>
+      <c r="O64" t="s">
+        <v>216</v>
+      </c>
+      <c r="P64" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>226</v>
+      </c>
+      <c r="R64" t="s">
+        <v>101</v>
+      </c>
+      <c r="S64" t="s">
+        <v>227</v>
+      </c>
+      <c r="T64" t="s">
+        <v>103</v>
+      </c>
+      <c r="U64" t="s">
+        <v>217</v>
+      </c>
+      <c r="V64" t="s">
+        <v>218</v>
+      </c>
+      <c r="X64" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y64" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD64" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE64" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF64" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG64" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH64" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI64" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" t="s">
+        <v>208</v>
+      </c>
+      <c r="D65" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
+      </c>
+      <c r="H65" t="s">
+        <v>93</v>
+      </c>
+      <c r="I65" t="s">
+        <v>214</v>
+      </c>
+      <c r="J65" t="s">
+        <v>95</v>
+      </c>
+      <c r="K65" t="s">
+        <v>215</v>
+      </c>
+      <c r="L65" t="s">
+        <v>95</v>
+      </c>
+      <c r="M65" t="s">
+        <v>216</v>
+      </c>
+      <c r="N65" t="s">
+        <v>98</v>
+      </c>
+      <c r="O65" t="s">
+        <v>216</v>
+      </c>
+      <c r="P65" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>226</v>
+      </c>
+      <c r="R65" t="s">
+        <v>101</v>
+      </c>
+      <c r="S65" t="s">
+        <v>227</v>
+      </c>
+      <c r="T65" t="s">
+        <v>103</v>
+      </c>
+      <c r="U65" t="s">
+        <v>217</v>
+      </c>
+      <c r="V65" t="s">
+        <v>218</v>
+      </c>
+      <c r="X65" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y65" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD65" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE65" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG65" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH65" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" t="s">
+        <v>209</v>
+      </c>
+      <c r="D66" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" t="s">
+        <v>92</v>
+      </c>
+      <c r="H66" t="s">
+        <v>93</v>
+      </c>
+      <c r="I66" t="s">
+        <v>214</v>
+      </c>
+      <c r="J66" t="s">
+        <v>95</v>
+      </c>
+      <c r="K66" t="s">
+        <v>215</v>
+      </c>
+      <c r="L66" t="s">
+        <v>95</v>
+      </c>
+      <c r="M66" t="s">
+        <v>216</v>
+      </c>
+      <c r="N66" t="s">
+        <v>98</v>
+      </c>
+      <c r="O66" t="s">
+        <v>216</v>
+      </c>
+      <c r="P66" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>226</v>
+      </c>
+      <c r="R66" t="s">
+        <v>101</v>
+      </c>
+      <c r="S66" t="s">
+        <v>227</v>
+      </c>
+      <c r="T66" t="s">
+        <v>103</v>
+      </c>
+      <c r="U66" t="s">
+        <v>217</v>
+      </c>
+      <c r="V66" t="s">
+        <v>218</v>
+      </c>
+      <c r="X66" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y66" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD66" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE66" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH66" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI66" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>185</v>
+      </c>
+      <c r="B67" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D67" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" t="s">
+        <v>93</v>
+      </c>
+      <c r="I67" t="s">
+        <v>214</v>
+      </c>
+      <c r="J67" t="s">
+        <v>95</v>
+      </c>
+      <c r="K67" t="s">
+        <v>215</v>
+      </c>
+      <c r="L67" t="s">
+        <v>95</v>
+      </c>
+      <c r="M67" t="s">
+        <v>216</v>
+      </c>
+      <c r="N67" t="s">
+        <v>98</v>
+      </c>
+      <c r="O67" t="s">
+        <v>216</v>
+      </c>
+      <c r="P67" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>226</v>
+      </c>
+      <c r="R67" t="s">
+        <v>101</v>
+      </c>
+      <c r="S67" t="s">
+        <v>227</v>
+      </c>
+      <c r="T67" t="s">
+        <v>103</v>
+      </c>
+      <c r="U67" t="s">
+        <v>217</v>
+      </c>
+      <c r="V67" t="s">
+        <v>218</v>
+      </c>
+      <c r="X67" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y67" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE67" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>186</v>
+      </c>
+      <c r="B68" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" t="s">
+        <v>92</v>
+      </c>
+      <c r="H68" t="s">
+        <v>93</v>
+      </c>
+      <c r="I68" t="s">
+        <v>214</v>
+      </c>
+      <c r="J68" t="s">
+        <v>95</v>
+      </c>
+      <c r="K68" t="s">
+        <v>215</v>
+      </c>
+      <c r="L68" t="s">
+        <v>95</v>
+      </c>
+      <c r="M68" t="s">
+        <v>216</v>
+      </c>
+      <c r="N68" t="s">
+        <v>98</v>
+      </c>
+      <c r="O68" t="s">
+        <v>216</v>
+      </c>
+      <c r="P68" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>226</v>
+      </c>
+      <c r="R68" t="s">
+        <v>101</v>
+      </c>
+      <c r="S68" t="s">
+        <v>227</v>
+      </c>
+      <c r="T68" t="s">
+        <v>103</v>
+      </c>
+      <c r="U68" t="s">
+        <v>217</v>
+      </c>
+      <c r="V68" t="s">
+        <v>218</v>
+      </c>
+      <c r="X68" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y68" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE68" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG68" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH68" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI68" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>187</v>
+      </c>
+      <c r="B69" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" t="s">
+        <v>212</v>
+      </c>
+      <c r="D69" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" t="s">
+        <v>93</v>
+      </c>
+      <c r="I69" t="s">
+        <v>214</v>
+      </c>
+      <c r="J69" t="s">
+        <v>95</v>
+      </c>
+      <c r="K69" t="s">
+        <v>215</v>
+      </c>
+      <c r="L69" t="s">
+        <v>95</v>
+      </c>
+      <c r="M69" t="s">
+        <v>216</v>
+      </c>
+      <c r="N69" t="s">
+        <v>98</v>
+      </c>
+      <c r="O69" t="s">
+        <v>216</v>
+      </c>
+      <c r="P69" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>226</v>
+      </c>
+      <c r="R69" t="s">
+        <v>101</v>
+      </c>
+      <c r="S69" t="s">
+        <v>227</v>
+      </c>
+      <c r="T69" t="s">
+        <v>103</v>
+      </c>
+      <c r="U69" t="s">
+        <v>217</v>
+      </c>
+      <c r="V69" t="s">
+        <v>218</v>
+      </c>
+      <c r="X69" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y69" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE69" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG69" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH69" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI69" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L70" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="M70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="N70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="P70" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q70" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="R70" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="S70" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="T70" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="U70" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="V70" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="X70" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y70" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z70" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA70" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB70" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC70" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD70" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE70" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF70" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG70" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH70" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI70" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -5269,6 +7728,8 @@
     <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
     <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{815F655D-2B61-C943-8EE4-8EF7E5CA0661}"/>
+    <hyperlink ref="B49:B61" r:id="rId48" display="https://ifcb-data.whoi.edu" xr:uid="{774C7D73-E849-6C4D-AEE5-D15B86527BD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5278,7 +7739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
updated metadata information for IFCB dashboard projects
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990A21DB-71FB-E845-94EF-05E266D8F2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="7280" yWindow="1340" windowWidth="28340" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="254">
   <si>
     <t>Project_ID</t>
   </si>
@@ -623,9 +629,6 @@
     <t>object_annotation_category</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>object_annotation_status</t>
   </si>
   <si>
@@ -777,13 +780,16 @@
   </si>
   <si>
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
+  </si>
+  <si>
+    <t>class_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -859,6 +865,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -905,7 +919,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -937,9 +951,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -971,6 +1003,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1146,14 +1196,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1345,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -1376,10 +1431,10 @@
         <v>201</v>
       </c>
       <c r="AJ2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -1465,10 +1520,10 @@
         <v>201</v>
       </c>
       <c r="AJ3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1554,10 +1609,10 @@
         <v>201</v>
       </c>
       <c r="AJ4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1643,10 +1698,10 @@
         <v>201</v>
       </c>
       <c r="AJ5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -1732,10 +1787,10 @@
         <v>201</v>
       </c>
       <c r="AJ6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -1821,10 +1876,10 @@
         <v>201</v>
       </c>
       <c r="AJ7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -1910,10 +1965,10 @@
         <v>201</v>
       </c>
       <c r="AJ8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -1999,10 +2054,10 @@
         <v>201</v>
       </c>
       <c r="AJ9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -2088,10 +2143,10 @@
         <v>201</v>
       </c>
       <c r="AJ10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -2177,10 +2232,10 @@
         <v>201</v>
       </c>
       <c r="AJ11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -2266,10 +2321,10 @@
         <v>201</v>
       </c>
       <c r="AJ12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -2355,10 +2410,10 @@
         <v>201</v>
       </c>
       <c r="AJ13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -2444,10 +2499,10 @@
         <v>201</v>
       </c>
       <c r="AJ14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -2533,10 +2588,10 @@
         <v>201</v>
       </c>
       <c r="AJ15" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -2622,10 +2677,10 @@
         <v>201</v>
       </c>
       <c r="AJ16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2711,10 +2766,10 @@
         <v>201</v>
       </c>
       <c r="AJ17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -2800,10 +2855,10 @@
         <v>201</v>
       </c>
       <c r="AJ18" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -2889,10 +2944,10 @@
         <v>201</v>
       </c>
       <c r="AJ19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -2978,10 +3033,10 @@
         <v>201</v>
       </c>
       <c r="AJ20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -3067,10 +3122,10 @@
         <v>201</v>
       </c>
       <c r="AJ21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3156,10 +3211,10 @@
         <v>201</v>
       </c>
       <c r="AJ22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3245,10 +3300,10 @@
         <v>201</v>
       </c>
       <c r="AJ23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3334,10 +3389,10 @@
         <v>201</v>
       </c>
       <c r="AJ24" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3423,10 +3478,10 @@
         <v>201</v>
       </c>
       <c r="AJ25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3512,10 +3567,10 @@
         <v>201</v>
       </c>
       <c r="AJ26" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="27" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3601,10 +3656,10 @@
         <v>201</v>
       </c>
       <c r="AJ27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3690,10 +3745,10 @@
         <v>201</v>
       </c>
       <c r="AJ28" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -3779,10 +3834,10 @@
         <v>201</v>
       </c>
       <c r="AJ29" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -3868,10 +3923,10 @@
         <v>201</v>
       </c>
       <c r="AJ30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -3957,10 +4012,10 @@
         <v>201</v>
       </c>
       <c r="AJ31" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -4046,10 +4101,10 @@
         <v>201</v>
       </c>
       <c r="AJ32" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="33" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4135,10 +4190,10 @@
         <v>201</v>
       </c>
       <c r="AJ33" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4224,10 +4279,10 @@
         <v>201</v>
       </c>
       <c r="AJ34" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="35" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4313,10 +4368,10 @@
         <v>201</v>
       </c>
       <c r="AJ35" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4402,10 +4457,10 @@
         <v>201</v>
       </c>
       <c r="AJ36" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="37" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4491,10 +4546,10 @@
         <v>201</v>
       </c>
       <c r="AJ37" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="38" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4580,10 +4635,10 @@
         <v>201</v>
       </c>
       <c r="AJ38" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4669,10 +4724,10 @@
         <v>201</v>
       </c>
       <c r="AJ39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -4758,10 +4813,10 @@
         <v>201</v>
       </c>
       <c r="AJ40" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -4847,10 +4902,10 @@
         <v>201</v>
       </c>
       <c r="AJ41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -4936,10 +4991,10 @@
         <v>201</v>
       </c>
       <c r="AJ42" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -5025,10 +5080,10 @@
         <v>201</v>
       </c>
       <c r="AJ43" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="44" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -5114,10 +5169,10 @@
         <v>201</v>
       </c>
       <c r="AJ44" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5203,10 +5258,10 @@
         <v>201</v>
       </c>
       <c r="AJ45" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="46" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5292,10 +5347,10 @@
         <v>201</v>
       </c>
       <c r="AJ46" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="47" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5381,10 +5436,10 @@
         <v>201</v>
       </c>
       <c r="AJ47" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="48" spans="1:36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -5479,10 +5534,10 @@
         <v>200</v>
       </c>
       <c r="AI48" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5577,10 +5632,10 @@
         <v>200</v>
       </c>
       <c r="AI49" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="50" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -5675,10 +5730,10 @@
         <v>200</v>
       </c>
       <c r="AI50" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="51" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -5773,10 +5828,10 @@
         <v>200</v>
       </c>
       <c r="AI51" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="52" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -5871,10 +5926,10 @@
         <v>200</v>
       </c>
       <c r="AI52" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="53" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -5969,10 +6024,10 @@
         <v>200</v>
       </c>
       <c r="AI53" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="54" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -6067,10 +6122,10 @@
         <v>200</v>
       </c>
       <c r="AI54" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -6165,10 +6220,10 @@
         <v>200</v>
       </c>
       <c r="AI55" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="56" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -6263,10 +6318,10 @@
         <v>200</v>
       </c>
       <c r="AI56" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="57" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -6361,10 +6416,10 @@
         <v>200</v>
       </c>
       <c r="AI57" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="58" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -6459,10 +6514,10 @@
         <v>200</v>
       </c>
       <c r="AI58" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="59" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -6557,10 +6612,10 @@
         <v>200</v>
       </c>
       <c r="AI59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -6655,10 +6710,10 @@
         <v>200</v>
       </c>
       <c r="AI60" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -6753,10 +6808,10 @@
         <v>200</v>
       </c>
       <c r="AI61" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="62" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -6851,10 +6906,10 @@
         <v>200</v>
       </c>
       <c r="AI62" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -6949,10 +7004,10 @@
         <v>200</v>
       </c>
       <c r="AI63" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="64" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -7047,10 +7102,10 @@
         <v>200</v>
       </c>
       <c r="AI64" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -7145,10 +7200,10 @@
         <v>200</v>
       </c>
       <c r="AI65" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="66" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -7243,10 +7298,10 @@
         <v>200</v>
       </c>
       <c r="AI66" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="67" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -7341,10 +7396,10 @@
         <v>200</v>
       </c>
       <c r="AI67" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="68" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -7439,10 +7494,10 @@
         <v>200</v>
       </c>
       <c r="AI68" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="69" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -7537,10 +7592,10 @@
         <v>200</v>
       </c>
       <c r="AI69" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="70" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -7635,10 +7690,10 @@
         <v>200</v>
       </c>
       <c r="AI70" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="71" spans="1:35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="71" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -7651,8 +7706,92 @@
       <c r="D71" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="72" spans="1:35">
+      <c r="E71" t="s">
+        <v>166</v>
+      </c>
+      <c r="H71" t="s">
+        <v>167</v>
+      </c>
+      <c r="I71" t="s">
+        <v>169</v>
+      </c>
+      <c r="J71" t="s">
+        <v>170</v>
+      </c>
+      <c r="K71" t="s">
+        <v>172</v>
+      </c>
+      <c r="L71" t="s">
+        <v>170</v>
+      </c>
+      <c r="M71" t="s">
+        <v>174</v>
+      </c>
+      <c r="N71" t="s">
+        <v>175</v>
+      </c>
+      <c r="O71" t="s">
+        <v>174</v>
+      </c>
+      <c r="P71" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>178</v>
+      </c>
+      <c r="R71" t="s">
+        <v>180</v>
+      </c>
+      <c r="S71" t="s">
+        <v>178</v>
+      </c>
+      <c r="T71" t="s">
+        <v>180</v>
+      </c>
+      <c r="U71" t="s">
+        <v>183</v>
+      </c>
+      <c r="V71" t="s">
+        <v>184</v>
+      </c>
+      <c r="X71" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA71" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG71" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH71" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI71" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="72" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -7665,8 +7804,92 @@
       <c r="D72" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="73" spans="1:35">
+      <c r="E72" t="s">
+        <v>166</v>
+      </c>
+      <c r="H72" t="s">
+        <v>167</v>
+      </c>
+      <c r="I72" t="s">
+        <v>169</v>
+      </c>
+      <c r="J72" t="s">
+        <v>170</v>
+      </c>
+      <c r="K72" t="s">
+        <v>172</v>
+      </c>
+      <c r="L72" t="s">
+        <v>170</v>
+      </c>
+      <c r="M72" t="s">
+        <v>174</v>
+      </c>
+      <c r="N72" t="s">
+        <v>175</v>
+      </c>
+      <c r="O72" t="s">
+        <v>174</v>
+      </c>
+      <c r="P72" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>178</v>
+      </c>
+      <c r="R72" t="s">
+        <v>180</v>
+      </c>
+      <c r="S72" t="s">
+        <v>178</v>
+      </c>
+      <c r="T72" t="s">
+        <v>180</v>
+      </c>
+      <c r="U72" t="s">
+        <v>183</v>
+      </c>
+      <c r="V72" t="s">
+        <v>184</v>
+      </c>
+      <c r="X72" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA72" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF72" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG72" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH72" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI72" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="73" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -7679,8 +7902,92 @@
       <c r="D73" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="74" spans="1:35">
+      <c r="E73" t="s">
+        <v>166</v>
+      </c>
+      <c r="H73" t="s">
+        <v>167</v>
+      </c>
+      <c r="I73" t="s">
+        <v>169</v>
+      </c>
+      <c r="J73" t="s">
+        <v>170</v>
+      </c>
+      <c r="K73" t="s">
+        <v>172</v>
+      </c>
+      <c r="L73" t="s">
+        <v>170</v>
+      </c>
+      <c r="M73" t="s">
+        <v>174</v>
+      </c>
+      <c r="N73" t="s">
+        <v>175</v>
+      </c>
+      <c r="O73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P73" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>178</v>
+      </c>
+      <c r="R73" t="s">
+        <v>180</v>
+      </c>
+      <c r="S73" t="s">
+        <v>178</v>
+      </c>
+      <c r="T73" t="s">
+        <v>180</v>
+      </c>
+      <c r="U73" t="s">
+        <v>183</v>
+      </c>
+      <c r="V73" t="s">
+        <v>184</v>
+      </c>
+      <c r="X73" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF73" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG73" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH73" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI73" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -7693,8 +8000,92 @@
       <c r="D74" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="75" spans="1:35">
+      <c r="E74" t="s">
+        <v>166</v>
+      </c>
+      <c r="H74" t="s">
+        <v>167</v>
+      </c>
+      <c r="I74" t="s">
+        <v>169</v>
+      </c>
+      <c r="J74" t="s">
+        <v>170</v>
+      </c>
+      <c r="K74" t="s">
+        <v>172</v>
+      </c>
+      <c r="L74" t="s">
+        <v>170</v>
+      </c>
+      <c r="M74" t="s">
+        <v>174</v>
+      </c>
+      <c r="N74" t="s">
+        <v>175</v>
+      </c>
+      <c r="O74" t="s">
+        <v>174</v>
+      </c>
+      <c r="P74" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>178</v>
+      </c>
+      <c r="R74" t="s">
+        <v>180</v>
+      </c>
+      <c r="S74" t="s">
+        <v>178</v>
+      </c>
+      <c r="T74" t="s">
+        <v>180</v>
+      </c>
+      <c r="U74" t="s">
+        <v>183</v>
+      </c>
+      <c r="V74" t="s">
+        <v>184</v>
+      </c>
+      <c r="X74" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG74" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH74" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI74" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="75" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -7707,8 +8098,92 @@
       <c r="D75" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="76" spans="1:35">
+      <c r="E75" t="s">
+        <v>166</v>
+      </c>
+      <c r="H75" t="s">
+        <v>167</v>
+      </c>
+      <c r="I75" t="s">
+        <v>169</v>
+      </c>
+      <c r="J75" t="s">
+        <v>170</v>
+      </c>
+      <c r="K75" t="s">
+        <v>172</v>
+      </c>
+      <c r="L75" t="s">
+        <v>170</v>
+      </c>
+      <c r="M75" t="s">
+        <v>174</v>
+      </c>
+      <c r="N75" t="s">
+        <v>175</v>
+      </c>
+      <c r="O75" t="s">
+        <v>174</v>
+      </c>
+      <c r="P75" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>178</v>
+      </c>
+      <c r="R75" t="s">
+        <v>180</v>
+      </c>
+      <c r="S75" t="s">
+        <v>178</v>
+      </c>
+      <c r="T75" t="s">
+        <v>180</v>
+      </c>
+      <c r="U75" t="s">
+        <v>183</v>
+      </c>
+      <c r="V75" t="s">
+        <v>184</v>
+      </c>
+      <c r="X75" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD75" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE75" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG75" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH75" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI75" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -7721,8 +8196,92 @@
       <c r="D76" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="77" spans="1:35">
+      <c r="E76" t="s">
+        <v>166</v>
+      </c>
+      <c r="H76" t="s">
+        <v>167</v>
+      </c>
+      <c r="I76" t="s">
+        <v>169</v>
+      </c>
+      <c r="J76" t="s">
+        <v>170</v>
+      </c>
+      <c r="K76" t="s">
+        <v>172</v>
+      </c>
+      <c r="L76" t="s">
+        <v>170</v>
+      </c>
+      <c r="M76" t="s">
+        <v>174</v>
+      </c>
+      <c r="N76" t="s">
+        <v>175</v>
+      </c>
+      <c r="O76" t="s">
+        <v>174</v>
+      </c>
+      <c r="P76" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>178</v>
+      </c>
+      <c r="R76" t="s">
+        <v>180</v>
+      </c>
+      <c r="S76" t="s">
+        <v>178</v>
+      </c>
+      <c r="T76" t="s">
+        <v>180</v>
+      </c>
+      <c r="U76" t="s">
+        <v>183</v>
+      </c>
+      <c r="V76" t="s">
+        <v>184</v>
+      </c>
+      <c r="X76" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC76" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD76" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF76" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG76" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH76" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI76" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -7735,8 +8294,92 @@
       <c r="D77" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="78" spans="1:35">
+      <c r="E77" t="s">
+        <v>166</v>
+      </c>
+      <c r="H77" t="s">
+        <v>167</v>
+      </c>
+      <c r="I77" t="s">
+        <v>169</v>
+      </c>
+      <c r="J77" t="s">
+        <v>170</v>
+      </c>
+      <c r="K77" t="s">
+        <v>172</v>
+      </c>
+      <c r="L77" t="s">
+        <v>170</v>
+      </c>
+      <c r="M77" t="s">
+        <v>174</v>
+      </c>
+      <c r="N77" t="s">
+        <v>175</v>
+      </c>
+      <c r="O77" t="s">
+        <v>174</v>
+      </c>
+      <c r="P77" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>178</v>
+      </c>
+      <c r="R77" t="s">
+        <v>180</v>
+      </c>
+      <c r="S77" t="s">
+        <v>178</v>
+      </c>
+      <c r="T77" t="s">
+        <v>180</v>
+      </c>
+      <c r="U77" t="s">
+        <v>183</v>
+      </c>
+      <c r="V77" t="s">
+        <v>184</v>
+      </c>
+      <c r="X77" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE77" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF77" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG77" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH77" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI77" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -7749,8 +8392,92 @@
       <c r="D78" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="79" spans="1:35">
+      <c r="E78" t="s">
+        <v>166</v>
+      </c>
+      <c r="H78" t="s">
+        <v>167</v>
+      </c>
+      <c r="I78" t="s">
+        <v>169</v>
+      </c>
+      <c r="J78" t="s">
+        <v>170</v>
+      </c>
+      <c r="K78" t="s">
+        <v>172</v>
+      </c>
+      <c r="L78" t="s">
+        <v>170</v>
+      </c>
+      <c r="M78" t="s">
+        <v>174</v>
+      </c>
+      <c r="N78" t="s">
+        <v>175</v>
+      </c>
+      <c r="O78" t="s">
+        <v>174</v>
+      </c>
+      <c r="P78" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>178</v>
+      </c>
+      <c r="R78" t="s">
+        <v>180</v>
+      </c>
+      <c r="S78" t="s">
+        <v>178</v>
+      </c>
+      <c r="T78" t="s">
+        <v>180</v>
+      </c>
+      <c r="U78" t="s">
+        <v>183</v>
+      </c>
+      <c r="V78" t="s">
+        <v>184</v>
+      </c>
+      <c r="X78" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC78" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD78" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE78" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF78" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG78" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH78" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI78" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -7763,8 +8490,92 @@
       <c r="D79" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="80" spans="1:35">
+      <c r="E79" t="s">
+        <v>166</v>
+      </c>
+      <c r="H79" t="s">
+        <v>167</v>
+      </c>
+      <c r="I79" t="s">
+        <v>169</v>
+      </c>
+      <c r="J79" t="s">
+        <v>170</v>
+      </c>
+      <c r="K79" t="s">
+        <v>172</v>
+      </c>
+      <c r="L79" t="s">
+        <v>170</v>
+      </c>
+      <c r="M79" t="s">
+        <v>174</v>
+      </c>
+      <c r="N79" t="s">
+        <v>175</v>
+      </c>
+      <c r="O79" t="s">
+        <v>174</v>
+      </c>
+      <c r="P79" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>178</v>
+      </c>
+      <c r="R79" t="s">
+        <v>180</v>
+      </c>
+      <c r="S79" t="s">
+        <v>178</v>
+      </c>
+      <c r="T79" t="s">
+        <v>180</v>
+      </c>
+      <c r="U79" t="s">
+        <v>183</v>
+      </c>
+      <c r="V79" t="s">
+        <v>184</v>
+      </c>
+      <c r="X79" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE79" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF79" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG79" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH79" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI79" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -7777,8 +8588,92 @@
       <c r="D80" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80" t="s">
+        <v>166</v>
+      </c>
+      <c r="H80" t="s">
+        <v>167</v>
+      </c>
+      <c r="I80" t="s">
+        <v>169</v>
+      </c>
+      <c r="J80" t="s">
+        <v>170</v>
+      </c>
+      <c r="K80" t="s">
+        <v>172</v>
+      </c>
+      <c r="L80" t="s">
+        <v>170</v>
+      </c>
+      <c r="M80" t="s">
+        <v>174</v>
+      </c>
+      <c r="N80" t="s">
+        <v>175</v>
+      </c>
+      <c r="O80" t="s">
+        <v>174</v>
+      </c>
+      <c r="P80" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>178</v>
+      </c>
+      <c r="R80" t="s">
+        <v>180</v>
+      </c>
+      <c r="S80" t="s">
+        <v>178</v>
+      </c>
+      <c r="T80" t="s">
+        <v>180</v>
+      </c>
+      <c r="U80" t="s">
+        <v>183</v>
+      </c>
+      <c r="V80" t="s">
+        <v>184</v>
+      </c>
+      <c r="X80" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD80" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE80" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF80" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG80" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH80" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI80" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="81" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -7791,8 +8686,92 @@
       <c r="D81" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81" t="s">
+        <v>166</v>
+      </c>
+      <c r="H81" t="s">
+        <v>167</v>
+      </c>
+      <c r="I81" t="s">
+        <v>169</v>
+      </c>
+      <c r="J81" t="s">
+        <v>170</v>
+      </c>
+      <c r="K81" t="s">
+        <v>172</v>
+      </c>
+      <c r="L81" t="s">
+        <v>170</v>
+      </c>
+      <c r="M81" t="s">
+        <v>174</v>
+      </c>
+      <c r="N81" t="s">
+        <v>175</v>
+      </c>
+      <c r="O81" t="s">
+        <v>174</v>
+      </c>
+      <c r="P81" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>178</v>
+      </c>
+      <c r="R81" t="s">
+        <v>180</v>
+      </c>
+      <c r="S81" t="s">
+        <v>178</v>
+      </c>
+      <c r="T81" t="s">
+        <v>180</v>
+      </c>
+      <c r="U81" t="s">
+        <v>183</v>
+      </c>
+      <c r="V81" t="s">
+        <v>184</v>
+      </c>
+      <c r="X81" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC81" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD81" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE81" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF81" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG81" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH81" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI81" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -7805,607 +8784,691 @@
       <c r="D82" t="s">
         <v>165</v>
       </c>
+      <c r="E82" t="s">
+        <v>166</v>
+      </c>
+      <c r="H82" t="s">
+        <v>167</v>
+      </c>
+      <c r="I82" t="s">
+        <v>169</v>
+      </c>
+      <c r="J82" t="s">
+        <v>170</v>
+      </c>
+      <c r="K82" t="s">
+        <v>172</v>
+      </c>
+      <c r="L82" t="s">
+        <v>170</v>
+      </c>
+      <c r="M82" t="s">
+        <v>174</v>
+      </c>
+      <c r="N82" t="s">
+        <v>175</v>
+      </c>
+      <c r="O82" t="s">
+        <v>174</v>
+      </c>
+      <c r="P82" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>178</v>
+      </c>
+      <c r="R82" t="s">
+        <v>180</v>
+      </c>
+      <c r="S82" t="s">
+        <v>178</v>
+      </c>
+      <c r="T82" t="s">
+        <v>180</v>
+      </c>
+      <c r="U82" t="s">
+        <v>183</v>
+      </c>
+      <c r="V82" t="s">
+        <v>184</v>
+      </c>
+      <c r="X82" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA82" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC82" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD82" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE82" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF82" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG82" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH82" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI82" t="s">
+        <v>253</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
-    <hyperlink ref="B77" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78"/>
-    <hyperlink ref="B80" r:id="rId79"/>
-    <hyperlink ref="B81" r:id="rId80"/>
-    <hyperlink ref="B82" r:id="rId81"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C33" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version after fixing list functions
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990A21DB-71FB-E845-94EF-05E266D8F2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="1340" windowWidth="28340" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -629,6 +623,9 @@
     <t>object_annotation_category</t>
   </si>
   <si>
+    <t>class_1</t>
+  </si>
+  <si>
     <t>object_annotation_status</t>
   </si>
   <si>
@@ -780,16 +777,13 @@
   </si>
   <si>
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
-  </si>
-  <si>
-    <t>class_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,14 +859,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -919,7 +905,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,27 +937,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1003,24 +971,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1196,19 +1146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1290,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -1431,10 +1376,10 @@
         <v>201</v>
       </c>
       <c r="AJ2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -1520,10 +1465,10 @@
         <v>201</v>
       </c>
       <c r="AJ3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1609,10 +1554,10 @@
         <v>201</v>
       </c>
       <c r="AJ4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1698,10 +1643,10 @@
         <v>201</v>
       </c>
       <c r="AJ5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -1787,10 +1732,10 @@
         <v>201</v>
       </c>
       <c r="AJ6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -1876,10 +1821,10 @@
         <v>201</v>
       </c>
       <c r="AJ7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -1965,10 +1910,10 @@
         <v>201</v>
       </c>
       <c r="AJ8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -2054,10 +1999,10 @@
         <v>201</v>
       </c>
       <c r="AJ9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -2143,10 +2088,10 @@
         <v>201</v>
       </c>
       <c r="AJ10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -2232,10 +2177,10 @@
         <v>201</v>
       </c>
       <c r="AJ11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -2321,10 +2266,10 @@
         <v>201</v>
       </c>
       <c r="AJ12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -2410,10 +2355,10 @@
         <v>201</v>
       </c>
       <c r="AJ13" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -2499,10 +2444,10 @@
         <v>201</v>
       </c>
       <c r="AJ14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -2588,10 +2533,10 @@
         <v>201</v>
       </c>
       <c r="AJ15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -2677,10 +2622,10 @@
         <v>201</v>
       </c>
       <c r="AJ16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2766,10 +2711,10 @@
         <v>201</v>
       </c>
       <c r="AJ17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -2855,10 +2800,10 @@
         <v>201</v>
       </c>
       <c r="AJ18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -2944,10 +2889,10 @@
         <v>201</v>
       </c>
       <c r="AJ19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -3033,10 +2978,10 @@
         <v>201</v>
       </c>
       <c r="AJ20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -3122,10 +3067,10 @@
         <v>201</v>
       </c>
       <c r="AJ21" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3211,10 +3156,10 @@
         <v>201</v>
       </c>
       <c r="AJ22" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3300,10 +3245,10 @@
         <v>201</v>
       </c>
       <c r="AJ23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3389,10 +3334,10 @@
         <v>201</v>
       </c>
       <c r="AJ24" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3478,10 +3423,10 @@
         <v>201</v>
       </c>
       <c r="AJ25" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3567,10 +3512,10 @@
         <v>201</v>
       </c>
       <c r="AJ26" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3656,10 +3601,10 @@
         <v>201</v>
       </c>
       <c r="AJ27" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3745,10 +3690,10 @@
         <v>201</v>
       </c>
       <c r="AJ28" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -3834,10 +3779,10 @@
         <v>201</v>
       </c>
       <c r="AJ29" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -3923,10 +3868,10 @@
         <v>201</v>
       </c>
       <c r="AJ30" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -4012,10 +3957,10 @@
         <v>201</v>
       </c>
       <c r="AJ31" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -4101,10 +4046,10 @@
         <v>201</v>
       </c>
       <c r="AJ32" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4190,10 +4135,10 @@
         <v>201</v>
       </c>
       <c r="AJ33" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4279,10 +4224,10 @@
         <v>201</v>
       </c>
       <c r="AJ34" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4368,10 +4313,10 @@
         <v>201</v>
       </c>
       <c r="AJ35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4457,10 +4402,10 @@
         <v>201</v>
       </c>
       <c r="AJ36" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4546,10 +4491,10 @@
         <v>201</v>
       </c>
       <c r="AJ37" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4635,10 +4580,10 @@
         <v>201</v>
       </c>
       <c r="AJ38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4724,10 +4669,10 @@
         <v>201</v>
       </c>
       <c r="AJ39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -4813,10 +4758,10 @@
         <v>201</v>
       </c>
       <c r="AJ40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -4902,10 +4847,10 @@
         <v>201</v>
       </c>
       <c r="AJ41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -4991,10 +4936,10 @@
         <v>201</v>
       </c>
       <c r="AJ42" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -5080,10 +5025,10 @@
         <v>201</v>
       </c>
       <c r="AJ43" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -5169,10 +5114,10 @@
         <v>201</v>
       </c>
       <c r="AJ44" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5258,10 +5203,10 @@
         <v>201</v>
       </c>
       <c r="AJ45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5347,10 +5292,10 @@
         <v>201</v>
       </c>
       <c r="AJ46" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5436,10 +5381,10 @@
         <v>201</v>
       </c>
       <c r="AJ47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -5534,10 +5479,10 @@
         <v>200</v>
       </c>
       <c r="AI48" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5632,10 +5577,10 @@
         <v>200</v>
       </c>
       <c r="AI49" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -5730,10 +5675,10 @@
         <v>200</v>
       </c>
       <c r="AI50" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -5828,10 +5773,10 @@
         <v>200</v>
       </c>
       <c r="AI51" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:35">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -5926,10 +5871,10 @@
         <v>200</v>
       </c>
       <c r="AI52" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:35">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -6024,10 +5969,10 @@
         <v>200</v>
       </c>
       <c r="AI53" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:35">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -6122,10 +6067,10 @@
         <v>200</v>
       </c>
       <c r="AI54" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -6220,10 +6165,10 @@
         <v>200</v>
       </c>
       <c r="AI55" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -6318,10 +6263,10 @@
         <v>200</v>
       </c>
       <c r="AI56" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -6416,10 +6361,10 @@
         <v>200</v>
       </c>
       <c r="AI57" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -6514,10 +6459,10 @@
         <v>200</v>
       </c>
       <c r="AI58" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:35">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -6612,10 +6557,10 @@
         <v>200</v>
       </c>
       <c r="AI59" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -6710,10 +6655,10 @@
         <v>200</v>
       </c>
       <c r="AI60" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -6808,10 +6753,10 @@
         <v>200</v>
       </c>
       <c r="AI61" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -6906,10 +6851,10 @@
         <v>200</v>
       </c>
       <c r="AI62" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -7004,10 +6949,10 @@
         <v>200</v>
       </c>
       <c r="AI63" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -7102,10 +7047,10 @@
         <v>200</v>
       </c>
       <c r="AI64" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -7200,10 +7145,10 @@
         <v>200</v>
       </c>
       <c r="AI65" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -7298,10 +7243,10 @@
         <v>200</v>
       </c>
       <c r="AI66" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -7396,10 +7341,10 @@
         <v>200</v>
       </c>
       <c r="AI67" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -7494,10 +7439,10 @@
         <v>200</v>
       </c>
       <c r="AI68" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -7592,10 +7537,10 @@
         <v>200</v>
       </c>
       <c r="AI69" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -7690,10 +7635,10 @@
         <v>200</v>
       </c>
       <c r="AI70" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:35">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -7788,10 +7733,10 @@
         <v>200</v>
       </c>
       <c r="AI71" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:35">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -7886,10 +7831,10 @@
         <v>200</v>
       </c>
       <c r="AI72" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:35">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -7984,10 +7929,10 @@
         <v>200</v>
       </c>
       <c r="AI73" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -8082,10 +8027,10 @@
         <v>200</v>
       </c>
       <c r="AI74" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:35">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -8180,10 +8125,10 @@
         <v>200</v>
       </c>
       <c r="AI75" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:35">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -8278,10 +8223,10 @@
         <v>200</v>
       </c>
       <c r="AI76" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -8376,10 +8321,10 @@
         <v>200</v>
       </c>
       <c r="AI77" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -8474,10 +8419,10 @@
         <v>200</v>
       </c>
       <c r="AI78" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -8572,10 +8517,10 @@
         <v>200</v>
       </c>
       <c r="AI79" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -8670,10 +8615,10 @@
         <v>200</v>
       </c>
       <c r="AI80" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:35">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -8768,10 +8713,10 @@
         <v>200</v>
       </c>
       <c r="AI81" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -8866,609 +8811,609 @@
         <v>200</v>
       </c>
       <c r="AI82" t="s">
-        <v>253</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B18" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B21" r:id="rId20"/>
+    <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="B23" r:id="rId22"/>
+    <hyperlink ref="B24" r:id="rId23"/>
+    <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="B39" r:id="rId38"/>
+    <hyperlink ref="B40" r:id="rId39"/>
+    <hyperlink ref="B41" r:id="rId40"/>
+    <hyperlink ref="B42" r:id="rId41"/>
+    <hyperlink ref="B43" r:id="rId42"/>
+    <hyperlink ref="B44" r:id="rId43"/>
+    <hyperlink ref="B45" r:id="rId44"/>
+    <hyperlink ref="B46" r:id="rId45"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="B53" r:id="rId52"/>
+    <hyperlink ref="B54" r:id="rId53"/>
+    <hyperlink ref="B55" r:id="rId54"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="B57" r:id="rId56"/>
+    <hyperlink ref="B58" r:id="rId57"/>
+    <hyperlink ref="B59" r:id="rId58"/>
+    <hyperlink ref="B60" r:id="rId59"/>
+    <hyperlink ref="B61" r:id="rId60"/>
+    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="B63" r:id="rId62"/>
+    <hyperlink ref="B64" r:id="rId63"/>
+    <hyperlink ref="B65" r:id="rId64"/>
+    <hyperlink ref="B66" r:id="rId65"/>
+    <hyperlink ref="B67" r:id="rId66"/>
+    <hyperlink ref="B68" r:id="rId67"/>
+    <hyperlink ref="B69" r:id="rId68"/>
+    <hyperlink ref="B70" r:id="rId69"/>
+    <hyperlink ref="B71" r:id="rId70"/>
+    <hyperlink ref="B72" r:id="rId71"/>
+    <hyperlink ref="B73" r:id="rId72"/>
+    <hyperlink ref="B74" r:id="rId73"/>
+    <hyperlink ref="B75" r:id="rId74"/>
+    <hyperlink ref="B76" r:id="rId75"/>
+    <hyperlink ref="B77" r:id="rId76"/>
+    <hyperlink ref="B78" r:id="rId77"/>
+    <hyperlink ref="B79" r:id="rId78"/>
+    <hyperlink ref="B80" r:id="rId79"/>
+    <hyperlink ref="B81" r:id="rId80"/>
+    <hyperlink ref="B82" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C25" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C26" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C30" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C36" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C38" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C40" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C41" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C43" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C45" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C46" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated after running step2
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2637" uniqueCount="300">
   <si>
     <t>Project_ID</t>
   </si>
@@ -627,6 +627,144 @@
   </si>
   <si>
     <t>object_annotation_status</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_2248_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3147_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3289_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3290_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3294_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3295_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3296_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3297_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3298_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3299_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3300_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3301_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3302_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3303_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3304_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3305_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3306_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3307_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3308_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3309_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3310_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3311_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3312_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3313_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3314_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3315_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3318_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3320_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3321_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3322_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3323_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3324_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3325_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3326_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3331_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3332_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3333_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3334_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3335_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3337_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3338_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3339_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3340_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3341_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3342_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/IFCB/project_3343_flags.tsv</t>
   </si>
   <si>
     <t>Variables</t>
@@ -1378,6 +1516,9 @@
       <c r="AJ2" t="s">
         <v>203</v>
       </c>
+      <c r="AK2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="3" spans="1:45">
       <c r="A3">
@@ -1467,6 +1608,9 @@
       <c r="AJ3" t="s">
         <v>203</v>
       </c>
+      <c r="AK3" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="4" spans="1:45">
       <c r="A4">
@@ -1556,6 +1700,9 @@
       <c r="AJ4" t="s">
         <v>203</v>
       </c>
+      <c r="AK4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="5" spans="1:45">
       <c r="A5">
@@ -1645,6 +1792,9 @@
       <c r="AJ5" t="s">
         <v>203</v>
       </c>
+      <c r="AK5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="6" spans="1:45">
       <c r="A6">
@@ -1734,6 +1884,9 @@
       <c r="AJ6" t="s">
         <v>203</v>
       </c>
+      <c r="AK6" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="7" spans="1:45">
       <c r="A7">
@@ -1823,6 +1976,9 @@
       <c r="AJ7" t="s">
         <v>203</v>
       </c>
+      <c r="AK7" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="8" spans="1:45">
       <c r="A8">
@@ -1912,6 +2068,9 @@
       <c r="AJ8" t="s">
         <v>203</v>
       </c>
+      <c r="AK8" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="9" spans="1:45">
       <c r="A9">
@@ -2001,6 +2160,9 @@
       <c r="AJ9" t="s">
         <v>203</v>
       </c>
+      <c r="AK9" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="10" spans="1:45">
       <c r="A10">
@@ -2090,6 +2252,9 @@
       <c r="AJ10" t="s">
         <v>203</v>
       </c>
+      <c r="AK10" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="11" spans="1:45">
       <c r="A11">
@@ -2179,6 +2344,9 @@
       <c r="AJ11" t="s">
         <v>203</v>
       </c>
+      <c r="AK11" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="12" spans="1:45">
       <c r="A12">
@@ -2268,6 +2436,9 @@
       <c r="AJ12" t="s">
         <v>203</v>
       </c>
+      <c r="AK12" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="13" spans="1:45">
       <c r="A13">
@@ -2357,6 +2528,9 @@
       <c r="AJ13" t="s">
         <v>203</v>
       </c>
+      <c r="AK13" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="14" spans="1:45">
       <c r="A14">
@@ -2446,6 +2620,9 @@
       <c r="AJ14" t="s">
         <v>203</v>
       </c>
+      <c r="AK14" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="15" spans="1:45">
       <c r="A15">
@@ -2535,6 +2712,9 @@
       <c r="AJ15" t="s">
         <v>203</v>
       </c>
+      <c r="AK15" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="16" spans="1:45">
       <c r="A16">
@@ -2624,8 +2804,11 @@
       <c r="AJ16" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="17" spans="1:36">
+      <c r="AK16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2713,8 +2896,11 @@
       <c r="AJ17" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="18" spans="1:36">
+      <c r="AK17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -2802,8 +2988,11 @@
       <c r="AJ18" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="19" spans="1:36">
+      <c r="AK18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -2891,8 +3080,11 @@
       <c r="AJ19" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="20" spans="1:36">
+      <c r="AK19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -2980,8 +3172,11 @@
       <c r="AJ20" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="21" spans="1:36">
+      <c r="AK20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -3069,8 +3264,11 @@
       <c r="AJ21" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:36">
+      <c r="AK21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3158,8 +3356,11 @@
       <c r="AJ22" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="23" spans="1:36">
+      <c r="AK22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3247,8 +3448,11 @@
       <c r="AJ23" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="24" spans="1:36">
+      <c r="AK23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3336,8 +3540,11 @@
       <c r="AJ24" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="25" spans="1:36">
+      <c r="AK24" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3425,8 +3632,11 @@
       <c r="AJ25" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="26" spans="1:36">
+      <c r="AK25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3514,8 +3724,11 @@
       <c r="AJ26" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="27" spans="1:36">
+      <c r="AK26" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3603,8 +3816,11 @@
       <c r="AJ27" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="28" spans="1:36">
+      <c r="AK27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3692,8 +3908,11 @@
       <c r="AJ28" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="29" spans="1:36">
+      <c r="AK28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -3781,8 +4000,11 @@
       <c r="AJ29" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="30" spans="1:36">
+      <c r="AK29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -3870,8 +4092,11 @@
       <c r="AJ30" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="31" spans="1:36">
+      <c r="AK30" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -3959,8 +4184,11 @@
       <c r="AJ31" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="32" spans="1:36">
+      <c r="AK31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -4048,8 +4276,11 @@
       <c r="AJ32" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="33" spans="1:36">
+      <c r="AK32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4137,8 +4368,11 @@
       <c r="AJ33" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="34" spans="1:36">
+      <c r="AK33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4226,8 +4460,11 @@
       <c r="AJ34" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="35" spans="1:36">
+      <c r="AK34" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4315,8 +4552,11 @@
       <c r="AJ35" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="36" spans="1:36">
+      <c r="AK35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4404,8 +4644,11 @@
       <c r="AJ36" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="37" spans="1:36">
+      <c r="AK36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4493,8 +4736,11 @@
       <c r="AJ37" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="38" spans="1:36">
+      <c r="AK37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4582,8 +4828,11 @@
       <c r="AJ38" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="39" spans="1:36">
+      <c r="AK38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4671,8 +4920,11 @@
       <c r="AJ39" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="40" spans="1:36">
+      <c r="AK39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -4760,8 +5012,11 @@
       <c r="AJ40" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="41" spans="1:36">
+      <c r="AK40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -4849,8 +5104,11 @@
       <c r="AJ41" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="42" spans="1:36">
+      <c r="AK41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -4938,8 +5196,11 @@
       <c r="AJ42" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="43" spans="1:36">
+      <c r="AK42" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -5027,8 +5288,11 @@
       <c r="AJ43" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="44" spans="1:36">
+      <c r="AK43" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -5116,8 +5380,11 @@
       <c r="AJ44" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="45" spans="1:36">
+      <c r="AK44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5205,8 +5472,11 @@
       <c r="AJ45" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="46" spans="1:36">
+      <c r="AK45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5294,8 +5564,11 @@
       <c r="AJ46" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="47" spans="1:36">
+      <c r="AK46" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5383,8 +5656,11 @@
       <c r="AJ47" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="48" spans="1:36">
+      <c r="AK47" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -8912,13 +9188,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8926,10 +9202,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8937,10 +9213,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
-        <v>210</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8948,10 +9224,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -8959,10 +9235,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8970,10 +9246,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8981,10 +9257,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8992,10 +9268,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -9003,10 +9279,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -9014,10 +9290,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -9025,10 +9301,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -9036,10 +9312,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -9047,10 +9323,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -9058,10 +9334,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -9069,10 +9345,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C15" t="s">
-        <v>222</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -9080,10 +9356,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -9091,10 +9367,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -9102,10 +9378,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C18" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -9113,10 +9389,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C19" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -9124,10 +9400,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C20" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -9135,10 +9411,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -9146,10 +9422,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C22" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -9157,10 +9433,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C23" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -9168,10 +9444,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -9179,10 +9455,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C25" t="s">
-        <v>232</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -9190,10 +9466,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -9201,10 +9477,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C27" t="s">
-        <v>234</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -9212,10 +9488,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -9223,10 +9499,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -9234,10 +9510,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C30" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -9245,10 +9521,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -9256,10 +9532,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C32" t="s">
-        <v>239</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -9267,10 +9543,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C33" t="s">
-        <v>240</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -9278,10 +9554,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -9289,10 +9565,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -9300,10 +9576,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -9311,10 +9587,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
+        <v>290</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -9322,10 +9598,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -9333,10 +9609,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -9344,10 +9620,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>293</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -9355,10 +9631,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
+        <v>294</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -9366,10 +9642,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -9377,10 +9653,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
+        <v>296</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -9388,10 +9664,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -9399,10 +9675,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -9410,10 +9686,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included dictionary like structure under the Sampling_description column, with the columns on the raw IFCB dashboard dataset that have IFCB config data
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A3053A-49C8-8D48-AB95-5A57B808C7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2637" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="303">
   <si>
     <t>Project_ID</t>
   </si>
@@ -915,13 +921,22 @@
   </si>
   <si>
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>minBlobArea</t>
+  </si>
+  <si>
+    <t>sample_vol_config:SyringeSampleVolume,pmtA:{voltage:PMTAhighVoltage,threshold:PMTAtriggerThreshold_DAQ_MCConly},pmtB{voltage:PMTBhighVoltage,threshold:PMTBtriggerThreshold_DAQ_MCConly}, pmtC:{voltage:PMTChighVoltage,threshold:PMTCtriggerThreshold_DAQ_MCConly}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,12 +999,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -997,11 +1013,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1043,7 +1067,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1075,9 +1099,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1109,6 +1151,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1284,14 +1344,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="S1" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1492,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -1520,7 +1584,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -1612,7 +1676,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1704,7 +1768,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1796,7 +1860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -1888,7 +1952,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -1980,7 +2044,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -2072,7 +2136,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -2164,7 +2228,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -2256,7 +2320,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -2348,7 +2412,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -2440,7 +2504,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -2532,7 +2596,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -2624,7 +2688,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -2716,7 +2780,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -2808,7 +2872,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2900,7 +2964,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -2992,7 +3056,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -3084,7 +3148,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -3176,7 +3240,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -3268,7 +3332,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3360,7 +3424,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3452,7 +3516,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3544,7 +3608,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3636,7 +3700,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3728,7 +3792,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3820,7 +3884,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3912,7 +3976,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -4004,7 +4068,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -4096,7 +4160,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -4188,7 +4252,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -4280,7 +4344,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4372,7 +4436,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4464,7 +4528,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4556,7 +4620,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4648,7 +4712,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4740,7 +4804,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4832,7 +4896,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4924,7 +4988,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -5016,7 +5080,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -5108,7 +5172,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -5200,7 +5264,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -5292,7 +5356,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -5384,7 +5448,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5476,7 +5540,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5568,7 +5632,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5660,7 +5724,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -5757,8 +5821,20 @@
       <c r="AI48" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="49" spans="1:35">
+      <c r="AN48" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO48" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP48" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS48" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5855,8 +5931,20 @@
       <c r="AI49" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="50" spans="1:35">
+      <c r="AN49" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO49" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS49" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -5953,8 +6041,20 @@
       <c r="AI50" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="51" spans="1:35">
+      <c r="AN50" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO50" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP50" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS50" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -6051,8 +6151,20 @@
       <c r="AI51" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="52" spans="1:35">
+      <c r="AN51" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO51" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP51" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS51" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -6149,8 +6261,20 @@
       <c r="AI52" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="53" spans="1:35">
+      <c r="AN52" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO52" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP52" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS52" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -6247,8 +6371,20 @@
       <c r="AI53" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="54" spans="1:35">
+      <c r="AN53" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO53" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP53" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS53" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -6345,8 +6481,20 @@
       <c r="AI54" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="55" spans="1:35">
+      <c r="AN54" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO54" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP54" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS54" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -6443,8 +6591,20 @@
       <c r="AI55" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="56" spans="1:35">
+      <c r="AN55" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO55" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS55" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -6541,8 +6701,20 @@
       <c r="AI56" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="57" spans="1:35">
+      <c r="AN56" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO56" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP56" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS56" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -6639,8 +6811,20 @@
       <c r="AI57" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="58" spans="1:35">
+      <c r="AN57" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO57" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP57" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS57" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -6737,8 +6921,20 @@
       <c r="AI58" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:35">
+      <c r="AN58" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO58" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP58" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS58" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -6835,8 +7031,20 @@
       <c r="AI59" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="60" spans="1:35">
+      <c r="AN59" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO59" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP59" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS59" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -6933,8 +7141,20 @@
       <c r="AI60" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="61" spans="1:35">
+      <c r="AN60" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO60" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP60" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS60" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -7031,8 +7251,20 @@
       <c r="AI61" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="62" spans="1:35">
+      <c r="AN61" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO61" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP61" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS61" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -7129,8 +7361,20 @@
       <c r="AI62" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="63" spans="1:35">
+      <c r="AN62" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO62" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP62" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS62" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -7227,8 +7471,20 @@
       <c r="AI63" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="64" spans="1:35">
+      <c r="AN63" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO63" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP63" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS63" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -7325,8 +7581,20 @@
       <c r="AI64" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="65" spans="1:35">
+      <c r="AN64" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO64" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP64" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS64" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -7423,8 +7691,20 @@
       <c r="AI65" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="66" spans="1:35">
+      <c r="AN65" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO65" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP65" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS65" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -7521,8 +7801,20 @@
       <c r="AI66" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="67" spans="1:35">
+      <c r="AN66" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO66" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP66" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS66" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -7619,8 +7911,20 @@
       <c r="AI67" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="68" spans="1:35">
+      <c r="AN67" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO67" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP67" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS67" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -7717,8 +8021,20 @@
       <c r="AI68" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="69" spans="1:35">
+      <c r="AN68" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO68" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP68" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS68" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -7815,8 +8131,20 @@
       <c r="AI69" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="70" spans="1:35">
+      <c r="AN69" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO69" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP69" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS69" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -7913,8 +8241,20 @@
       <c r="AI70" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="71" spans="1:35">
+      <c r="AN70" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO70" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP70" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS70" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -8011,8 +8351,20 @@
       <c r="AI71" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="72" spans="1:35">
+      <c r="AN71" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO71" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP71" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS71" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -8109,8 +8461,20 @@
       <c r="AI72" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="73" spans="1:35">
+      <c r="AN72" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO72" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP72" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS72" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -8207,8 +8571,20 @@
       <c r="AI73" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="74" spans="1:35">
+      <c r="AN73" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO73" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP73" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS73" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -8305,8 +8681,20 @@
       <c r="AI74" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="75" spans="1:35">
+      <c r="AN74" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO74" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP74" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS74" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -8403,8 +8791,20 @@
       <c r="AI75" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="76" spans="1:35">
+      <c r="AN75" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO75" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP75" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS75" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -8501,8 +8901,20 @@
       <c r="AI76" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="77" spans="1:35">
+      <c r="AN76" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO76" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP76" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS76" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -8599,8 +9011,20 @@
       <c r="AI77" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="78" spans="1:35">
+      <c r="AN77" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO77" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP77" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS77" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -8697,8 +9121,20 @@
       <c r="AI78" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="79" spans="1:35">
+      <c r="AN78" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO78" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP78" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS78" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -8795,8 +9231,20 @@
       <c r="AI79" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="80" spans="1:35">
+      <c r="AN79" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO79" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP79" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS79" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -8893,8 +9341,20 @@
       <c r="AI80" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="81" spans="1:35">
+      <c r="AN80" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO80" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP80" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS80" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="81" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -8991,8 +9451,20 @@
       <c r="AI81" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="82" spans="1:35">
+      <c r="AN81" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO81" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP81" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS81" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="82" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -9089,104 +9561,116 @@
       <c r="AI82" t="s">
         <v>202</v>
       </c>
+      <c r="AN82" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO82" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP82" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS82" t="s">
+        <v>302</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
-    <hyperlink ref="B77" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78"/>
-    <hyperlink ref="B80" r:id="rId79"/>
-    <hyperlink ref="B81" r:id="rId80"/>
-    <hyperlink ref="B82" r:id="rId81"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>250</v>
       </c>
@@ -9197,7 +9681,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9208,7 +9692,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -9219,7 +9703,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -9230,7 +9714,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -9241,7 +9725,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -9252,7 +9736,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -9263,7 +9747,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -9274,7 +9758,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -9285,7 +9769,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -9296,7 +9780,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -9307,7 +9791,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -9318,7 +9802,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -9329,7 +9813,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -9340,7 +9824,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -9351,7 +9835,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -9362,7 +9846,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -9373,7 +9857,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -9384,7 +9868,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -9395,7 +9879,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -9406,7 +9890,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -9417,7 +9901,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -9428,7 +9912,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -9439,7 +9923,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -9450,7 +9934,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -9461,7 +9945,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -9472,7 +9956,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -9483,7 +9967,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -9494,7 +9978,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -9505,7 +9989,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -9516,7 +10000,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -9527,7 +10011,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -9538,7 +10022,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -9549,7 +10033,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -9560,7 +10044,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -9571,7 +10055,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -9582,7 +10066,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -9593,7 +10077,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -9604,7 +10088,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -9615,7 +10099,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -9626,7 +10110,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -9637,7 +10121,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -9648,7 +10132,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -9659,7 +10143,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -9670,7 +10154,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -9681,7 +10165,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
updated to try to fix IFCB dashboard downloads after running step0
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A3053A-49C8-8D48-AB95-5A57B808C7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -773,6 +767,15 @@
     <t>~/GIT/PSSdb/raw/flags/IFCB/project_3343_flags.tsv</t>
   </si>
   <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>minBlobArea</t>
+  </si>
+  <si>
+    <t>sample_vol_config:SyringeSampleVolume,pmtA:{voltage:PMTAhighVoltage,threshold:PMTAtriggerThreshold_DAQ_MCConly},pmtB{voltage:PMTBhighVoltage,threshold:PMTBtriggerThreshold_DAQ_MCConly}, pmtC:{voltage:PMTChighVoltage,threshold:PMTCtriggerThreshold_DAQ_MCConly}</t>
+  </si>
+  <si>
     <t>Variables</t>
   </si>
   <si>
@@ -921,22 +924,13 @@
   </si>
   <si>
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>minBlobArea</t>
-  </si>
-  <si>
-    <t>sample_vol_config:SyringeSampleVolume,pmtA:{voltage:PMTAhighVoltage,threshold:PMTAtriggerThreshold_DAQ_MCConly},pmtB{voltage:PMTBhighVoltage,threshold:PMTBtriggerThreshold_DAQ_MCConly}, pmtC:{voltage:PMTChighVoltage,threshold:PMTCtriggerThreshold_DAQ_MCConly}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -999,13 +993,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1013,19 +1006,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1067,7 +1052,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1099,27 +1084,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1151,24 +1118,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1344,18 +1293,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -1584,7 +1529,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -1676,7 +1621,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1768,7 +1713,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1860,7 +1805,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -1952,7 +1897,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -2044,7 +1989,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -2136,7 +2081,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -2228,7 +2173,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -2320,7 +2265,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -2412,7 +2357,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -2504,7 +2449,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -2596,7 +2541,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -2688,7 +2633,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -2780,7 +2725,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -2872,7 +2817,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2964,7 +2909,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -3056,7 +3001,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -3148,7 +3093,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -3240,7 +3185,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -3332,7 +3277,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3424,7 +3369,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3516,7 +3461,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3608,7 +3553,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3700,7 +3645,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3792,7 +3737,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3884,7 +3829,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3976,7 +3921,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -4068,7 +4013,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -4160,7 +4105,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -4252,7 +4197,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -4344,7 +4289,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:45">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4436,7 +4381,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:45">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4528,7 +4473,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:45">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4620,7 +4565,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:45">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4712,7 +4657,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:45">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4804,7 +4749,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:45">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4896,7 +4841,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:45">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4988,7 +4933,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:45">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -5080,7 +5025,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:45">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -5172,7 +5117,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:45">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -5264,7 +5209,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:45">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -5356,7 +5301,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:45">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -5448,7 +5393,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:45">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5540,7 +5485,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:45">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5632,7 +5577,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:45">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5724,7 +5669,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:45">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -5822,19 +5767,19 @@
         <v>202</v>
       </c>
       <c r="AN48" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO48" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO48" t="s">
+        <v>251</v>
       </c>
       <c r="AP48" t="s">
         <v>194</v>
       </c>
       <c r="AS48" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5932,19 +5877,19 @@
         <v>202</v>
       </c>
       <c r="AN49" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO49" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO49" t="s">
+        <v>251</v>
       </c>
       <c r="AP49" t="s">
         <v>194</v>
       </c>
       <c r="AS49" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -6042,19 +5987,19 @@
         <v>202</v>
       </c>
       <c r="AN50" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO50" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO50" t="s">
+        <v>251</v>
       </c>
       <c r="AP50" t="s">
         <v>194</v>
       </c>
       <c r="AS50" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -6152,19 +6097,19 @@
         <v>202</v>
       </c>
       <c r="AN51" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO51" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO51" t="s">
+        <v>251</v>
       </c>
       <c r="AP51" t="s">
         <v>194</v>
       </c>
       <c r="AS51" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:45">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -6262,19 +6207,19 @@
         <v>202</v>
       </c>
       <c r="AN52" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO52" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO52" t="s">
+        <v>251</v>
       </c>
       <c r="AP52" t="s">
         <v>194</v>
       </c>
       <c r="AS52" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:45">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -6372,19 +6317,19 @@
         <v>202</v>
       </c>
       <c r="AN53" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO53" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO53" t="s">
+        <v>251</v>
       </c>
       <c r="AP53" t="s">
         <v>194</v>
       </c>
       <c r="AS53" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:45">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -6482,19 +6427,19 @@
         <v>202</v>
       </c>
       <c r="AN54" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO54" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO54" t="s">
+        <v>251</v>
       </c>
       <c r="AP54" t="s">
         <v>194</v>
       </c>
       <c r="AS54" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:45">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -6592,19 +6537,19 @@
         <v>202</v>
       </c>
       <c r="AN55" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO55" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO55" t="s">
+        <v>251</v>
       </c>
       <c r="AP55" t="s">
         <v>194</v>
       </c>
       <c r="AS55" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:45">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -6702,19 +6647,19 @@
         <v>202</v>
       </c>
       <c r="AN56" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO56" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO56" t="s">
+        <v>251</v>
       </c>
       <c r="AP56" t="s">
         <v>194</v>
       </c>
       <c r="AS56" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:45">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -6812,19 +6757,19 @@
         <v>202</v>
       </c>
       <c r="AN57" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO57" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO57" t="s">
+        <v>251</v>
       </c>
       <c r="AP57" t="s">
         <v>194</v>
       </c>
       <c r="AS57" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:45">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -6922,19 +6867,19 @@
         <v>202</v>
       </c>
       <c r="AN58" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO58" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO58" t="s">
+        <v>251</v>
       </c>
       <c r="AP58" t="s">
         <v>194</v>
       </c>
       <c r="AS58" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:45">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -7032,19 +6977,19 @@
         <v>202</v>
       </c>
       <c r="AN59" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO59" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO59" t="s">
+        <v>251</v>
       </c>
       <c r="AP59" t="s">
         <v>194</v>
       </c>
       <c r="AS59" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:45">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -7142,19 +7087,19 @@
         <v>202</v>
       </c>
       <c r="AN60" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO60" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO60" t="s">
+        <v>251</v>
       </c>
       <c r="AP60" t="s">
         <v>194</v>
       </c>
       <c r="AS60" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:45">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -7252,19 +7197,19 @@
         <v>202</v>
       </c>
       <c r="AN61" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO61" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO61" t="s">
+        <v>251</v>
       </c>
       <c r="AP61" t="s">
         <v>194</v>
       </c>
       <c r="AS61" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:45">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -7362,19 +7307,19 @@
         <v>202</v>
       </c>
       <c r="AN62" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO62" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO62" t="s">
+        <v>251</v>
       </c>
       <c r="AP62" t="s">
         <v>194</v>
       </c>
       <c r="AS62" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:45">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -7472,19 +7417,19 @@
         <v>202</v>
       </c>
       <c r="AN63" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO63" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO63" t="s">
+        <v>251</v>
       </c>
       <c r="AP63" t="s">
         <v>194</v>
       </c>
       <c r="AS63" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:45">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -7582,19 +7527,19 @@
         <v>202</v>
       </c>
       <c r="AN64" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO64" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO64" t="s">
+        <v>251</v>
       </c>
       <c r="AP64" t="s">
         <v>194</v>
       </c>
       <c r="AS64" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:45">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -7692,19 +7637,19 @@
         <v>202</v>
       </c>
       <c r="AN65" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO65" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO65" t="s">
+        <v>251</v>
       </c>
       <c r="AP65" t="s">
         <v>194</v>
       </c>
       <c r="AS65" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:45">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -7802,19 +7747,19 @@
         <v>202</v>
       </c>
       <c r="AN66" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO66" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO66" t="s">
+        <v>251</v>
       </c>
       <c r="AP66" t="s">
         <v>194</v>
       </c>
       <c r="AS66" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:45">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -7912,19 +7857,19 @@
         <v>202</v>
       </c>
       <c r="AN67" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO67" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO67" t="s">
+        <v>251</v>
       </c>
       <c r="AP67" t="s">
         <v>194</v>
       </c>
       <c r="AS67" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:45">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -8022,19 +7967,19 @@
         <v>202</v>
       </c>
       <c r="AN68" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO68" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO68" t="s">
+        <v>251</v>
       </c>
       <c r="AP68" t="s">
         <v>194</v>
       </c>
       <c r="AS68" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:45">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -8132,19 +8077,19 @@
         <v>202</v>
       </c>
       <c r="AN69" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO69" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO69" t="s">
+        <v>251</v>
       </c>
       <c r="AP69" t="s">
         <v>194</v>
       </c>
       <c r="AS69" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:45">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -8242,19 +8187,19 @@
         <v>202</v>
       </c>
       <c r="AN70" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO70" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO70" t="s">
+        <v>251</v>
       </c>
       <c r="AP70" t="s">
         <v>194</v>
       </c>
       <c r="AS70" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:45">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -8352,19 +8297,19 @@
         <v>202</v>
       </c>
       <c r="AN71" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO71" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO71" t="s">
+        <v>251</v>
       </c>
       <c r="AP71" t="s">
         <v>194</v>
       </c>
       <c r="AS71" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:45">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -8462,19 +8407,19 @@
         <v>202</v>
       </c>
       <c r="AN72" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO72" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO72" t="s">
+        <v>251</v>
       </c>
       <c r="AP72" t="s">
         <v>194</v>
       </c>
       <c r="AS72" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:45">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -8572,19 +8517,19 @@
         <v>202</v>
       </c>
       <c r="AN73" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO73" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO73" t="s">
+        <v>251</v>
       </c>
       <c r="AP73" t="s">
         <v>194</v>
       </c>
       <c r="AS73" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:45">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -8682,19 +8627,19 @@
         <v>202</v>
       </c>
       <c r="AN74" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO74" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO74" t="s">
+        <v>251</v>
       </c>
       <c r="AP74" t="s">
         <v>194</v>
       </c>
       <c r="AS74" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:45">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -8792,19 +8737,19 @@
         <v>202</v>
       </c>
       <c r="AN75" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO75" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO75" t="s">
+        <v>251</v>
       </c>
       <c r="AP75" t="s">
         <v>194</v>
       </c>
       <c r="AS75" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:45">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -8902,19 +8847,19 @@
         <v>202</v>
       </c>
       <c r="AN76" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO76" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO76" t="s">
+        <v>251</v>
       </c>
       <c r="AP76" t="s">
         <v>194</v>
       </c>
       <c r="AS76" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:45">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -9012,19 +8957,19 @@
         <v>202</v>
       </c>
       <c r="AN77" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO77" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO77" t="s">
+        <v>251</v>
       </c>
       <c r="AP77" t="s">
         <v>194</v>
       </c>
       <c r="AS77" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:45">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -9122,19 +9067,19 @@
         <v>202</v>
       </c>
       <c r="AN78" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO78" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO78" t="s">
+        <v>251</v>
       </c>
       <c r="AP78" t="s">
         <v>194</v>
       </c>
       <c r="AS78" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="1:45">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -9232,19 +9177,19 @@
         <v>202</v>
       </c>
       <c r="AN79" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO79" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO79" t="s">
+        <v>251</v>
       </c>
       <c r="AP79" t="s">
         <v>194</v>
       </c>
       <c r="AS79" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="1:45">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -9342,19 +9287,19 @@
         <v>202</v>
       </c>
       <c r="AN80" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO80" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO80" t="s">
+        <v>251</v>
       </c>
       <c r="AP80" t="s">
         <v>194</v>
       </c>
       <c r="AS80" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:45">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -9452,19 +9397,19 @@
         <v>202</v>
       </c>
       <c r="AN81" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO81" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO81" t="s">
+        <v>251</v>
       </c>
       <c r="AP81" t="s">
         <v>194</v>
       </c>
       <c r="AS81" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="82" spans="1:45" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:45">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -9562,618 +9507,618 @@
         <v>202</v>
       </c>
       <c r="AN82" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO82" s="3" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="AO82" t="s">
+        <v>251</v>
       </c>
       <c r="AP82" t="s">
         <v>194</v>
       </c>
       <c r="AS82" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B18" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B21" r:id="rId20"/>
+    <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="B23" r:id="rId22"/>
+    <hyperlink ref="B24" r:id="rId23"/>
+    <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="B39" r:id="rId38"/>
+    <hyperlink ref="B40" r:id="rId39"/>
+    <hyperlink ref="B41" r:id="rId40"/>
+    <hyperlink ref="B42" r:id="rId41"/>
+    <hyperlink ref="B43" r:id="rId42"/>
+    <hyperlink ref="B44" r:id="rId43"/>
+    <hyperlink ref="B45" r:id="rId44"/>
+    <hyperlink ref="B46" r:id="rId45"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="B53" r:id="rId52"/>
+    <hyperlink ref="B54" r:id="rId53"/>
+    <hyperlink ref="B55" r:id="rId54"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="B57" r:id="rId56"/>
+    <hyperlink ref="B58" r:id="rId57"/>
+    <hyperlink ref="B59" r:id="rId58"/>
+    <hyperlink ref="B60" r:id="rId59"/>
+    <hyperlink ref="B61" r:id="rId60"/>
+    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="B63" r:id="rId62"/>
+    <hyperlink ref="B64" r:id="rId63"/>
+    <hyperlink ref="B65" r:id="rId64"/>
+    <hyperlink ref="B66" r:id="rId65"/>
+    <hyperlink ref="B67" r:id="rId66"/>
+    <hyperlink ref="B68" r:id="rId67"/>
+    <hyperlink ref="B69" r:id="rId68"/>
+    <hyperlink ref="B70" r:id="rId69"/>
+    <hyperlink ref="B71" r:id="rId70"/>
+    <hyperlink ref="B72" r:id="rId71"/>
+    <hyperlink ref="B73" r:id="rId72"/>
+    <hyperlink ref="B74" r:id="rId73"/>
+    <hyperlink ref="B75" r:id="rId74"/>
+    <hyperlink ref="B76" r:id="rId75"/>
+    <hyperlink ref="B77" r:id="rId76"/>
+    <hyperlink ref="B78" r:id="rId77"/>
+    <hyperlink ref="B79" r:id="rId78"/>
+    <hyperlink ref="B80" r:id="rId79"/>
+    <hyperlink ref="B81" r:id="rId80"/>
+    <hyperlink ref="B82" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C13" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C18" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C21" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C22" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C23" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C24" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C25" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C26" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C27" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C29" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C30" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C31" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C32" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C33" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C34" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C35" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C36" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C37" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C38" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C39" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C40" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C41" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C42" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C43" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C44" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C45" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C46" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed sample ID for IFCB dashboard projects
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B1E522-405F-9B45-8E37-AFCE38E8CBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="37300" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="304">
   <si>
     <t>Project_ID</t>
   </si>
@@ -767,15 +773,15 @@
     <t>~/GIT/PSSdb/raw/flags/IFCB/project_3343_flags.tsv</t>
   </si>
   <si>
+    <t>~/GIT/PSSdb/raw/flags/EXPORTS/project_EXPORTS_flags.tsv</t>
+  </si>
+  <si>
     <t>sample_type</t>
   </si>
   <si>
     <t>minBlobArea</t>
   </si>
   <si>
-    <t>sample_vol_config:SyringeSampleVolume,pmtA:{voltage:PMTAhighVoltage,threshold:PMTAtriggerThreshold_DAQ_MCConly},pmtB{voltage:PMTBhighVoltage,threshold:PMTBtriggerThreshold_DAQ_MCConly}, pmtC:{voltage:PMTChighVoltage,threshold:PMTCtriggerThreshold_DAQ_MCConly}</t>
-  </si>
-  <si>
     <t>Variables</t>
   </si>
   <si>
@@ -924,13 +930,16 @@
   </si>
   <si>
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
+  </si>
+  <si>
+    <t>sample_vol_config:SyringeSampleVolume; pmtA: {voltage:PMTAhighVoltage,threshold:PMTAtriggerThreshold_DAQ_MCConly}; pmtB: {voltage:PMTBhighVoltage,threshold:PMTBtriggerThreshold_DAQ_MCConly}; pmtC: {voltage:PMTChighVoltage,threshold:PMTCtriggerThreshold_DAQ_MCConly}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1006,6 +1015,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1052,7 +1069,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1084,9 +1101,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1118,6 +1153,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1293,14 +1346,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AF37" workbookViewId="0">
+      <selection activeCell="AV71" sqref="AV71"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1492,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2248</v>
       </c>
@@ -1529,7 +1584,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3147</v>
       </c>
@@ -1621,7 +1676,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3289</v>
       </c>
@@ -1713,7 +1768,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3290</v>
       </c>
@@ -1805,7 +1860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3294</v>
       </c>
@@ -1897,7 +1952,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3295</v>
       </c>
@@ -1989,7 +2044,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3296</v>
       </c>
@@ -2081,7 +2136,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3297</v>
       </c>
@@ -2173,7 +2228,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3298</v>
       </c>
@@ -2265,7 +2320,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3299</v>
       </c>
@@ -2357,7 +2412,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3300</v>
       </c>
@@ -2449,7 +2504,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3301</v>
       </c>
@@ -2541,7 +2596,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3302</v>
       </c>
@@ -2633,7 +2688,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3303</v>
       </c>
@@ -2725,7 +2780,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3304</v>
       </c>
@@ -2817,7 +2872,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3305</v>
       </c>
@@ -2909,7 +2964,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3306</v>
       </c>
@@ -3001,7 +3056,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3307</v>
       </c>
@@ -3093,7 +3148,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3308</v>
       </c>
@@ -3185,7 +3240,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3309</v>
       </c>
@@ -3277,7 +3332,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3310</v>
       </c>
@@ -3369,7 +3424,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3311</v>
       </c>
@@ -3461,7 +3516,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3312</v>
       </c>
@@ -3553,7 +3608,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3313</v>
       </c>
@@ -3645,7 +3700,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3314</v>
       </c>
@@ -3737,7 +3792,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3315</v>
       </c>
@@ -3829,7 +3884,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3318</v>
       </c>
@@ -3921,7 +3976,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3320</v>
       </c>
@@ -4013,7 +4068,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3321</v>
       </c>
@@ -4105,7 +4160,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3322</v>
       </c>
@@ -4197,7 +4252,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3323</v>
       </c>
@@ -4289,7 +4344,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:45">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3324</v>
       </c>
@@ -4381,7 +4436,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:45">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3325</v>
       </c>
@@ -4473,7 +4528,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:45">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3326</v>
       </c>
@@ -4565,7 +4620,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:45">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3331</v>
       </c>
@@ -4657,7 +4712,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:45">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3332</v>
       </c>
@@ -4749,7 +4804,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:45">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3333</v>
       </c>
@@ -4841,7 +4896,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:45">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3334</v>
       </c>
@@ -4933,7 +4988,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:45">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3335</v>
       </c>
@@ -5025,7 +5080,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:45">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3337</v>
       </c>
@@ -5117,7 +5172,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:45">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3338</v>
       </c>
@@ -5209,7 +5264,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:45">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3339</v>
       </c>
@@ -5301,7 +5356,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:45">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3340</v>
       </c>
@@ -5393,7 +5448,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:45">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3341</v>
       </c>
@@ -5485,7 +5540,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:45">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3342</v>
       </c>
@@ -5577,7 +5632,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:45">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3343</v>
       </c>
@@ -5669,7 +5724,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:45">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -5767,19 +5822,19 @@
         <v>202</v>
       </c>
       <c r="AN48" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO48" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP48" t="s">
         <v>194</v>
       </c>
       <c r="AS48" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="49" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5877,19 +5932,19 @@
         <v>202</v>
       </c>
       <c r="AN49" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO49" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP49" t="s">
         <v>194</v>
       </c>
       <c r="AS49" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="50" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -5986,20 +6041,23 @@
       <c r="AI50" t="s">
         <v>202</v>
       </c>
+      <c r="AK50" t="s">
+        <v>250</v>
+      </c>
       <c r="AN50" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO50" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP50" t="s">
         <v>194</v>
       </c>
       <c r="AS50" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="51" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -6097,19 +6155,19 @@
         <v>202</v>
       </c>
       <c r="AN51" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO51" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP51" t="s">
         <v>194</v>
       </c>
       <c r="AS51" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="52" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -6207,19 +6265,19 @@
         <v>202</v>
       </c>
       <c r="AN52" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO52" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP52" t="s">
         <v>194</v>
       </c>
       <c r="AS52" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -6317,19 +6375,19 @@
         <v>202</v>
       </c>
       <c r="AN53" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO53" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP53" t="s">
         <v>194</v>
       </c>
       <c r="AS53" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="54" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -6427,19 +6485,19 @@
         <v>202</v>
       </c>
       <c r="AN54" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO54" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP54" t="s">
         <v>194</v>
       </c>
       <c r="AS54" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="55" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -6537,19 +6595,19 @@
         <v>202</v>
       </c>
       <c r="AN55" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO55" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP55" t="s">
         <v>194</v>
       </c>
       <c r="AS55" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="56" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -6647,19 +6705,19 @@
         <v>202</v>
       </c>
       <c r="AN56" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO56" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP56" t="s">
         <v>194</v>
       </c>
       <c r="AS56" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="57" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -6757,19 +6815,19 @@
         <v>202</v>
       </c>
       <c r="AN57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO57" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP57" t="s">
         <v>194</v>
       </c>
       <c r="AS57" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="58" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -6867,19 +6925,19 @@
         <v>202</v>
       </c>
       <c r="AN58" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO58" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP58" t="s">
         <v>194</v>
       </c>
       <c r="AS58" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="59" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -6977,19 +7035,19 @@
         <v>202</v>
       </c>
       <c r="AN59" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO59" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP59" t="s">
         <v>194</v>
       </c>
       <c r="AS59" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="60" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -7087,19 +7145,19 @@
         <v>202</v>
       </c>
       <c r="AN60" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO60" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP60" t="s">
         <v>194</v>
       </c>
       <c r="AS60" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -7197,19 +7255,19 @@
         <v>202</v>
       </c>
       <c r="AN61" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO61" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP61" t="s">
         <v>194</v>
       </c>
       <c r="AS61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="62" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -7307,19 +7365,19 @@
         <v>202</v>
       </c>
       <c r="AN62" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO62" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP62" t="s">
         <v>194</v>
       </c>
       <c r="AS62" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="63" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -7417,19 +7475,19 @@
         <v>202</v>
       </c>
       <c r="AN63" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO63" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP63" t="s">
         <v>194</v>
       </c>
       <c r="AS63" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="64" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -7527,19 +7585,19 @@
         <v>202</v>
       </c>
       <c r="AN64" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO64" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP64" t="s">
         <v>194</v>
       </c>
       <c r="AS64" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="65" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -7637,19 +7695,19 @@
         <v>202</v>
       </c>
       <c r="AN65" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO65" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP65" t="s">
         <v>194</v>
       </c>
       <c r="AS65" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -7747,19 +7805,19 @@
         <v>202</v>
       </c>
       <c r="AN66" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO66" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP66" t="s">
         <v>194</v>
       </c>
       <c r="AS66" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="67" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -7857,19 +7915,19 @@
         <v>202</v>
       </c>
       <c r="AN67" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO67" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP67" t="s">
         <v>194</v>
       </c>
       <c r="AS67" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="68" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -7967,19 +8025,19 @@
         <v>202</v>
       </c>
       <c r="AN68" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO68" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP68" t="s">
         <v>194</v>
       </c>
       <c r="AS68" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="69" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -8077,19 +8135,19 @@
         <v>202</v>
       </c>
       <c r="AN69" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO69" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP69" t="s">
         <v>194</v>
       </c>
       <c r="AS69" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="70" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -8187,19 +8245,19 @@
         <v>202</v>
       </c>
       <c r="AN70" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO70" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP70" t="s">
         <v>194</v>
       </c>
       <c r="AS70" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="71" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -8297,19 +8355,19 @@
         <v>202</v>
       </c>
       <c r="AN71" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO71" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP71" t="s">
         <v>194</v>
       </c>
       <c r="AS71" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="72" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -8407,19 +8465,19 @@
         <v>202</v>
       </c>
       <c r="AN72" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO72" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP72" t="s">
         <v>194</v>
       </c>
       <c r="AS72" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="73" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -8517,19 +8575,19 @@
         <v>202</v>
       </c>
       <c r="AN73" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO73" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP73" t="s">
         <v>194</v>
       </c>
       <c r="AS73" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="74" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -8627,19 +8685,19 @@
         <v>202</v>
       </c>
       <c r="AN74" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO74" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP74" t="s">
         <v>194</v>
       </c>
       <c r="AS74" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="75" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -8737,19 +8795,19 @@
         <v>202</v>
       </c>
       <c r="AN75" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO75" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP75" t="s">
         <v>194</v>
       </c>
       <c r="AS75" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="76" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -8847,19 +8905,19 @@
         <v>202</v>
       </c>
       <c r="AN76" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO76" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP76" t="s">
         <v>194</v>
       </c>
       <c r="AS76" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="77" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -8957,19 +9015,19 @@
         <v>202</v>
       </c>
       <c r="AN77" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO77" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP77" t="s">
         <v>194</v>
       </c>
       <c r="AS77" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="78" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -9067,19 +9125,19 @@
         <v>202</v>
       </c>
       <c r="AN78" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO78" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP78" t="s">
         <v>194</v>
       </c>
       <c r="AS78" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="79" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -9177,19 +9235,19 @@
         <v>202</v>
       </c>
       <c r="AN79" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO79" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP79" t="s">
         <v>194</v>
       </c>
       <c r="AS79" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="80" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -9287,19 +9345,19 @@
         <v>202</v>
       </c>
       <c r="AN80" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO80" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP80" t="s">
         <v>194</v>
       </c>
       <c r="AS80" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="81" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="81" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -9397,19 +9455,19 @@
         <v>202</v>
       </c>
       <c r="AN81" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO81" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP81" t="s">
         <v>194</v>
       </c>
       <c r="AS81" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="82" spans="1:45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="82" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -9507,115 +9565,115 @@
         <v>202</v>
       </c>
       <c r="AN82" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AO82" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AP82" t="s">
         <v>194</v>
       </c>
       <c r="AS82" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
-    <hyperlink ref="B77" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78"/>
-    <hyperlink ref="B80" r:id="rId79"/>
-    <hyperlink ref="B81" r:id="rId80"/>
-    <hyperlink ref="B82" r:id="rId81"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>253</v>
       </c>
@@ -9626,7 +9684,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9637,7 +9695,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -9648,7 +9706,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -9659,7 +9717,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -9670,7 +9728,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -9681,7 +9739,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -9692,7 +9750,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -9703,7 +9761,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -9714,7 +9772,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -9725,7 +9783,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -9736,7 +9794,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -9747,7 +9805,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -9758,7 +9816,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -9769,7 +9827,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -9780,7 +9838,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -9791,7 +9849,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -9802,7 +9860,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -9813,7 +9871,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -9824,7 +9882,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -9835,7 +9893,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -9846,7 +9904,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -9857,7 +9915,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -9868,7 +9926,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -9879,7 +9937,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -9890,7 +9948,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -9901,7 +9959,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -9912,7 +9970,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -9923,7 +9981,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -9934,7 +9992,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -9945,7 +10003,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -9956,7 +10014,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -9967,7 +10025,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -9978,7 +10036,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -9989,7 +10047,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -10000,7 +10058,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -10011,7 +10069,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -10022,7 +10080,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -10033,7 +10091,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -10044,7 +10102,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -10055,7 +10113,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -10066,7 +10124,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -10077,7 +10135,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -10088,7 +10146,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -10099,7 +10157,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -10110,7 +10168,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
modified dictionary structure in the sampling_description to determine if it works better with step2
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B1E522-405F-9B45-8E37-AFCE38E8CBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCB3D20-36BA-D741-8EE4-7605857C0BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="37300" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37300" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -932,7 +932,7 @@
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
   </si>
   <si>
-    <t>sample_vol_config:SyringeSampleVolume; pmtA: {voltage:PMTAhighVoltage,threshold:PMTAtriggerThreshold_DAQ_MCConly}; pmtB: {voltage:PMTBhighVoltage,threshold:PMTBtriggerThreshold_DAQ_MCConly}; pmtC: {voltage:PMTChighVoltage,threshold:PMTCtriggerThreshold_DAQ_MCConly}</t>
+    <t>sample_vol_config:{field:SyringeSampleVolume}; pmtA: {voltage_field:PMTAhighVoltage,threshold_field:PMTAtriggerThreshold_DAQ_MCConly}; pmtB: {voltage_field:PMTBhighVoltage,threshold_field:PMTBtriggerThreshold_DAQ_MCConly}; pmtC: {voltage_field:PMTChighVoltage,threshold_field:PMTCtriggerThreshold_DAQ_MCConly}</t>
   </si>
 </sst>
 </file>
@@ -1349,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF37" workbookViewId="0">
-      <selection activeCell="AV71" sqref="AV71"/>
+    <sheetView tabSelected="1" topLeftCell="AF34" workbookViewId="0">
+      <selection activeCell="AT43" sqref="AT43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Sampling_description column was modified to include imageResizeFactor, blobXgrowAmount and blobYgrowAmount
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B06A61E-5A60-974A-B51E-48AA38546852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D651E996-6A4B-E543-A862-F8FFC676156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34180" yWindow="80" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="900" windowWidth="38400" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -926,10 +926,10 @@
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
   </si>
   <si>
-    <t>sample_vol_config:{field:SyringeSampleVolume};pmtA_voltage:{field:PMTAhighVoltage};pmtA_threshold:{field:PMTAtriggerThreshold_DAQ_MCConly};pmtB_voltage: {field:PMTBhighVoltage};pmtB_threshold:{field:PMTBtriggerThreshold_DAQ_MCConly};pmtC_voltage:{field:PMTChighVoltage};pmtC_threshold:{field:PMTCtriggerThreshold_DAQ_MCConly}</t>
-  </si>
-  <si>
     <t>%Y%m%d %H:%M:%S</t>
+  </si>
+  <si>
+    <t>image_resize_factor:{field:imageResizeFactor};blob_x_grow:{field:blobXgrowAmount};blob_y_grow:{field:blobYgrowAmount};sample_vol_config:{field:SyringeSampleVolume};pmtA_voltage:{field:PMTAhighVoltage};pmtA_threshold:{field:PMTAtriggerThreshold_DAQ_MCConly};pmtB_voltage: {field:PMTBhighVoltage};pmtB_threshold:{field:PMTBtriggerThreshold_DAQ_MCConly};pmtC_voltage:{field:PMTChighVoltage};pmtC_threshold:{field:PMTCtriggerThreshold_DAQ_MCConly}</t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="AG82" sqref="AG82"/>
+    <sheetView tabSelected="1" topLeftCell="AF44" workbookViewId="0">
+      <selection activeCell="AV86" sqref="AV86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5772,7 +5772,7 @@
         <v>178</v>
       </c>
       <c r="T48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U48" t="s">
         <v>182</v>
@@ -5826,7 +5826,7 @@
         <v>196</v>
       </c>
       <c r="AS48" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.2">
@@ -5876,7 +5876,7 @@
         <v>178</v>
       </c>
       <c r="T49" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U49" t="s">
         <v>182</v>
@@ -5930,7 +5930,7 @@
         <v>196</v>
       </c>
       <c r="AS49" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.2">
@@ -5980,7 +5980,7 @@
         <v>178</v>
       </c>
       <c r="T50" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U50" t="s">
         <v>182</v>
@@ -6034,7 +6034,7 @@
         <v>196</v>
       </c>
       <c r="AS50" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.2">
@@ -6084,7 +6084,7 @@
         <v>178</v>
       </c>
       <c r="T51" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U51" t="s">
         <v>182</v>
@@ -6138,7 +6138,7 @@
         <v>196</v>
       </c>
       <c r="AS51" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.2">
@@ -6188,7 +6188,7 @@
         <v>178</v>
       </c>
       <c r="T52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U52" t="s">
         <v>182</v>
@@ -6242,7 +6242,7 @@
         <v>196</v>
       </c>
       <c r="AS52" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.2">
@@ -6292,7 +6292,7 @@
         <v>178</v>
       </c>
       <c r="T53" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U53" t="s">
         <v>182</v>
@@ -6346,7 +6346,7 @@
         <v>196</v>
       </c>
       <c r="AS53" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.2">
@@ -6396,7 +6396,7 @@
         <v>178</v>
       </c>
       <c r="T54" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U54" t="s">
         <v>182</v>
@@ -6450,7 +6450,7 @@
         <v>196</v>
       </c>
       <c r="AS54" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.2">
@@ -6500,7 +6500,7 @@
         <v>178</v>
       </c>
       <c r="T55" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U55" t="s">
         <v>182</v>
@@ -6554,7 +6554,7 @@
         <v>196</v>
       </c>
       <c r="AS55" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.2">
@@ -6604,7 +6604,7 @@
         <v>178</v>
       </c>
       <c r="T56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U56" t="s">
         <v>182</v>
@@ -6658,7 +6658,7 @@
         <v>196</v>
       </c>
       <c r="AS56" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.2">
@@ -6708,7 +6708,7 @@
         <v>178</v>
       </c>
       <c r="T57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U57" t="s">
         <v>182</v>
@@ -6762,7 +6762,7 @@
         <v>196</v>
       </c>
       <c r="AS57" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.2">
@@ -6812,7 +6812,7 @@
         <v>178</v>
       </c>
       <c r="T58" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U58" t="s">
         <v>182</v>
@@ -6866,7 +6866,7 @@
         <v>196</v>
       </c>
       <c r="AS58" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.2">
@@ -6916,7 +6916,7 @@
         <v>178</v>
       </c>
       <c r="T59" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U59" t="s">
         <v>182</v>
@@ -6970,7 +6970,7 @@
         <v>196</v>
       </c>
       <c r="AS59" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.2">
@@ -7020,7 +7020,7 @@
         <v>178</v>
       </c>
       <c r="T60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U60" t="s">
         <v>182</v>
@@ -7074,7 +7074,7 @@
         <v>196</v>
       </c>
       <c r="AS60" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.2">
@@ -7124,7 +7124,7 @@
         <v>178</v>
       </c>
       <c r="T61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U61" t="s">
         <v>182</v>
@@ -7178,7 +7178,7 @@
         <v>196</v>
       </c>
       <c r="AS61" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.2">
@@ -7228,7 +7228,7 @@
         <v>178</v>
       </c>
       <c r="T62" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U62" t="s">
         <v>182</v>
@@ -7282,7 +7282,7 @@
         <v>196</v>
       </c>
       <c r="AS62" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.2">
@@ -7332,7 +7332,7 @@
         <v>178</v>
       </c>
       <c r="T63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U63" t="s">
         <v>182</v>
@@ -7386,7 +7386,7 @@
         <v>196</v>
       </c>
       <c r="AS63" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.2">
@@ -7436,7 +7436,7 @@
         <v>178</v>
       </c>
       <c r="T64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U64" t="s">
         <v>182</v>
@@ -7490,7 +7490,7 @@
         <v>196</v>
       </c>
       <c r="AS64" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.2">
@@ -7540,7 +7540,7 @@
         <v>178</v>
       </c>
       <c r="T65" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U65" t="s">
         <v>182</v>
@@ -7594,7 +7594,7 @@
         <v>196</v>
       </c>
       <c r="AS65" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.2">
@@ -7644,7 +7644,7 @@
         <v>178</v>
       </c>
       <c r="T66" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U66" t="s">
         <v>182</v>
@@ -7698,7 +7698,7 @@
         <v>196</v>
       </c>
       <c r="AS66" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.2">
@@ -7748,7 +7748,7 @@
         <v>178</v>
       </c>
       <c r="T67" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U67" t="s">
         <v>182</v>
@@ -7802,7 +7802,7 @@
         <v>196</v>
       </c>
       <c r="AS67" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.2">
@@ -7852,7 +7852,7 @@
         <v>178</v>
       </c>
       <c r="T68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U68" t="s">
         <v>182</v>
@@ -7906,7 +7906,7 @@
         <v>196</v>
       </c>
       <c r="AS68" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.2">
@@ -7956,7 +7956,7 @@
         <v>178</v>
       </c>
       <c r="T69" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U69" t="s">
         <v>182</v>
@@ -8010,7 +8010,7 @@
         <v>196</v>
       </c>
       <c r="AS69" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.2">
@@ -8060,7 +8060,7 @@
         <v>178</v>
       </c>
       <c r="T70" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U70" t="s">
         <v>182</v>
@@ -8114,7 +8114,7 @@
         <v>196</v>
       </c>
       <c r="AS70" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.2">
@@ -8164,7 +8164,7 @@
         <v>178</v>
       </c>
       <c r="T71" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U71" t="s">
         <v>182</v>
@@ -8218,7 +8218,7 @@
         <v>196</v>
       </c>
       <c r="AS71" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.2">
@@ -8268,7 +8268,7 @@
         <v>178</v>
       </c>
       <c r="T72" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U72" t="s">
         <v>182</v>
@@ -8322,7 +8322,7 @@
         <v>196</v>
       </c>
       <c r="AS72" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.2">
@@ -8372,7 +8372,7 @@
         <v>178</v>
       </c>
       <c r="T73" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U73" t="s">
         <v>182</v>
@@ -8426,7 +8426,7 @@
         <v>196</v>
       </c>
       <c r="AS73" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.2">
@@ -8476,7 +8476,7 @@
         <v>178</v>
       </c>
       <c r="T74" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U74" t="s">
         <v>182</v>
@@ -8530,7 +8530,7 @@
         <v>196</v>
       </c>
       <c r="AS74" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.2">
@@ -8580,7 +8580,7 @@
         <v>178</v>
       </c>
       <c r="T75" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U75" t="s">
         <v>182</v>
@@ -8634,7 +8634,7 @@
         <v>196</v>
       </c>
       <c r="AS75" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.2">
@@ -8684,7 +8684,7 @@
         <v>178</v>
       </c>
       <c r="T76" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U76" t="s">
         <v>182</v>
@@ -8738,7 +8738,7 @@
         <v>196</v>
       </c>
       <c r="AS76" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.2">
@@ -8788,7 +8788,7 @@
         <v>178</v>
       </c>
       <c r="T77" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U77" t="s">
         <v>182</v>
@@ -8842,7 +8842,7 @@
         <v>196</v>
       </c>
       <c r="AS77" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.2">
@@ -8892,7 +8892,7 @@
         <v>178</v>
       </c>
       <c r="T78" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U78" t="s">
         <v>182</v>
@@ -8946,7 +8946,7 @@
         <v>196</v>
       </c>
       <c r="AS78" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.2">
@@ -8996,7 +8996,7 @@
         <v>178</v>
       </c>
       <c r="T79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U79" t="s">
         <v>182</v>
@@ -9050,7 +9050,7 @@
         <v>196</v>
       </c>
       <c r="AS79" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.2">
@@ -9100,7 +9100,7 @@
         <v>178</v>
       </c>
       <c r="T80" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U80" t="s">
         <v>182</v>
@@ -9154,7 +9154,7 @@
         <v>196</v>
       </c>
       <c r="AS80" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.2">
@@ -9204,7 +9204,7 @@
         <v>178</v>
       </c>
       <c r="T81" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U81" t="s">
         <v>182</v>
@@ -9258,7 +9258,7 @@
         <v>196</v>
       </c>
       <c r="AS81" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.2">
@@ -9308,7 +9308,7 @@
         <v>178</v>
       </c>
       <c r="T82" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U82" t="s">
         <v>182</v>
@@ -9362,7 +9362,7 @@
         <v>196</v>
       </c>
       <c r="AS82" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating spreadsheets with NA values id
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D651E996-6A4B-E543-A862-F8FFC676156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B93EA1-FCEB-3449-8B65-985757CE17BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="900" windowWidth="38400" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1346,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF44" workbookViewId="0">
-      <selection activeCell="AV86" sqref="AV86"/>
+    <sheetView tabSelected="1" topLeftCell="U44" workbookViewId="0">
+      <selection activeCell="AL65" sqref="AL65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5816,6 +5816,9 @@
       <c r="AI48" t="s">
         <v>201</v>
       </c>
+      <c r="AL48">
+        <v>-9999999</v>
+      </c>
       <c r="AN48" t="s">
         <v>249</v>
       </c>
@@ -5920,6 +5923,9 @@
       <c r="AI49" t="s">
         <v>201</v>
       </c>
+      <c r="AL49">
+        <v>-9999999</v>
+      </c>
       <c r="AN49" t="s">
         <v>249</v>
       </c>
@@ -6024,6 +6030,9 @@
       <c r="AI50" t="s">
         <v>201</v>
       </c>
+      <c r="AL50">
+        <v>-9999999</v>
+      </c>
       <c r="AN50" t="s">
         <v>249</v>
       </c>
@@ -6128,6 +6137,9 @@
       <c r="AI51" t="s">
         <v>201</v>
       </c>
+      <c r="AL51">
+        <v>-9999999</v>
+      </c>
       <c r="AN51" t="s">
         <v>249</v>
       </c>
@@ -6232,6 +6244,9 @@
       <c r="AI52" t="s">
         <v>201</v>
       </c>
+      <c r="AL52">
+        <v>-9999999</v>
+      </c>
       <c r="AN52" t="s">
         <v>249</v>
       </c>
@@ -6336,6 +6351,9 @@
       <c r="AI53" t="s">
         <v>201</v>
       </c>
+      <c r="AL53">
+        <v>-9999999</v>
+      </c>
       <c r="AN53" t="s">
         <v>249</v>
       </c>
@@ -6440,6 +6458,9 @@
       <c r="AI54" t="s">
         <v>201</v>
       </c>
+      <c r="AL54">
+        <v>-9999999</v>
+      </c>
       <c r="AN54" t="s">
         <v>249</v>
       </c>
@@ -6544,6 +6565,9 @@
       <c r="AI55" t="s">
         <v>201</v>
       </c>
+      <c r="AL55">
+        <v>-9999999</v>
+      </c>
       <c r="AN55" t="s">
         <v>249</v>
       </c>
@@ -6648,6 +6672,9 @@
       <c r="AI56" t="s">
         <v>201</v>
       </c>
+      <c r="AL56">
+        <v>-9999999</v>
+      </c>
       <c r="AN56" t="s">
         <v>249</v>
       </c>
@@ -6752,6 +6779,9 @@
       <c r="AI57" t="s">
         <v>201</v>
       </c>
+      <c r="AL57">
+        <v>-9999999</v>
+      </c>
       <c r="AN57" t="s">
         <v>249</v>
       </c>
@@ -6856,6 +6886,9 @@
       <c r="AI58" t="s">
         <v>201</v>
       </c>
+      <c r="AL58">
+        <v>-9999999</v>
+      </c>
       <c r="AN58" t="s">
         <v>249</v>
       </c>
@@ -6960,6 +6993,9 @@
       <c r="AI59" t="s">
         <v>201</v>
       </c>
+      <c r="AL59">
+        <v>-9999999</v>
+      </c>
       <c r="AN59" t="s">
         <v>249</v>
       </c>
@@ -7064,6 +7100,9 @@
       <c r="AI60" t="s">
         <v>201</v>
       </c>
+      <c r="AL60">
+        <v>-9999999</v>
+      </c>
       <c r="AN60" t="s">
         <v>249</v>
       </c>
@@ -7168,6 +7207,9 @@
       <c r="AI61" t="s">
         <v>201</v>
       </c>
+      <c r="AL61">
+        <v>-9999999</v>
+      </c>
       <c r="AN61" t="s">
         <v>249</v>
       </c>
@@ -7272,6 +7314,9 @@
       <c r="AI62" t="s">
         <v>201</v>
       </c>
+      <c r="AL62">
+        <v>-9999999</v>
+      </c>
       <c r="AN62" t="s">
         <v>249</v>
       </c>
@@ -7376,6 +7421,9 @@
       <c r="AI63" t="s">
         <v>201</v>
       </c>
+      <c r="AL63">
+        <v>-9999999</v>
+      </c>
       <c r="AN63" t="s">
         <v>249</v>
       </c>
@@ -7480,6 +7528,9 @@
       <c r="AI64" t="s">
         <v>201</v>
       </c>
+      <c r="AL64">
+        <v>-9999999</v>
+      </c>
       <c r="AN64" t="s">
         <v>249</v>
       </c>
@@ -7584,6 +7635,9 @@
       <c r="AI65" t="s">
         <v>201</v>
       </c>
+      <c r="AL65">
+        <v>-9999999</v>
+      </c>
       <c r="AN65" t="s">
         <v>249</v>
       </c>
@@ -7688,6 +7742,9 @@
       <c r="AI66" t="s">
         <v>201</v>
       </c>
+      <c r="AL66">
+        <v>-9999999</v>
+      </c>
       <c r="AN66" t="s">
         <v>249</v>
       </c>
@@ -7792,6 +7849,9 @@
       <c r="AI67" t="s">
         <v>201</v>
       </c>
+      <c r="AL67">
+        <v>-9999999</v>
+      </c>
       <c r="AN67" t="s">
         <v>249</v>
       </c>
@@ -7896,6 +7956,9 @@
       <c r="AI68" t="s">
         <v>201</v>
       </c>
+      <c r="AL68">
+        <v>-9999999</v>
+      </c>
       <c r="AN68" t="s">
         <v>249</v>
       </c>
@@ -8000,6 +8063,9 @@
       <c r="AI69" t="s">
         <v>201</v>
       </c>
+      <c r="AL69">
+        <v>-9999999</v>
+      </c>
       <c r="AN69" t="s">
         <v>249</v>
       </c>
@@ -8104,6 +8170,9 @@
       <c r="AI70" t="s">
         <v>201</v>
       </c>
+      <c r="AL70">
+        <v>-9999999</v>
+      </c>
       <c r="AN70" t="s">
         <v>249</v>
       </c>
@@ -8208,6 +8277,9 @@
       <c r="AI71" t="s">
         <v>201</v>
       </c>
+      <c r="AL71">
+        <v>-9999999</v>
+      </c>
       <c r="AN71" t="s">
         <v>249</v>
       </c>
@@ -8312,6 +8384,9 @@
       <c r="AI72" t="s">
         <v>201</v>
       </c>
+      <c r="AL72">
+        <v>-9999999</v>
+      </c>
       <c r="AN72" t="s">
         <v>249</v>
       </c>
@@ -8416,6 +8491,9 @@
       <c r="AI73" t="s">
         <v>201</v>
       </c>
+      <c r="AL73">
+        <v>-9999999</v>
+      </c>
       <c r="AN73" t="s">
         <v>249</v>
       </c>
@@ -8520,6 +8598,9 @@
       <c r="AI74" t="s">
         <v>201</v>
       </c>
+      <c r="AL74">
+        <v>-9999999</v>
+      </c>
       <c r="AN74" t="s">
         <v>249</v>
       </c>
@@ -8624,6 +8705,9 @@
       <c r="AI75" t="s">
         <v>201</v>
       </c>
+      <c r="AL75">
+        <v>-9999999</v>
+      </c>
       <c r="AN75" t="s">
         <v>249</v>
       </c>
@@ -8728,6 +8812,9 @@
       <c r="AI76" t="s">
         <v>201</v>
       </c>
+      <c r="AL76">
+        <v>-9999999</v>
+      </c>
       <c r="AN76" t="s">
         <v>249</v>
       </c>
@@ -8832,6 +8919,9 @@
       <c r="AI77" t="s">
         <v>201</v>
       </c>
+      <c r="AL77">
+        <v>-9999999</v>
+      </c>
       <c r="AN77" t="s">
         <v>249</v>
       </c>
@@ -8936,6 +9026,9 @@
       <c r="AI78" t="s">
         <v>201</v>
       </c>
+      <c r="AL78">
+        <v>-9999999</v>
+      </c>
       <c r="AN78" t="s">
         <v>249</v>
       </c>
@@ -9040,6 +9133,9 @@
       <c r="AI79" t="s">
         <v>201</v>
       </c>
+      <c r="AL79">
+        <v>-9999999</v>
+      </c>
       <c r="AN79" t="s">
         <v>249</v>
       </c>
@@ -9144,6 +9240,9 @@
       <c r="AI80" t="s">
         <v>201</v>
       </c>
+      <c r="AL80">
+        <v>-9999999</v>
+      </c>
       <c r="AN80" t="s">
         <v>249</v>
       </c>
@@ -9248,6 +9347,9 @@
       <c r="AI81" t="s">
         <v>201</v>
       </c>
+      <c r="AL81">
+        <v>-9999999</v>
+      </c>
       <c r="AN81" t="s">
         <v>249</v>
       </c>
@@ -9351,6 +9453,9 @@
       </c>
       <c r="AI82" t="s">
         <v>201</v>
+      </c>
+      <c r="AL82">
+        <v>-9999999</v>
       </c>
       <c r="AN82" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
Updated standardization for IFCB proejcts ok
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -11250,7 +11250,11 @@
         </is>
       </c>
       <c r="AJ64" t="inlineStr"/>
-      <c r="AK64" t="inlineStr"/>
+      <c r="AK64" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/IFCB_dashboard_downloads/project_EXPORTS_flags.csv</t>
+        </is>
+      </c>
       <c r="AL64" t="n">
         <v>-9999999</v>
       </c>

</xml_diff>

<commit_message>
Last flag ok. Pushing for standardization on server
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -12381,7 +12381,11 @@
         </is>
       </c>
       <c r="AJ69" t="inlineStr"/>
-      <c r="AK69" t="inlineStr"/>
+      <c r="AK69" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/IFCB_dashboard_downloads/project_NESLTER_transect_flags.csv</t>
+        </is>
+      </c>
       <c r="AL69" t="n">
         <v>-9999999</v>
       </c>
@@ -12936,7 +12940,11 @@
         </is>
       </c>
       <c r="AJ72" t="inlineStr"/>
-      <c r="AK72" t="inlineStr"/>
+      <c r="AK72" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/IFCB_dashboard_downloads/project_arctic_flags.csv</t>
+        </is>
+      </c>
       <c r="AL72" t="n">
         <v>-9999999</v>
       </c>
@@ -13306,7 +13314,11 @@
         </is>
       </c>
       <c r="AJ74" t="inlineStr"/>
-      <c r="AK74" t="inlineStr"/>
+      <c r="AK74" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/IFCB_dashboard_downloads/project_NESLTER_broadscale_flags.csv</t>
+        </is>
+      </c>
       <c r="AL74" t="n">
         <v>-9999999</v>
       </c>

</xml_diff>

<commit_message>
Adding custom unit def
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FCE7F5-E6CD-E647-939E-8684AF6F6A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B48BE4-3B46-8D44-A58A-6B97F4045CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34380" yWindow="580" windowWidth="29140" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1388,7 +1388,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="V45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA62" sqref="AA62:AE62"/>
+      <selection pane="bottomRight" activeCell="AH60" sqref="AH60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Re-running QC on arctic and WHOI dock IFCB projects
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,11 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -43,12 +48,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -76,12 +96,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -494,227 +517,227 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Project_ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Project_source</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Project_localpath</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Instrument</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Cruise_field</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Station_field</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Profile_field</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Sample_field</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Latitude_field</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Latitude_unit</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>Longitude_field</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>Longitude_unit</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>Depth_min_field</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>Depth_min_unit</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>Depth_max_field</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>Depth_max_unit</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>Sampling_date_field</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>Sampling_date_format</t>
         </is>
       </c>
-      <c r="S1" s="2" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>Sampling_time_field</t>
         </is>
       </c>
-      <c r="T1" s="2" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>Sampling_time_format</t>
         </is>
       </c>
-      <c r="U1" s="2" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>Volume_analyzed_field</t>
         </is>
       </c>
-      <c r="V1" s="2" t="inlineStr">
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>Volume_analyzed_unit</t>
         </is>
       </c>
-      <c r="W1" s="2" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>Dilution_field</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="X1" s="3" t="inlineStr">
         <is>
           <t>ROI_field</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>ESD_field</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>ESD_unit</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AA1" s="3" t="inlineStr">
         <is>
           <t>Biovolume_field</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AB1" s="3" t="inlineStr">
         <is>
           <t>Biovolume_unit</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AC1" s="3" t="inlineStr">
         <is>
           <t>Area_field</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AD1" s="3" t="inlineStr">
         <is>
           <t>Area_unit</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AE1" s="3" t="inlineStr">
         <is>
           <t>Minor_axis_field</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AF1" s="3" t="inlineStr">
         <is>
           <t>Minor_axis_unit</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AG1" s="3" t="inlineStr">
         <is>
           <t>Pixel_field</t>
         </is>
       </c>
-      <c r="AH1" s="2" t="inlineStr">
+      <c r="AH1" s="3" t="inlineStr">
         <is>
           <t>Pixel_unit</t>
         </is>
       </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="AI1" s="3" t="inlineStr">
         <is>
           <t>Category_field</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
+      <c r="AJ1" s="3" t="inlineStr">
         <is>
           <t>Annotation_field</t>
         </is>
       </c>
-      <c r="AK1" s="2" t="inlineStr">
+      <c r="AK1" s="3" t="inlineStr">
         <is>
           <t>Flag_path</t>
         </is>
       </c>
-      <c r="AL1" s="2" t="inlineStr">
+      <c r="AL1" s="3" t="inlineStr">
         <is>
           <t>NA_value</t>
         </is>
       </c>
-      <c r="AM1" s="2" t="inlineStr">
+      <c r="AM1" s="3" t="inlineStr">
         <is>
           <t>External_project</t>
         </is>
       </c>
-      <c r="AN1" s="2" t="inlineStr">
+      <c r="AN1" s="3" t="inlineStr">
         <is>
           <t>Sampling_type_field</t>
         </is>
       </c>
-      <c r="AO1" s="2" t="inlineStr">
+      <c r="AO1" s="3" t="inlineStr">
         <is>
           <t>Sampling_lower_size_field</t>
         </is>
       </c>
-      <c r="AP1" s="2" t="inlineStr">
+      <c r="AP1" s="3" t="inlineStr">
         <is>
           <t>Sampling_lower_size_unit</t>
         </is>
       </c>
-      <c r="AQ1" s="2" t="inlineStr">
+      <c r="AQ1" s="3" t="inlineStr">
         <is>
           <t>Sampling_upper_size_field</t>
         </is>
       </c>
-      <c r="AR1" s="2" t="inlineStr">
+      <c r="AR1" s="3" t="inlineStr">
         <is>
           <t>Sampling_upper_size_unit</t>
         </is>
       </c>
-      <c r="AS1" s="2" t="inlineStr">
+      <c r="AS1" s="3" t="inlineStr">
         <is>
           <t>Sampling_description</t>
         </is>

</xml_diff>

<commit_message>
changed IFCB dashboard pixel area to summed_area
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4214/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FF4400-D312-9A49-8570-121AA276E237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029B87D8-C7E1-444D-96D2-30893F80C355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39680" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="2720" windowWidth="51200" windowHeight="27300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1382,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z87" sqref="Z87"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7438,7 +7438,7 @@
         <v>62</v>
       </c>
       <c r="AC64" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="AD64" t="s">
         <v>64</v>
@@ -7946,7 +7946,7 @@
         <v>62</v>
       </c>
       <c r="AC69" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="AD69" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Updating standardizer pixel size units
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A5E06A-3832-354D-B3C5-AE6FBC9CE0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AB69B2-B3B9-5B49-AE7B-4F5D6F0D28BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -570,9 +570,6 @@
     <t>pixel_to_micron</t>
   </si>
   <si>
-    <t>micrometer_per_pixel</t>
-  </si>
-  <si>
     <t>class_1</t>
   </si>
   <si>
@@ -973,6 +970,9 @@
   </si>
   <si>
     <t>~/GIT/PSSdb/raw/flags/IFCB_dashboard_downloads/project_san-francisco-pier-17_flags.csv</t>
+  </si>
+  <si>
+    <t>pixel_per_micrometer</t>
   </si>
 </sst>
 </file>
@@ -1364,11 +1364,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U26" workbookViewId="0">
-      <selection activeCell="AK49" sqref="AK49"/>
+    <sheetView tabSelected="1" topLeftCell="AG39" workbookViewId="0">
+      <selection activeCell="AN68" sqref="AN68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -5819,33 +5823,33 @@
         <v>177</v>
       </c>
       <c r="AH48" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI48" t="s">
         <v>178</v>
       </c>
-      <c r="AI48" t="s">
-        <v>179</v>
-      </c>
       <c r="AK48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AL48">
         <v>-9999999</v>
       </c>
       <c r="AO48" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP48" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS48" t="s">
         <v>180</v>
-      </c>
-      <c r="AP48" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS48" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" t="s">
         <v>182</v>
-      </c>
-      <c r="B49" t="s">
-        <v>183</v>
       </c>
       <c r="C49" t="s">
         <v>164</v>
@@ -5920,33 +5924,33 @@
         <v>177</v>
       </c>
       <c r="AH49" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI49" t="s">
         <v>178</v>
       </c>
-      <c r="AI49" t="s">
-        <v>179</v>
-      </c>
       <c r="AK49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AL49">
         <v>-9999999</v>
       </c>
       <c r="AO49" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS49" t="s">
         <v>180</v>
-      </c>
-      <c r="AP49" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS49" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s">
         <v>185</v>
-      </c>
-      <c r="B50" t="s">
-        <v>186</v>
       </c>
       <c r="C50" t="s">
         <v>164</v>
@@ -5955,7 +5959,7 @@
         <v>47</v>
       </c>
       <c r="E50" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H50" t="s">
         <v>49</v>
@@ -6000,19 +6004,19 @@
         <v>173</v>
       </c>
       <c r="AA50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB50" t="s">
         <v>62</v>
       </c>
       <c r="AC50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD50" t="s">
         <v>64</v>
       </c>
       <c r="AE50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF50" t="s">
         <v>66</v>
@@ -6021,33 +6025,33 @@
         <v>177</v>
       </c>
       <c r="AH50" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI50" t="s">
         <v>178</v>
-      </c>
-      <c r="AI50" t="s">
-        <v>179</v>
       </c>
       <c r="AL50">
         <v>-9999999</v>
       </c>
       <c r="AN50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO50" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP50" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS50" t="s">
         <v>180</v>
-      </c>
-      <c r="AP50" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS50" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" t="s">
         <v>191</v>
-      </c>
-      <c r="B51" t="s">
-        <v>192</v>
       </c>
       <c r="C51" t="s">
         <v>164</v>
@@ -6056,7 +6060,7 @@
         <v>47</v>
       </c>
       <c r="E51" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H51" t="s">
         <v>49</v>
@@ -6101,19 +6105,19 @@
         <v>173</v>
       </c>
       <c r="AA51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB51" t="s">
         <v>62</v>
       </c>
       <c r="AC51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD51" t="s">
         <v>64</v>
       </c>
       <c r="AE51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF51" t="s">
         <v>66</v>
@@ -6122,33 +6126,33 @@
         <v>177</v>
       </c>
       <c r="AH51" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI51" t="s">
         <v>178</v>
-      </c>
-      <c r="AI51" t="s">
-        <v>179</v>
       </c>
       <c r="AL51">
         <v>-9999999</v>
       </c>
       <c r="AN51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO51" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP51" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS51" t="s">
         <v>180</v>
-      </c>
-      <c r="AP51" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS51" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>192</v>
+      </c>
+      <c r="B52" t="s">
         <v>193</v>
-      </c>
-      <c r="B52" t="s">
-        <v>194</v>
       </c>
       <c r="C52" t="s">
         <v>164</v>
@@ -6157,7 +6161,7 @@
         <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H52" t="s">
         <v>49</v>
@@ -6202,19 +6206,19 @@
         <v>173</v>
       </c>
       <c r="AA52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB52" t="s">
         <v>62</v>
       </c>
       <c r="AC52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD52" t="s">
         <v>64</v>
       </c>
       <c r="AE52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF52" t="s">
         <v>66</v>
@@ -6223,33 +6227,33 @@
         <v>177</v>
       </c>
       <c r="AH52" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI52" t="s">
         <v>178</v>
-      </c>
-      <c r="AI52" t="s">
-        <v>179</v>
       </c>
       <c r="AL52">
         <v>-9999999</v>
       </c>
       <c r="AN52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO52" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP52" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS52" t="s">
         <v>180</v>
-      </c>
-      <c r="AP52" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS52" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" t="s">
         <v>195</v>
-      </c>
-      <c r="B53" t="s">
-        <v>196</v>
       </c>
       <c r="C53" t="s">
         <v>164</v>
@@ -6258,7 +6262,7 @@
         <v>47</v>
       </c>
       <c r="E53" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H53" t="s">
         <v>49</v>
@@ -6303,19 +6307,19 @@
         <v>173</v>
       </c>
       <c r="AA53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB53" t="s">
         <v>62</v>
       </c>
       <c r="AC53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD53" t="s">
         <v>64</v>
       </c>
       <c r="AE53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF53" t="s">
         <v>66</v>
@@ -6324,33 +6328,33 @@
         <v>177</v>
       </c>
       <c r="AH53" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI53" t="s">
         <v>178</v>
-      </c>
-      <c r="AI53" t="s">
-        <v>179</v>
       </c>
       <c r="AL53">
         <v>-9999999</v>
       </c>
       <c r="AN53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO53" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP53" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS53" t="s">
         <v>180</v>
-      </c>
-      <c r="AP53" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS53" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" t="s">
         <v>197</v>
-      </c>
-      <c r="B54" t="s">
-        <v>198</v>
       </c>
       <c r="C54" t="s">
         <v>164</v>
@@ -6359,7 +6363,7 @@
         <v>47</v>
       </c>
       <c r="E54" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H54" t="s">
         <v>49</v>
@@ -6404,19 +6408,19 @@
         <v>173</v>
       </c>
       <c r="AA54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB54" t="s">
         <v>62</v>
       </c>
       <c r="AC54" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD54" t="s">
         <v>64</v>
       </c>
       <c r="AE54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF54" t="s">
         <v>66</v>
@@ -6425,33 +6429,33 @@
         <v>177</v>
       </c>
       <c r="AH54" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI54" t="s">
         <v>178</v>
-      </c>
-      <c r="AI54" t="s">
-        <v>179</v>
       </c>
       <c r="AL54">
         <v>-9999999</v>
       </c>
       <c r="AN54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO54" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP54" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS54" t="s">
         <v>180</v>
-      </c>
-      <c r="AP54" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS54" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>198</v>
+      </c>
+      <c r="B55" t="s">
         <v>199</v>
-      </c>
-      <c r="B55" t="s">
-        <v>200</v>
       </c>
       <c r="C55" t="s">
         <v>164</v>
@@ -6460,7 +6464,7 @@
         <v>47</v>
       </c>
       <c r="E55" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H55" t="s">
         <v>49</v>
@@ -6505,19 +6509,19 @@
         <v>173</v>
       </c>
       <c r="AA55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB55" t="s">
         <v>62</v>
       </c>
       <c r="AC55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD55" t="s">
         <v>64</v>
       </c>
       <c r="AE55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF55" t="s">
         <v>66</v>
@@ -6526,33 +6530,33 @@
         <v>177</v>
       </c>
       <c r="AH55" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI55" t="s">
         <v>178</v>
-      </c>
-      <c r="AI55" t="s">
-        <v>179</v>
       </c>
       <c r="AL55">
         <v>-9999999</v>
       </c>
       <c r="AN55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO55" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS55" t="s">
         <v>180</v>
-      </c>
-      <c r="AP55" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS55" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" t="s">
         <v>201</v>
-      </c>
-      <c r="B56" t="s">
-        <v>202</v>
       </c>
       <c r="C56" t="s">
         <v>164</v>
@@ -6561,7 +6565,7 @@
         <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H56" t="s">
         <v>49</v>
@@ -6606,19 +6610,19 @@
         <v>173</v>
       </c>
       <c r="AA56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB56" t="s">
         <v>62</v>
       </c>
       <c r="AC56" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD56" t="s">
         <v>64</v>
       </c>
       <c r="AE56" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF56" t="s">
         <v>66</v>
@@ -6627,33 +6631,33 @@
         <v>177</v>
       </c>
       <c r="AH56" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI56" t="s">
         <v>178</v>
-      </c>
-      <c r="AI56" t="s">
-        <v>179</v>
       </c>
       <c r="AL56">
         <v>-9999999</v>
       </c>
       <c r="AN56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO56" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP56" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS56" t="s">
         <v>180</v>
-      </c>
-      <c r="AP56" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS56" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>202</v>
+      </c>
+      <c r="B57" t="s">
         <v>203</v>
-      </c>
-      <c r="B57" t="s">
-        <v>204</v>
       </c>
       <c r="C57" t="s">
         <v>164</v>
@@ -6662,7 +6666,7 @@
         <v>47</v>
       </c>
       <c r="E57" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H57" t="s">
         <v>49</v>
@@ -6707,19 +6711,19 @@
         <v>173</v>
       </c>
       <c r="AA57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB57" t="s">
         <v>62</v>
       </c>
       <c r="AC57" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD57" t="s">
         <v>64</v>
       </c>
       <c r="AE57" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF57" t="s">
         <v>66</v>
@@ -6728,33 +6732,33 @@
         <v>177</v>
       </c>
       <c r="AH57" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI57" t="s">
         <v>178</v>
-      </c>
-      <c r="AI57" t="s">
-        <v>179</v>
       </c>
       <c r="AL57">
         <v>-9999999</v>
       </c>
       <c r="AN57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO57" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP57" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS57" t="s">
         <v>180</v>
-      </c>
-      <c r="AP57" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS57" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" t="s">
         <v>205</v>
-      </c>
-      <c r="B58" t="s">
-        <v>206</v>
       </c>
       <c r="C58" t="s">
         <v>164</v>
@@ -6763,7 +6767,7 @@
         <v>47</v>
       </c>
       <c r="E58" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H58" t="s">
         <v>49</v>
@@ -6808,19 +6812,19 @@
         <v>173</v>
       </c>
       <c r="AA58" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB58" t="s">
         <v>62</v>
       </c>
       <c r="AC58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD58" t="s">
         <v>64</v>
       </c>
       <c r="AE58" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF58" t="s">
         <v>66</v>
@@ -6829,33 +6833,33 @@
         <v>177</v>
       </c>
       <c r="AH58" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI58" t="s">
         <v>178</v>
-      </c>
-      <c r="AI58" t="s">
-        <v>179</v>
       </c>
       <c r="AL58">
         <v>-9999999</v>
       </c>
       <c r="AN58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO58" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP58" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS58" t="s">
         <v>180</v>
-      </c>
-      <c r="AP58" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS58" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" t="s">
         <v>207</v>
-      </c>
-      <c r="B59" t="s">
-        <v>208</v>
       </c>
       <c r="C59" t="s">
         <v>164</v>
@@ -6864,7 +6868,7 @@
         <v>47</v>
       </c>
       <c r="E59" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H59" t="s">
         <v>49</v>
@@ -6909,19 +6913,19 @@
         <v>173</v>
       </c>
       <c r="AA59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB59" t="s">
         <v>62</v>
       </c>
       <c r="AC59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD59" t="s">
         <v>64</v>
       </c>
       <c r="AE59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF59" t="s">
         <v>66</v>
@@ -6930,33 +6934,33 @@
         <v>177</v>
       </c>
       <c r="AH59" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI59" t="s">
         <v>178</v>
-      </c>
-      <c r="AI59" t="s">
-        <v>179</v>
       </c>
       <c r="AL59">
         <v>-9999999</v>
       </c>
       <c r="AN59" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO59" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP59" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS59" t="s">
         <v>180</v>
-      </c>
-      <c r="AP59" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS59" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>208</v>
+      </c>
+      <c r="B60" t="s">
         <v>209</v>
-      </c>
-      <c r="B60" t="s">
-        <v>210</v>
       </c>
       <c r="C60" t="s">
         <v>164</v>
@@ -6965,7 +6969,7 @@
         <v>47</v>
       </c>
       <c r="E60" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H60" t="s">
         <v>49</v>
@@ -7010,19 +7014,19 @@
         <v>173</v>
       </c>
       <c r="AA60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB60" t="s">
         <v>62</v>
       </c>
       <c r="AC60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD60" t="s">
         <v>64</v>
       </c>
       <c r="AE60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF60" t="s">
         <v>66</v>
@@ -7031,33 +7035,33 @@
         <v>177</v>
       </c>
       <c r="AH60" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI60" t="s">
         <v>178</v>
-      </c>
-      <c r="AI60" t="s">
-        <v>179</v>
       </c>
       <c r="AL60">
         <v>-9999999</v>
       </c>
       <c r="AN60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO60" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP60" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS60" t="s">
         <v>180</v>
-      </c>
-      <c r="AP60" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS60" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" t="s">
         <v>211</v>
-      </c>
-      <c r="B61" t="s">
-        <v>212</v>
       </c>
       <c r="C61" t="s">
         <v>164</v>
@@ -7066,7 +7070,7 @@
         <v>47</v>
       </c>
       <c r="E61" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H61" t="s">
         <v>49</v>
@@ -7111,19 +7115,19 @@
         <v>173</v>
       </c>
       <c r="AA61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB61" t="s">
         <v>62</v>
       </c>
       <c r="AC61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD61" t="s">
         <v>64</v>
       </c>
       <c r="AE61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF61" t="s">
         <v>66</v>
@@ -7132,33 +7136,33 @@
         <v>177</v>
       </c>
       <c r="AH61" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI61" t="s">
         <v>178</v>
-      </c>
-      <c r="AI61" t="s">
-        <v>179</v>
       </c>
       <c r="AL61">
         <v>-9999999</v>
       </c>
       <c r="AN61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO61" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP61" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS61" t="s">
         <v>180</v>
-      </c>
-      <c r="AP61" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS61" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>212</v>
+      </c>
+      <c r="B62" t="s">
         <v>213</v>
-      </c>
-      <c r="B62" t="s">
-        <v>214</v>
       </c>
       <c r="C62" t="s">
         <v>164</v>
@@ -7167,7 +7171,7 @@
         <v>47</v>
       </c>
       <c r="E62" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H62" t="s">
         <v>49</v>
@@ -7233,36 +7237,36 @@
         <v>177</v>
       </c>
       <c r="AH62" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI62" t="s">
         <v>178</v>
       </c>
-      <c r="AI62" t="s">
-        <v>179</v>
-      </c>
       <c r="AK62" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AL62">
         <v>-9999999</v>
       </c>
       <c r="AN62" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO62" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP62" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS62" t="s">
         <v>180</v>
-      </c>
-      <c r="AP62" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS62" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" t="s">
         <v>216</v>
-      </c>
-      <c r="B63" t="s">
-        <v>217</v>
       </c>
       <c r="C63" t="s">
         <v>164</v>
@@ -7271,7 +7275,7 @@
         <v>47</v>
       </c>
       <c r="E63" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H63" t="s">
         <v>49</v>
@@ -7316,19 +7320,19 @@
         <v>173</v>
       </c>
       <c r="AA63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB63" t="s">
         <v>62</v>
       </c>
       <c r="AC63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD63" t="s">
         <v>64</v>
       </c>
       <c r="AE63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF63" t="s">
         <v>66</v>
@@ -7337,33 +7341,33 @@
         <v>177</v>
       </c>
       <c r="AH63" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI63" t="s">
         <v>178</v>
-      </c>
-      <c r="AI63" t="s">
-        <v>179</v>
       </c>
       <c r="AL63">
         <v>-9999999</v>
       </c>
       <c r="AN63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO63" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP63" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS63" t="s">
         <v>180</v>
-      </c>
-      <c r="AP63" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS63" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" t="s">
         <v>218</v>
-      </c>
-      <c r="B64" t="s">
-        <v>219</v>
       </c>
       <c r="C64" t="s">
         <v>164</v>
@@ -7372,7 +7376,7 @@
         <v>47</v>
       </c>
       <c r="E64" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H64" t="s">
         <v>49</v>
@@ -7417,7 +7421,7 @@
         <v>173</v>
       </c>
       <c r="AA64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB64" t="s">
         <v>62</v>
@@ -7429,7 +7433,7 @@
         <v>64</v>
       </c>
       <c r="AE64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF64" t="s">
         <v>66</v>
@@ -7438,36 +7442,36 @@
         <v>177</v>
       </c>
       <c r="AH64" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI64" t="s">
         <v>178</v>
       </c>
-      <c r="AI64" t="s">
-        <v>179</v>
-      </c>
       <c r="AK64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AL64">
         <v>-9999999</v>
       </c>
       <c r="AN64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO64" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP64" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS64" t="s">
         <v>180</v>
-      </c>
-      <c r="AP64" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS64" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" t="s">
         <v>221</v>
-      </c>
-      <c r="B65" t="s">
-        <v>222</v>
       </c>
       <c r="C65" t="s">
         <v>164</v>
@@ -7476,7 +7480,7 @@
         <v>47</v>
       </c>
       <c r="E65" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H65" t="s">
         <v>49</v>
@@ -7521,19 +7525,19 @@
         <v>173</v>
       </c>
       <c r="AA65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB65" t="s">
         <v>62</v>
       </c>
       <c r="AC65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD65" t="s">
         <v>64</v>
       </c>
       <c r="AE65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF65" t="s">
         <v>66</v>
@@ -7542,33 +7546,33 @@
         <v>177</v>
       </c>
       <c r="AH65" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI65" t="s">
         <v>178</v>
-      </c>
-      <c r="AI65" t="s">
-        <v>179</v>
       </c>
       <c r="AL65">
         <v>-9999999</v>
       </c>
       <c r="AN65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO65" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP65" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS65" t="s">
         <v>180</v>
-      </c>
-      <c r="AP65" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS65" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B66" t="s">
         <v>223</v>
-      </c>
-      <c r="B66" t="s">
-        <v>224</v>
       </c>
       <c r="C66" t="s">
         <v>164</v>
@@ -7577,7 +7581,7 @@
         <v>47</v>
       </c>
       <c r="E66" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H66" t="s">
         <v>49</v>
@@ -7622,19 +7626,19 @@
         <v>173</v>
       </c>
       <c r="AA66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB66" t="s">
         <v>62</v>
       </c>
       <c r="AC66" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD66" t="s">
         <v>64</v>
       </c>
       <c r="AE66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF66" t="s">
         <v>66</v>
@@ -7643,33 +7647,33 @@
         <v>177</v>
       </c>
       <c r="AH66" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI66" t="s">
         <v>178</v>
-      </c>
-      <c r="AI66" t="s">
-        <v>179</v>
       </c>
       <c r="AL66">
         <v>-9999999</v>
       </c>
       <c r="AN66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO66" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP66" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS66" t="s">
         <v>180</v>
-      </c>
-      <c r="AP66" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS66" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>224</v>
+      </c>
+      <c r="B67" t="s">
         <v>225</v>
-      </c>
-      <c r="B67" t="s">
-        <v>226</v>
       </c>
       <c r="C67" t="s">
         <v>164</v>
@@ -7678,7 +7682,7 @@
         <v>47</v>
       </c>
       <c r="E67" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H67" t="s">
         <v>49</v>
@@ -7723,19 +7727,19 @@
         <v>173</v>
       </c>
       <c r="AA67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB67" t="s">
         <v>62</v>
       </c>
       <c r="AC67" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD67" t="s">
         <v>64</v>
       </c>
       <c r="AE67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF67" t="s">
         <v>66</v>
@@ -7744,33 +7748,33 @@
         <v>177</v>
       </c>
       <c r="AH67" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI67" t="s">
         <v>178</v>
-      </c>
-      <c r="AI67" t="s">
-        <v>179</v>
       </c>
       <c r="AL67">
         <v>-9999999</v>
       </c>
       <c r="AN67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO67" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP67" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS67" t="s">
         <v>180</v>
-      </c>
-      <c r="AP67" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS67" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>226</v>
+      </c>
+      <c r="B68" t="s">
         <v>227</v>
-      </c>
-      <c r="B68" t="s">
-        <v>228</v>
       </c>
       <c r="C68" t="s">
         <v>164</v>
@@ -7779,7 +7783,7 @@
         <v>47</v>
       </c>
       <c r="E68" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H68" t="s">
         <v>49</v>
@@ -7845,33 +7849,30 @@
         <v>177</v>
       </c>
       <c r="AH68" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI68" t="s">
         <v>178</v>
-      </c>
-      <c r="AI68" t="s">
-        <v>179</v>
       </c>
       <c r="AL68">
         <v>-9999999</v>
       </c>
-      <c r="AN68" t="s">
-        <v>190</v>
-      </c>
       <c r="AO68" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP68" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS68" t="s">
         <v>180</v>
-      </c>
-      <c r="AP68" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS68" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>228</v>
+      </c>
+      <c r="B69" t="s">
         <v>229</v>
-      </c>
-      <c r="B69" t="s">
-        <v>230</v>
       </c>
       <c r="C69" t="s">
         <v>164</v>
@@ -7925,7 +7926,7 @@
         <v>173</v>
       </c>
       <c r="AA69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB69" t="s">
         <v>62</v>
@@ -7937,7 +7938,7 @@
         <v>64</v>
       </c>
       <c r="AE69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF69" t="s">
         <v>66</v>
@@ -7946,36 +7947,36 @@
         <v>177</v>
       </c>
       <c r="AH69" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI69" t="s">
         <v>178</v>
       </c>
-      <c r="AI69" t="s">
-        <v>179</v>
-      </c>
       <c r="AK69" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AL69">
         <v>-9999999</v>
       </c>
       <c r="AN69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO69" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP69" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS69" t="s">
         <v>180</v>
-      </c>
-      <c r="AP69" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS69" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" t="s">
         <v>232</v>
-      </c>
-      <c r="B70" t="s">
-        <v>233</v>
       </c>
       <c r="C70" t="s">
         <v>164</v>
@@ -7984,7 +7985,7 @@
         <v>47</v>
       </c>
       <c r="E70" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H70" t="s">
         <v>49</v>
@@ -8029,19 +8030,19 @@
         <v>173</v>
       </c>
       <c r="AA70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB70" t="s">
         <v>62</v>
       </c>
       <c r="AC70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD70" t="s">
         <v>64</v>
       </c>
       <c r="AE70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF70" t="s">
         <v>66</v>
@@ -8050,33 +8051,33 @@
         <v>177</v>
       </c>
       <c r="AH70" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI70" t="s">
         <v>178</v>
-      </c>
-      <c r="AI70" t="s">
-        <v>179</v>
       </c>
       <c r="AL70">
         <v>-9999999</v>
       </c>
       <c r="AN70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO70" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP70" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS70" t="s">
         <v>180</v>
-      </c>
-      <c r="AP70" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS70" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>233</v>
+      </c>
+      <c r="B71" t="s">
         <v>234</v>
-      </c>
-      <c r="B71" t="s">
-        <v>235</v>
       </c>
       <c r="C71" t="s">
         <v>164</v>
@@ -8085,7 +8086,7 @@
         <v>47</v>
       </c>
       <c r="E71" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H71" t="s">
         <v>49</v>
@@ -8130,19 +8131,19 @@
         <v>173</v>
       </c>
       <c r="AA71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB71" t="s">
         <v>62</v>
       </c>
       <c r="AC71" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD71" t="s">
         <v>64</v>
       </c>
       <c r="AE71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF71" t="s">
         <v>66</v>
@@ -8151,33 +8152,33 @@
         <v>177</v>
       </c>
       <c r="AH71" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI71" t="s">
         <v>178</v>
-      </c>
-      <c r="AI71" t="s">
-        <v>179</v>
       </c>
       <c r="AL71">
         <v>-9999999</v>
       </c>
       <c r="AN71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO71" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP71" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS71" t="s">
         <v>180</v>
-      </c>
-      <c r="AP71" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS71" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>235</v>
+      </c>
+      <c r="B72" t="s">
         <v>236</v>
-      </c>
-      <c r="B72" t="s">
-        <v>237</v>
       </c>
       <c r="C72" t="s">
         <v>164</v>
@@ -8185,6 +8186,9 @@
       <c r="D72" t="s">
         <v>47</v>
       </c>
+      <c r="E72" t="s">
+        <v>165</v>
+      </c>
       <c r="H72" t="s">
         <v>49</v>
       </c>
@@ -8249,33 +8253,33 @@
         <v>177</v>
       </c>
       <c r="AH72" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI72" t="s">
         <v>178</v>
       </c>
-      <c r="AI72" t="s">
-        <v>179</v>
-      </c>
       <c r="AK72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AL72">
         <v>-9999999</v>
       </c>
       <c r="AO72" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP72" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS72" t="s">
         <v>180</v>
-      </c>
-      <c r="AP72" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS72" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>238</v>
+      </c>
+      <c r="B73" t="s">
         <v>239</v>
-      </c>
-      <c r="B73" t="s">
-        <v>240</v>
       </c>
       <c r="C73" t="s">
         <v>164</v>
@@ -8284,7 +8288,7 @@
         <v>47</v>
       </c>
       <c r="E73" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H73" t="s">
         <v>49</v>
@@ -8329,19 +8333,19 @@
         <v>173</v>
       </c>
       <c r="AA73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB73" t="s">
         <v>62</v>
       </c>
       <c r="AC73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD73" t="s">
         <v>64</v>
       </c>
       <c r="AE73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF73" t="s">
         <v>66</v>
@@ -8350,33 +8354,33 @@
         <v>177</v>
       </c>
       <c r="AH73" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI73" t="s">
         <v>178</v>
-      </c>
-      <c r="AI73" t="s">
-        <v>179</v>
       </c>
       <c r="AL73">
         <v>-9999999</v>
       </c>
       <c r="AN73" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO73" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP73" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS73" t="s">
         <v>180</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS73" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>240</v>
+      </c>
+      <c r="B74" t="s">
         <v>241</v>
-      </c>
-      <c r="B74" t="s">
-        <v>242</v>
       </c>
       <c r="C74" t="s">
         <v>164</v>
@@ -8385,7 +8389,7 @@
         <v>47</v>
       </c>
       <c r="E74" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H74" t="s">
         <v>49</v>
@@ -8451,36 +8455,36 @@
         <v>177</v>
       </c>
       <c r="AH74" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI74" t="s">
         <v>178</v>
       </c>
-      <c r="AI74" t="s">
-        <v>179</v>
-      </c>
       <c r="AK74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL74">
         <v>-9999999</v>
       </c>
       <c r="AN74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO74" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP74" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS74" t="s">
         <v>180</v>
-      </c>
-      <c r="AP74" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS74" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>243</v>
+      </c>
+      <c r="B75" t="s">
         <v>244</v>
-      </c>
-      <c r="B75" t="s">
-        <v>245</v>
       </c>
       <c r="C75" t="s">
         <v>164</v>
@@ -8489,7 +8493,7 @@
         <v>47</v>
       </c>
       <c r="E75" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H75" t="s">
         <v>49</v>
@@ -8555,36 +8559,36 @@
         <v>177</v>
       </c>
       <c r="AH75" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI75" t="s">
         <v>178</v>
       </c>
-      <c r="AI75" t="s">
-        <v>179</v>
-      </c>
       <c r="AK75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AL75">
         <v>-9999999</v>
       </c>
       <c r="AN75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO75" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP75" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS75" t="s">
         <v>180</v>
-      </c>
-      <c r="AP75" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS75" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>246</v>
+      </c>
+      <c r="B76" t="s">
         <v>247</v>
-      </c>
-      <c r="B76" t="s">
-        <v>248</v>
       </c>
       <c r="C76" t="s">
         <v>164</v>
@@ -8593,7 +8597,7 @@
         <v>47</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H76" t="s">
         <v>49</v>
@@ -8638,19 +8642,19 @@
         <v>173</v>
       </c>
       <c r="AA76" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB76" t="s">
         <v>62</v>
       </c>
       <c r="AC76" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD76" t="s">
         <v>64</v>
       </c>
       <c r="AE76" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF76" t="s">
         <v>66</v>
@@ -8659,33 +8663,33 @@
         <v>177</v>
       </c>
       <c r="AH76" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI76" t="s">
         <v>178</v>
-      </c>
-      <c r="AI76" t="s">
-        <v>179</v>
       </c>
       <c r="AL76">
         <v>-9999999</v>
       </c>
       <c r="AN76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO76" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP76" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS76" t="s">
         <v>180</v>
-      </c>
-      <c r="AP76" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS76" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>248</v>
+      </c>
+      <c r="B77" t="s">
         <v>249</v>
-      </c>
-      <c r="B77" t="s">
-        <v>250</v>
       </c>
       <c r="C77" t="s">
         <v>164</v>
@@ -8694,7 +8698,7 @@
         <v>47</v>
       </c>
       <c r="E77" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H77" t="s">
         <v>49</v>
@@ -8739,19 +8743,19 @@
         <v>173</v>
       </c>
       <c r="AA77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB77" t="s">
         <v>62</v>
       </c>
       <c r="AC77" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD77" t="s">
         <v>64</v>
       </c>
       <c r="AE77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF77" t="s">
         <v>66</v>
@@ -8760,33 +8764,33 @@
         <v>177</v>
       </c>
       <c r="AH77" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI77" t="s">
         <v>178</v>
-      </c>
-      <c r="AI77" t="s">
-        <v>179</v>
       </c>
       <c r="AL77">
         <v>-9999999</v>
       </c>
       <c r="AN77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO77" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP77" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS77" t="s">
         <v>180</v>
-      </c>
-      <c r="AP77" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS77" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>250</v>
+      </c>
+      <c r="B78" t="s">
         <v>251</v>
-      </c>
-      <c r="B78" t="s">
-        <v>252</v>
       </c>
       <c r="C78" t="s">
         <v>164</v>
@@ -8795,7 +8799,7 @@
         <v>47</v>
       </c>
       <c r="E78" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H78" t="s">
         <v>49</v>
@@ -8840,19 +8844,19 @@
         <v>173</v>
       </c>
       <c r="AA78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB78" t="s">
         <v>62</v>
       </c>
       <c r="AC78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD78" t="s">
         <v>64</v>
       </c>
       <c r="AE78" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF78" t="s">
         <v>66</v>
@@ -8861,33 +8865,33 @@
         <v>177</v>
       </c>
       <c r="AH78" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI78" t="s">
         <v>178</v>
-      </c>
-      <c r="AI78" t="s">
-        <v>179</v>
       </c>
       <c r="AL78">
         <v>-9999999</v>
       </c>
       <c r="AN78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO78" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP78" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS78" t="s">
         <v>180</v>
-      </c>
-      <c r="AP78" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS78" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>252</v>
+      </c>
+      <c r="B79" t="s">
         <v>253</v>
-      </c>
-      <c r="B79" t="s">
-        <v>254</v>
       </c>
       <c r="C79" t="s">
         <v>164</v>
@@ -8896,7 +8900,7 @@
         <v>47</v>
       </c>
       <c r="E79" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H79" t="s">
         <v>49</v>
@@ -8941,19 +8945,19 @@
         <v>173</v>
       </c>
       <c r="AA79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB79" t="s">
         <v>62</v>
       </c>
       <c r="AC79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD79" t="s">
         <v>64</v>
       </c>
       <c r="AE79" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF79" t="s">
         <v>66</v>
@@ -8962,33 +8966,33 @@
         <v>177</v>
       </c>
       <c r="AH79" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI79" t="s">
         <v>178</v>
-      </c>
-      <c r="AI79" t="s">
-        <v>179</v>
       </c>
       <c r="AL79">
         <v>-9999999</v>
       </c>
       <c r="AN79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO79" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP79" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS79" t="s">
         <v>180</v>
-      </c>
-      <c r="AP79" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS79" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>254</v>
+      </c>
+      <c r="B80" t="s">
         <v>255</v>
-      </c>
-      <c r="B80" t="s">
-        <v>256</v>
       </c>
       <c r="C80" t="s">
         <v>164</v>
@@ -8997,7 +9001,7 @@
         <v>47</v>
       </c>
       <c r="E80" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H80" t="s">
         <v>49</v>
@@ -9042,19 +9046,19 @@
         <v>173</v>
       </c>
       <c r="AA80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB80" t="s">
         <v>62</v>
       </c>
       <c r="AC80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD80" t="s">
         <v>64</v>
       </c>
       <c r="AE80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF80" t="s">
         <v>66</v>
@@ -9063,33 +9067,33 @@
         <v>177</v>
       </c>
       <c r="AH80" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI80" t="s">
         <v>178</v>
-      </c>
-      <c r="AI80" t="s">
-        <v>179</v>
       </c>
       <c r="AL80">
         <v>-9999999</v>
       </c>
       <c r="AN80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO80" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP80" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS80" t="s">
         <v>180</v>
-      </c>
-      <c r="AP80" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS80" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" t="s">
         <v>257</v>
-      </c>
-      <c r="B81" t="s">
-        <v>258</v>
       </c>
       <c r="C81" t="s">
         <v>164</v>
@@ -9098,7 +9102,7 @@
         <v>47</v>
       </c>
       <c r="E81" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H81" t="s">
         <v>49</v>
@@ -9143,19 +9147,19 @@
         <v>173</v>
       </c>
       <c r="AA81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB81" t="s">
         <v>62</v>
       </c>
       <c r="AC81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD81" t="s">
         <v>64</v>
       </c>
       <c r="AE81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF81" t="s">
         <v>66</v>
@@ -9164,33 +9168,33 @@
         <v>177</v>
       </c>
       <c r="AH81" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI81" t="s">
         <v>178</v>
-      </c>
-      <c r="AI81" t="s">
-        <v>179</v>
       </c>
       <c r="AL81">
         <v>-9999999</v>
       </c>
       <c r="AN81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO81" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP81" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS81" t="s">
         <v>180</v>
-      </c>
-      <c r="AP81" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS81" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>258</v>
+      </c>
+      <c r="B82" t="s">
         <v>259</v>
-      </c>
-      <c r="B82" t="s">
-        <v>260</v>
       </c>
       <c r="C82" t="s">
         <v>164</v>
@@ -9199,7 +9203,7 @@
         <v>47</v>
       </c>
       <c r="E82" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H82" t="s">
         <v>49</v>
@@ -9244,19 +9248,19 @@
         <v>173</v>
       </c>
       <c r="AA82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB82" t="s">
         <v>62</v>
       </c>
       <c r="AC82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD82" t="s">
         <v>64</v>
       </c>
       <c r="AE82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF82" t="s">
         <v>66</v>
@@ -9265,33 +9269,33 @@
         <v>177</v>
       </c>
       <c r="AH82" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI82" t="s">
         <v>178</v>
-      </c>
-      <c r="AI82" t="s">
-        <v>179</v>
       </c>
       <c r="AL82">
         <v>-9999999</v>
       </c>
       <c r="AN82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO82" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP82" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS82" t="s">
         <v>180</v>
-      </c>
-      <c r="AP82" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS82" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>260</v>
+      </c>
+      <c r="B83" t="s">
         <v>261</v>
-      </c>
-      <c r="B83" t="s">
-        <v>262</v>
       </c>
       <c r="C83" t="s">
         <v>164</v>
@@ -9300,7 +9304,7 @@
         <v>47</v>
       </c>
       <c r="E83" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="H83" t="s">
         <v>49</v>
@@ -9345,19 +9349,19 @@
         <v>173</v>
       </c>
       <c r="AA83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB83" t="s">
         <v>62</v>
       </c>
       <c r="AC83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AD83" t="s">
         <v>64</v>
       </c>
       <c r="AE83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AF83" t="s">
         <v>66</v>
@@ -9366,25 +9370,25 @@
         <v>177</v>
       </c>
       <c r="AH83" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI83" t="s">
         <v>178</v>
-      </c>
-      <c r="AI83" t="s">
-        <v>179</v>
       </c>
       <c r="AL83">
         <v>-9999999</v>
       </c>
       <c r="AN83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AO83" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP83" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS83" t="s">
         <v>180</v>
-      </c>
-      <c r="AP83" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS83" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -9402,13 +9406,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -9416,10 +9420,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" t="s">
         <v>266</v>
-      </c>
-      <c r="C2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -9427,10 +9431,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -9438,10 +9442,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -9449,10 +9453,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -9460,10 +9464,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -9471,10 +9475,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -9482,10 +9486,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -9493,10 +9497,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -9504,10 +9508,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -9515,10 +9519,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -9526,10 +9530,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -9537,10 +9541,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -9548,10 +9552,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -9559,10 +9563,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -9570,10 +9574,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -9581,10 +9585,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -9592,10 +9596,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -9603,10 +9607,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -9614,10 +9618,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -9625,10 +9629,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -9636,10 +9640,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -9647,10 +9651,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -9658,10 +9662,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -9669,10 +9673,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -9680,10 +9684,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -9691,10 +9695,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -9702,10 +9706,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -9713,10 +9717,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -9724,10 +9728,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -9735,10 +9739,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -9746,10 +9750,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -9757,10 +9761,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -9768,10 +9772,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -9779,10 +9783,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -9790,10 +9794,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -9801,10 +9805,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -9812,10 +9816,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -9823,10 +9827,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -9834,10 +9838,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -9845,10 +9849,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -9856,10 +9860,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -9867,10 +9871,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C43" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -9878,10 +9882,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -9889,10 +9893,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C45" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -9900,10 +9904,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardization of new scanner projects ok
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -14705,20 +14705,20 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Variables</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Variable_types</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Description</t>
         </is>

</xml_diff>

<commit_message>
Running standardization and QC on newest projects
</commit_message>
<xml_diff>
--- a/raw/project_IFCB_standardizer.xlsx
+++ b/raw/project_IFCB_standardizer.xlsx
@@ -11252,7 +11252,11 @@
         </is>
       </c>
       <c r="AL60" t="inlineStr"/>
-      <c r="AM60" t="inlineStr"/>
+      <c r="AM60" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/IFCB_dashboard_downloads/project_harpswell_flags.csv</t>
+        </is>
+      </c>
       <c r="AN60" t="n">
         <v>-9999999</v>
       </c>

</xml_diff>